<commit_message>
Added two new rules. See #402
</commit_message>
<xml_diff>
--- a/Deliverables/RULES/USDM_CORE_Rules.xlsx
+++ b/Deliverables/RULES/USDM_CORE_Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stack\CL027\Publish\CORE\3.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2428D27-85DE-4AA8-87C4-0E079CBABDD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378E6348-74D3-4D1C-9DAB-DFB8F678266F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10215" yWindow="-17385" windowWidth="26820" windowHeight="15330" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
+    <workbookView xWindow="-8310" yWindow="-18930" windowWidth="23010" windowHeight="18330" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
   </bookViews>
   <sheets>
     <sheet name="Release 3.3 CORE rules" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="460">
   <si>
     <t>Textual statement of rule</t>
   </si>
@@ -1407,6 +1407,18 @@
   </si>
   <si>
     <t>DDF00003</t>
+  </si>
+  <si>
+    <t>An activity with children must not refer to a timeline, procedure, biomedical concept, biomedical concept category or biomedical concept surrogate.</t>
+  </si>
+  <si>
+    <t>CHK0178</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The ordering of activities (using the previous and next attributes) must include the parents (e.g. activities refering to children) preceding their children. </t>
+  </si>
+  <si>
+    <t>CHK0179</t>
   </si>
 </sst>
 </file>
@@ -1820,10 +1832,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FACE88-1C57-4099-A43D-8DA482706A91}">
-  <dimension ref="A1:H142"/>
+  <dimension ref="A1:H144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="A142" sqref="A142"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2105,33 +2117,33 @@
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>147</v>
+        <v>456</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>141</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>14</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="7" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>295</v>
+        <v>147</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>115</v>
@@ -2140,31 +2152,31 @@
         <v>141</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>296</v>
+        <v>148</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="7" t="s">
-        <v>294</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>153</v>
+        <v>295</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>115</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>155</v>
+        <v>296</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>7</v>
@@ -2174,47 +2186,45 @@
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="7" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>105</v>
+        <v>458</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>107</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="G15" s="6"/>
       <c r="H15" s="7" t="s">
-        <v>104</v>
+        <v>459</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>421</v>
+        <v>153</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>106</v>
+        <v>154</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>107</v>
+        <v>155</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>7</v>
@@ -2224,21 +2234,21 @@
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>160</v>
+        <v>105</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>161</v>
+        <v>106</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>5</v>
+        <v>107</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>7</v>
@@ -2246,99 +2256,99 @@
       <c r="F17" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G17" s="6"/>
+      <c r="G17" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="H17" s="7" t="s">
-        <v>159</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="6"/>
+      <c r="H18" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="6"/>
+      <c r="H19" s="7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="5" t="s">
+      <c r="B20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D20" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18" s="6" t="s">
+      <c r="E20" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="H18" s="7" t="s">
+      <c r="H20" s="7" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="5" t="s">
-        <v>342</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>343</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>455</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" s="6"/>
-      <c r="H20" s="7" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>235</v>
+        <v>41</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>7</v>
@@ -2346,23 +2356,25 @@
       <c r="F21" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="6"/>
+      <c r="G21" s="6" t="s">
+        <v>455</v>
+      </c>
       <c r="H21" s="7" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>163</v>
+        <v>234</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>164</v>
+        <v>235</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>165</v>
+        <v>236</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>7</v>
@@ -2372,21 +2384,21 @@
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="7" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>444</v>
+        <v>350</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>164</v>
+        <v>235</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>165</v>
+        <v>351</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>7</v>
@@ -2396,21 +2408,21 @@
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="7" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>325</v>
+        <v>163</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>297</v>
+        <v>164</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>326</v>
+        <v>165</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>7</v>
@@ -2420,173 +2432,173 @@
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="7" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>136</v>
+        <v>444</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>115</v>
       </c>
       <c r="C25" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" s="6"/>
+      <c r="H25" s="7" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="6"/>
+      <c r="H26" s="7" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D27" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G25" s="6" t="s">
+      <c r="E27" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="6" t="s">
         <v>453</v>
       </c>
-      <c r="H25" s="7" t="s">
+      <c r="H27" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="5" t="s">
+    <row r="28" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="5" t="s">
+      <c r="B28" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>450</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D28" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="E26" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G26" s="6" t="s">
+      <c r="E28" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" s="6" t="s">
         <v>451</v>
       </c>
-      <c r="H26" s="7" t="s">
+      <c r="H28" s="7" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="5" t="s">
+    <row r="29" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="5" t="s">
+      <c r="B29" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D29" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G27" s="6" t="s">
+      <c r="E29" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="H27" s="7" t="s">
+      <c r="H29" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="5" t="s">
+    <row r="30" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" s="5" t="s">
         <v>427</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B30" s="6" t="s">
         <v>115</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A29" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G29" s="6"/>
-      <c r="H29" s="7" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="5" t="s">
-        <v>445</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>6</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>290</v>
       </c>
       <c r="D30" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>291</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G30" s="6"/>
-      <c r="H30" s="7" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>7</v>
@@ -2596,21 +2608,21 @@
       </c>
       <c r="G31" s="6"/>
       <c r="H31" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
-        <v>167</v>
+        <v>445</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>67</v>
+        <v>290</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>68</v>
+        <v>291</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>7</v>
@@ -2620,12 +2632,12 @@
       </c>
       <c r="G32" s="6"/>
       <c r="H32" s="7" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
-        <v>238</v>
+        <v>66</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>6</v>
@@ -2634,7 +2646,7 @@
         <v>67</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>186</v>
+        <v>68</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>7</v>
@@ -2644,21 +2656,21 @@
       </c>
       <c r="G33" s="6"/>
       <c r="H33" s="7" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
-        <v>315</v>
+        <v>167</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>316</v>
+        <v>67</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>317</v>
+        <v>68</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>7</v>
@@ -2668,21 +2680,21 @@
       </c>
       <c r="G34" s="6"/>
       <c r="H34" s="7" t="s">
-        <v>314</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>185</v>
+        <v>67</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>227</v>
+        <v>186</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>7</v>
@@ -2692,21 +2704,21 @@
       </c>
       <c r="G35" s="6"/>
       <c r="H35" s="7" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
-        <v>120</v>
+        <v>315</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>121</v>
+        <v>316</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>122</v>
+        <v>317</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>7</v>
@@ -2714,25 +2726,23 @@
       <c r="F36" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G36" s="6" t="s">
-        <v>123</v>
-      </c>
+      <c r="G36" s="6"/>
       <c r="H36" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
-        <v>125</v>
+        <v>226</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>121</v>
+        <v>185</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>122</v>
+        <v>227</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>7</v>
@@ -2742,21 +2752,21 @@
       </c>
       <c r="G37" s="6"/>
       <c r="H37" s="7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
-        <v>356</v>
+        <v>120</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>357</v>
+        <v>122</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>7</v>
@@ -2764,23 +2774,25 @@
       <c r="F38" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G38" s="6"/>
+      <c r="G38" s="6" t="s">
+        <v>123</v>
+      </c>
       <c r="H38" s="7" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
-        <v>384</v>
+        <v>125</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>357</v>
+        <v>122</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>7</v>
@@ -2790,12 +2802,12 @@
       </c>
       <c r="G39" s="6"/>
       <c r="H39" s="7" t="s">
-        <v>383</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
-        <v>221</v>
+        <v>356</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>6</v>
@@ -2804,22 +2816,22 @@
         <v>114</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>222</v>
+        <v>357</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G40" s="6"/>
       <c r="H40" s="7" t="s">
-        <v>220</v>
+        <v>355</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>6</v>
@@ -2828,22 +2840,22 @@
         <v>114</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>222</v>
+        <v>357</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G41" s="6"/>
       <c r="H41" s="7" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
-        <v>393</v>
+        <v>221</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>6</v>
@@ -2852,22 +2864,22 @@
         <v>114</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>394</v>
+        <v>222</v>
       </c>
       <c r="E42" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>7</v>
       </c>
       <c r="G42" s="6"/>
       <c r="H42" s="7" t="s">
-        <v>392</v>
+        <v>220</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>6</v>
@@ -2876,46 +2888,46 @@
         <v>114</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>394</v>
+        <v>222</v>
       </c>
       <c r="E43" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>7</v>
       </c>
       <c r="G43" s="6"/>
       <c r="H43" s="7" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
-        <v>113</v>
+        <v>393</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>114</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>107</v>
+        <v>394</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G44" s="6"/>
       <c r="H44" s="7" t="s">
-        <v>112</v>
+        <v>392</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
-        <v>441</v>
+        <v>396</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>6</v>
@@ -2924,31 +2936,31 @@
         <v>114</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>340</v>
+        <v>394</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G45" s="6"/>
       <c r="H45" s="7" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>7</v>
@@ -2956,25 +2968,23 @@
       <c r="F46" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G46" s="6" t="s">
-        <v>99</v>
-      </c>
+      <c r="G46" s="6"/>
       <c r="H46" s="7" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
-        <v>423</v>
+        <v>441</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>95</v>
+        <v>340</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>7</v>
@@ -2984,21 +2994,21 @@
       </c>
       <c r="G47" s="6"/>
       <c r="H47" s="7" t="s">
-        <v>178</v>
+        <v>339</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
-        <v>304</v>
+        <v>97</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>305</v>
+        <v>98</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>306</v>
+        <v>95</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>7</v>
@@ -3006,23 +3016,25 @@
       <c r="F48" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G48" s="6"/>
+      <c r="G48" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="H48" s="7" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
-        <v>169</v>
+        <v>423</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>170</v>
+        <v>98</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>171</v>
+        <v>95</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>7</v>
@@ -3032,21 +3044,21 @@
       </c>
       <c r="G49" s="6"/>
       <c r="H49" s="7" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
-        <v>173</v>
+        <v>304</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>170</v>
+        <v>305</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>171</v>
+        <v>306</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>7</v>
@@ -3056,12 +3068,12 @@
       </c>
       <c r="G50" s="6"/>
       <c r="H50" s="7" t="s">
-        <v>172</v>
+        <v>303</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>6</v>
@@ -3080,12 +3092,12 @@
       </c>
       <c r="G51" s="6"/>
       <c r="H51" s="7" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>6</v>
@@ -3104,21 +3116,21 @@
       </c>
       <c r="G52" s="6"/>
       <c r="H52" s="7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
-        <v>376</v>
+        <v>175</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>377</v>
+        <v>170</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>378</v>
+        <v>171</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>7</v>
@@ -3128,21 +3140,21 @@
       </c>
       <c r="G53" s="6"/>
       <c r="H53" s="7" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
-        <v>266</v>
+        <v>177</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>267</v>
+        <v>170</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>232</v>
+        <v>171</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>7</v>
@@ -3152,21 +3164,21 @@
       </c>
       <c r="G54" s="6"/>
       <c r="H54" s="7" t="s">
-        <v>265</v>
+        <v>176</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
-        <v>200</v>
+        <v>376</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>128</v>
+        <v>377</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>201</v>
+        <v>378</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>7</v>
@@ -3176,21 +3188,21 @@
       </c>
       <c r="G55" s="6"/>
       <c r="H55" s="7" t="s">
-        <v>199</v>
+        <v>375</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
-        <v>311</v>
+        <v>266</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>128</v>
+        <v>267</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>201</v>
+        <v>232</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>7</v>
@@ -3200,15 +3212,15 @@
       </c>
       <c r="G56" s="6"/>
       <c r="H56" s="7" t="s">
-        <v>310</v>
+        <v>265</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
-        <v>313</v>
+        <v>200</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>128</v>
@@ -3224,12 +3236,12 @@
       </c>
       <c r="G57" s="6"/>
       <c r="H57" s="7" t="s">
-        <v>312</v>
+        <v>199</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
-        <v>328</v>
+        <v>311</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>115</v>
@@ -3238,7 +3250,7 @@
         <v>128</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>329</v>
+        <v>201</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>7</v>
@@ -3248,21 +3260,21 @@
       </c>
       <c r="G58" s="6"/>
       <c r="H58" s="7" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
-        <v>127</v>
+        <v>313</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>128</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>122</v>
+        <v>201</v>
       </c>
       <c r="E59" s="6" t="s">
         <v>7</v>
@@ -3272,21 +3284,21 @@
       </c>
       <c r="G59" s="6"/>
       <c r="H59" s="7" t="s">
-        <v>126</v>
+        <v>312</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
-        <v>353</v>
+        <v>328</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>128</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>122</v>
+        <v>329</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>7</v>
@@ -3296,21 +3308,21 @@
       </c>
       <c r="G60" s="6"/>
       <c r="H60" s="7" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>7</v>
@@ -3320,21 +3332,21 @@
       </c>
       <c r="G61" s="6"/>
       <c r="H61" s="7" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
-        <v>244</v>
+        <v>353</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
       <c r="E62" s="6" t="s">
         <v>7</v>
@@ -3344,21 +3356,21 @@
       </c>
       <c r="G62" s="6"/>
       <c r="H62" s="7" t="s">
-        <v>243</v>
+        <v>352</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
-        <v>269</v>
+        <v>93</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>270</v>
+        <v>94</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>271</v>
+        <v>95</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>7</v>
@@ -3368,21 +3380,21 @@
       </c>
       <c r="G63" s="6"/>
       <c r="H63" s="7" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="116" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
-        <v>405</v>
+        <v>244</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>270</v>
+        <v>94</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>271</v>
+        <v>95</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>7</v>
@@ -3392,21 +3404,21 @@
       </c>
       <c r="G64" s="6"/>
       <c r="H64" s="7" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
-        <v>422</v>
+        <v>269</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>157</v>
+        <v>270</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>158</v>
+        <v>271</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>7</v>
@@ -3416,21 +3428,21 @@
       </c>
       <c r="G65" s="6"/>
       <c r="H65" s="7" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="116" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
-        <v>426</v>
+        <v>405</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>157</v>
+        <v>270</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>158</v>
+        <v>271</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>7</v>
@@ -3440,21 +3452,21 @@
       </c>
       <c r="G66" s="6"/>
       <c r="H66" s="7" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
-        <v>48</v>
+        <v>422</v>
       </c>
       <c r="B67" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>49</v>
+        <v>157</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>50</v>
+        <v>158</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>7</v>
@@ -3462,25 +3474,23 @@
       <c r="F67" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G67" s="6" t="s">
-        <v>452</v>
-      </c>
+      <c r="G67" s="6"/>
       <c r="H67" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
-        <v>437</v>
+        <v>426</v>
       </c>
       <c r="B68" s="6" t="s">
         <v>115</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>224</v>
+        <v>157</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>299</v>
+        <v>158</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>7</v>
@@ -3490,45 +3500,47 @@
       </c>
       <c r="G68" s="6"/>
       <c r="H68" s="7" t="s">
-        <v>298</v>
+        <v>192</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
-        <v>322</v>
+        <v>48</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>224</v>
+        <v>49</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>323</v>
+        <v>50</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G69" s="6"/>
+        <v>7</v>
+      </c>
+      <c r="G69" s="6" t="s">
+        <v>452</v>
+      </c>
       <c r="H69" s="7" t="s">
-        <v>321</v>
+        <v>47</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
-        <v>432</v>
+        <v>437</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>224</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>50</v>
+        <v>299</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>7</v>
@@ -3538,45 +3550,45 @@
       </c>
       <c r="G70" s="6"/>
       <c r="H70" s="7" t="s">
-        <v>223</v>
+        <v>298</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
-        <v>433</v>
+        <v>322</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>224</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>50</v>
+        <v>323</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="G71" s="6"/>
       <c r="H71" s="7" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="B72" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>53</v>
+        <v>224</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>212</v>
+        <v>50</v>
       </c>
       <c r="E72" s="6" t="s">
         <v>7</v>
@@ -3586,21 +3598,21 @@
       </c>
       <c r="G72" s="6"/>
       <c r="H72" s="7" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
-        <v>188</v>
+        <v>433</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>53</v>
+        <v>224</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>189</v>
+        <v>50</v>
       </c>
       <c r="E73" s="6" t="s">
         <v>7</v>
@@ -3610,12 +3622,12 @@
       </c>
       <c r="G73" s="6"/>
       <c r="H73" s="7" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A74" s="5" t="s">
-        <v>194</v>
+        <v>429</v>
       </c>
       <c r="B74" s="6" t="s">
         <v>6</v>
@@ -3624,7 +3636,7 @@
         <v>53</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>195</v>
+        <v>212</v>
       </c>
       <c r="E74" s="6" t="s">
         <v>7</v>
@@ -3632,25 +3644,23 @@
       <c r="F74" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G74" s="6" t="s">
-        <v>454</v>
-      </c>
+      <c r="G74" s="6"/>
       <c r="H74" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
-        <v>430</v>
+        <v>188</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>53</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E75" s="6" t="s">
         <v>7</v>
@@ -3660,12 +3670,12 @@
       </c>
       <c r="G75" s="6"/>
       <c r="H75" s="7" t="s">
-        <v>213</v>
+        <v>187</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
-        <v>89</v>
+        <v>194</v>
       </c>
       <c r="B76" s="6" t="s">
         <v>6</v>
@@ -3674,7 +3684,7 @@
         <v>53</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>90</v>
+        <v>195</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>7</v>
@@ -3683,15 +3693,15 @@
         <v>7</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>91</v>
+        <v>454</v>
       </c>
       <c r="H76" s="7" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A77" s="5" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="B77" s="6" t="s">
         <v>6</v>
@@ -3700,7 +3710,7 @@
         <v>53</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>90</v>
+        <v>195</v>
       </c>
       <c r="E77" s="6" t="s">
         <v>7</v>
@@ -3710,12 +3720,12 @@
       </c>
       <c r="G77" s="6"/>
       <c r="H77" s="7" t="s">
-        <v>332</v>
+        <v>213</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
-        <v>52</v>
+        <v>89</v>
       </c>
       <c r="B78" s="6" t="s">
         <v>6</v>
@@ -3724,170 +3734,172 @@
         <v>53</v>
       </c>
       <c r="D78" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G78" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="H78" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A79" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G79" s="6"/>
+      <c r="H79" s="7" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A80" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D80" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E78" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F78" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G78" s="6" t="s">
+      <c r="E80" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G80" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H78" s="7" t="s">
+      <c r="H80" s="7" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A79" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="B79" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F79" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G79" s="6" t="s">
-        <v>449</v>
-      </c>
-      <c r="H79" s="7" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A80" s="5" t="s">
-        <v>428</v>
-      </c>
-      <c r="B80" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="D80" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="E80" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F80" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G80" s="6"/>
-      <c r="H80" s="7" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
-        <v>331</v>
+        <v>278</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C81" s="5" t="s">
         <v>210</v>
       </c>
       <c r="D81" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F81" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G81" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="H81" s="7" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A82" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D82" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="E81" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F81" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G81" s="6"/>
-      <c r="H81" s="7" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A82" s="5" t="s">
-        <v>389</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>387</v>
-      </c>
-      <c r="D82" s="5" t="s">
-        <v>279</v>
-      </c>
       <c r="E82" s="6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F82" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G82" s="6"/>
       <c r="H82" s="7" t="s">
-        <v>388</v>
+        <v>209</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
-        <v>398</v>
+        <v>331</v>
       </c>
       <c r="B83" s="6" t="s">
         <v>115</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>387</v>
+        <v>210</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>279</v>
+        <v>189</v>
       </c>
       <c r="E83" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F83" s="6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G83" s="6"/>
       <c r="H83" s="7" t="s">
-        <v>397</v>
+        <v>330</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C84" s="5" t="s">
         <v>387</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>195</v>
+        <v>279</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F84" s="6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G84" s="6"/>
       <c r="H84" s="7" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
-        <v>386</v>
+        <v>398</v>
       </c>
       <c r="B85" s="6" t="s">
         <v>115</v>
@@ -3896,7 +3908,7 @@
         <v>387</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>90</v>
+        <v>279</v>
       </c>
       <c r="E85" s="6" t="s">
         <v>7</v>
@@ -3906,62 +3918,60 @@
       </c>
       <c r="G85" s="6"/>
       <c r="H85" s="7" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
-        <v>215</v>
+        <v>391</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>75</v>
+        <v>387</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
       <c r="E86" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F86" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="G86" s="6"/>
       <c r="H86" s="7" t="s">
-        <v>214</v>
+        <v>390</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
-        <v>74</v>
+        <v>386</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>75</v>
+        <v>387</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="E87" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F87" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G87" s="6" t="s">
-        <v>77</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="G87" s="6"/>
       <c r="H87" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
-        <v>180</v>
+        <v>215</v>
       </c>
       <c r="B88" s="6" t="s">
         <v>6</v>
@@ -3970,7 +3980,7 @@
         <v>75</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>76</v>
+        <v>216</v>
       </c>
       <c r="E88" s="6" t="s">
         <v>7</v>
@@ -3978,51 +3988,49 @@
       <c r="F88" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G88" s="6" t="s">
-        <v>181</v>
-      </c>
+      <c r="G88" s="6"/>
       <c r="H88" s="7" t="s">
-        <v>179</v>
+        <v>214</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
-        <v>417</v>
+        <v>74</v>
       </c>
       <c r="B89" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>418</v>
+        <v>75</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>419</v>
+        <v>76</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F89" s="6" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>420</v>
+        <v>77</v>
       </c>
       <c r="H89" s="7" t="s">
-        <v>416</v>
+        <v>73</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
-        <v>424</v>
+        <v>180</v>
       </c>
       <c r="B90" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>183</v>
+        <v>75</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>184</v>
+        <v>76</v>
       </c>
       <c r="E90" s="6" t="s">
         <v>7</v>
@@ -4030,47 +4038,51 @@
       <c r="F90" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G90" s="6"/>
+      <c r="G90" s="6" t="s">
+        <v>181</v>
+      </c>
       <c r="H90" s="7" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A91" s="5" t="s">
-        <v>334</v>
+        <v>417</v>
       </c>
       <c r="B91" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>101</v>
+        <v>418</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>335</v>
+        <v>419</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F91" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G91" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="G91" s="6" t="s">
+        <v>420</v>
+      </c>
       <c r="H91" s="7" t="s">
-        <v>333</v>
+        <v>416</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
-        <v>440</v>
+        <v>424</v>
       </c>
       <c r="B92" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>101</v>
+        <v>183</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>335</v>
+        <v>184</v>
       </c>
       <c r="E92" s="6" t="s">
         <v>7</v>
@@ -4080,12 +4092,12 @@
       </c>
       <c r="G92" s="6"/>
       <c r="H92" s="7" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" s="5" t="s">
-        <v>446</v>
+        <v>334</v>
       </c>
       <c r="B93" s="6" t="s">
         <v>6</v>
@@ -4094,7 +4106,7 @@
         <v>101</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>102</v>
+        <v>335</v>
       </c>
       <c r="E93" s="6" t="s">
         <v>7</v>
@@ -4102,16 +4114,14 @@
       <c r="F93" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G93" s="6" t="s">
-        <v>103</v>
-      </c>
+      <c r="G93" s="6"/>
       <c r="H93" s="7" t="s">
-        <v>100</v>
+        <v>333</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A94" s="5" t="s">
-        <v>337</v>
+        <v>440</v>
       </c>
       <c r="B94" s="6" t="s">
         <v>6</v>
@@ -4120,7 +4130,7 @@
         <v>101</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>102</v>
+        <v>335</v>
       </c>
       <c r="E94" s="6" t="s">
         <v>7</v>
@@ -4130,21 +4140,21 @@
       </c>
       <c r="G94" s="6"/>
       <c r="H94" s="7" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A95" s="5" t="s">
-        <v>260</v>
+        <v>446</v>
       </c>
       <c r="B95" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>251</v>
+        <v>101</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>261</v>
+        <v>102</v>
       </c>
       <c r="E95" s="6" t="s">
         <v>7</v>
@@ -4152,23 +4162,25 @@
       <c r="F95" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G95" s="6"/>
+      <c r="G95" s="6" t="s">
+        <v>103</v>
+      </c>
       <c r="H95" s="7" t="s">
-        <v>259</v>
+        <v>100</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A96" s="5" t="s">
-        <v>263</v>
+        <v>337</v>
       </c>
       <c r="B96" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>251</v>
+        <v>101</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>264</v>
+        <v>102</v>
       </c>
       <c r="E96" s="6" t="s">
         <v>7</v>
@@ -4178,12 +4190,12 @@
       </c>
       <c r="G96" s="6"/>
       <c r="H96" s="7" t="s">
-        <v>262</v>
+        <v>336</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A97" s="5" t="s">
-        <v>367</v>
+        <v>260</v>
       </c>
       <c r="B97" s="6" t="s">
         <v>6</v>
@@ -4192,7 +4204,7 @@
         <v>251</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="E97" s="6" t="s">
         <v>7</v>
@@ -4202,12 +4214,12 @@
       </c>
       <c r="G97" s="6"/>
       <c r="H97" s="7" t="s">
-        <v>366</v>
+        <v>259</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A98" s="5" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="B98" s="6" t="s">
         <v>6</v>
@@ -4216,7 +4228,7 @@
         <v>251</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="E98" s="6" t="s">
         <v>7</v>
@@ -4226,21 +4238,21 @@
       </c>
       <c r="G98" s="6"/>
       <c r="H98" s="7" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A99" s="5" t="s">
-        <v>293</v>
+        <v>367</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C99" s="5" t="s">
         <v>251</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>219</v>
+        <v>264</v>
       </c>
       <c r="E99" s="6" t="s">
         <v>7</v>
@@ -4250,12 +4262,12 @@
       </c>
       <c r="G99" s="6"/>
       <c r="H99" s="7" t="s">
-        <v>292</v>
+        <v>366</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A100" s="5" t="s">
-        <v>371</v>
+        <v>257</v>
       </c>
       <c r="B100" s="6" t="s">
         <v>6</v>
@@ -4264,7 +4276,7 @@
         <v>251</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>372</v>
+        <v>258</v>
       </c>
       <c r="E100" s="6" t="s">
         <v>7</v>
@@ -4274,21 +4286,21 @@
       </c>
       <c r="G100" s="6"/>
       <c r="H100" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A101" s="5" t="s">
-        <v>250</v>
+        <v>293</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C101" s="5" t="s">
         <v>251</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>252</v>
+        <v>219</v>
       </c>
       <c r="E101" s="6" t="s">
         <v>7</v>
@@ -4298,12 +4310,12 @@
       </c>
       <c r="G101" s="6"/>
       <c r="H101" s="7" t="s">
-        <v>249</v>
+        <v>292</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B102" s="6" t="s">
         <v>6</v>
@@ -4312,7 +4324,7 @@
         <v>251</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>252</v>
+        <v>372</v>
       </c>
       <c r="E102" s="6" t="s">
         <v>7</v>
@@ -4322,12 +4334,12 @@
       </c>
       <c r="G102" s="6"/>
       <c r="H102" s="7" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A103" s="5" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B103" s="6" t="s">
         <v>6</v>
@@ -4336,7 +4348,7 @@
         <v>251</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E103" s="6" t="s">
         <v>7</v>
@@ -4346,12 +4358,12 @@
       </c>
       <c r="G103" s="6"/>
       <c r="H103" s="7" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A104" s="5" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
       <c r="B104" s="6" t="s">
         <v>6</v>
@@ -4360,7 +4372,7 @@
         <v>251</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E104" s="6" t="s">
         <v>7</v>
@@ -4370,45 +4382,45 @@
       </c>
       <c r="G104" s="6"/>
       <c r="H104" s="7" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A105" s="5" t="s">
-        <v>414</v>
+        <v>254</v>
       </c>
       <c r="B105" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>12</v>
+        <v>251</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>13</v>
+        <v>255</v>
       </c>
       <c r="E105" s="6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F105" s="6" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G105" s="6"/>
       <c r="H105" s="7" t="s">
-        <v>413</v>
+        <v>253</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A106" s="5" t="s">
-        <v>45</v>
+        <v>369</v>
       </c>
       <c r="B106" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>12</v>
+        <v>251</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>46</v>
+        <v>255</v>
       </c>
       <c r="E106" s="6" t="s">
         <v>7</v>
@@ -4418,12 +4430,12 @@
       </c>
       <c r="G106" s="6"/>
       <c r="H106" s="7" t="s">
-        <v>44</v>
+        <v>368</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A107" s="5" t="s">
-        <v>361</v>
+        <v>414</v>
       </c>
       <c r="B107" s="6" t="s">
         <v>6</v>
@@ -4432,22 +4444,22 @@
         <v>12</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>362</v>
+        <v>13</v>
       </c>
       <c r="E107" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F107" s="6" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="G107" s="6"/>
       <c r="H107" s="7" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A108" s="5" t="s">
-        <v>301</v>
+        <v>45</v>
       </c>
       <c r="B108" s="6" t="s">
         <v>6</v>
@@ -4456,7 +4468,7 @@
         <v>12</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>302</v>
+        <v>46</v>
       </c>
       <c r="E108" s="6" t="s">
         <v>7</v>
@@ -4466,12 +4478,12 @@
       </c>
       <c r="G108" s="6"/>
       <c r="H108" s="7" t="s">
-        <v>300</v>
+        <v>44</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A109" s="5" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B109" s="6" t="s">
         <v>6</v>
@@ -4480,7 +4492,7 @@
         <v>12</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="E109" s="6" t="s">
         <v>7</v>
@@ -4490,12 +4502,12 @@
       </c>
       <c r="G109" s="6"/>
       <c r="H109" s="7" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A110" s="5" t="s">
-        <v>109</v>
+        <v>301</v>
       </c>
       <c r="B110" s="6" t="s">
         <v>6</v>
@@ -4504,7 +4516,7 @@
         <v>12</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>110</v>
+        <v>302</v>
       </c>
       <c r="E110" s="6" t="s">
         <v>7</v>
@@ -4514,21 +4526,21 @@
       </c>
       <c r="G110" s="6"/>
       <c r="H110" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A111" s="5" t="s">
-        <v>431</v>
+        <v>364</v>
       </c>
       <c r="B111" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>218</v>
+        <v>12</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>219</v>
+        <v>365</v>
       </c>
       <c r="E111" s="6" t="s">
         <v>7</v>
@@ -4538,21 +4550,21 @@
       </c>
       <c r="G111" s="6"/>
       <c r="H111" s="7" t="s">
-        <v>217</v>
+        <v>363</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A112" s="5" t="s">
-        <v>438</v>
+        <v>109</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>319</v>
+        <v>12</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>320</v>
+        <v>110</v>
       </c>
       <c r="E112" s="6" t="s">
         <v>7</v>
@@ -4562,190 +4574,190 @@
       </c>
       <c r="G112" s="6"/>
       <c r="H112" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A113" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C113" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="D113" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="E113" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F113" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G113" s="6"/>
+      <c r="H113" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A114" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="B114" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="E114" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F114" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G114" s="6"/>
+      <c r="H114" s="7" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A113" s="5" t="s">
+    <row r="115" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A115" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B113" s="6" t="s">
+      <c r="B115" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C113" s="5" t="s">
+      <c r="C115" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="D113" s="5" t="s">
+      <c r="D115" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="E113" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F113" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G113" s="6" t="s">
+      <c r="E115" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F115" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G115" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H113" s="7" t="s">
+      <c r="H115" s="7" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A114" s="5" t="s">
-        <v>447</v>
-      </c>
-      <c r="B114" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C114" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="D114" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="E114" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F114" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G114" s="6" t="s">
-        <v>448</v>
-      </c>
-      <c r="H114" s="7" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A115" s="5" t="s">
-        <v>442</v>
-      </c>
-      <c r="B115" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C115" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D115" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="E115" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F115" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G115" s="6" t="s">
-        <v>443</v>
-      </c>
-      <c r="H115" s="7" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="116" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A116" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="B116" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C116" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="D116" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="E116" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F116" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G116" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="H116" s="7" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A117" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="B117" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C117" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D117" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="E117" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F117" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G117" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="H117" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A118" s="5" t="s">
         <v>415</v>
       </c>
-      <c r="B116" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C116" s="5" t="s">
+      <c r="B118" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C118" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D116" s="5" t="s">
+      <c r="D118" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E116" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F116" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G116" s="6" t="s">
+      <c r="E118" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F118" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G118" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H116" s="7" t="s">
+      <c r="H118" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A117" s="5" t="s">
+    <row r="119" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A119" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="B117" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C117" s="5" t="s">
+      <c r="B119" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C119" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D117" s="5" t="s">
+      <c r="D119" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E117" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F117" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G117" s="6" t="s">
+      <c r="E119" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F119" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G119" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="H117" s="7" t="s">
+      <c r="H119" s="7" t="s">
         <v>196</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A118" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="B118" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C118" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="D118" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="E118" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F118" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G118" s="6"/>
-      <c r="H118" s="7" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A119" s="5" t="s">
-        <v>347</v>
-      </c>
-      <c r="B119" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C119" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="D119" s="5" t="s">
-        <v>348</v>
-      </c>
-      <c r="E119" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F119" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G119" s="6"/>
-      <c r="H119" s="7" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="120" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A120" s="5" t="s">
-        <v>230</v>
+        <v>380</v>
       </c>
       <c r="B120" s="6" t="s">
         <v>6</v>
@@ -4754,7 +4766,7 @@
         <v>231</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>232</v>
+        <v>378</v>
       </c>
       <c r="E120" s="6" t="s">
         <v>7</v>
@@ -4764,12 +4776,12 @@
       </c>
       <c r="G120" s="6"/>
       <c r="H120" s="7" t="s">
-        <v>229</v>
+        <v>379</v>
       </c>
     </row>
     <row r="121" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A121" s="5" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B121" s="6" t="s">
         <v>6</v>
@@ -4778,7 +4790,7 @@
         <v>231</v>
       </c>
       <c r="D121" s="5" t="s">
-        <v>80</v>
+        <v>348</v>
       </c>
       <c r="E121" s="6" t="s">
         <v>7</v>
@@ -4788,21 +4800,21 @@
       </c>
       <c r="G121" s="6"/>
       <c r="H121" s="7" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A122" s="5" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="B122" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="D122" s="5" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="E122" s="6" t="s">
         <v>7</v>
@@ -4812,18 +4824,18 @@
       </c>
       <c r="G122" s="6"/>
       <c r="H122" s="7" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
     </row>
     <row r="123" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A123" s="5" t="s">
-        <v>425</v>
+        <v>345</v>
       </c>
       <c r="B123" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>191</v>
+        <v>231</v>
       </c>
       <c r="D123" s="5" t="s">
         <v>80</v>
@@ -4836,21 +4848,21 @@
       </c>
       <c r="G123" s="6"/>
       <c r="H123" s="7" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A124" s="5" t="s">
-        <v>434</v>
+        <v>246</v>
       </c>
       <c r="B124" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>191</v>
+        <v>247</v>
       </c>
       <c r="D124" s="5" t="s">
-        <v>80</v>
+        <v>248</v>
       </c>
       <c r="E124" s="6" t="s">
         <v>7</v>
@@ -4860,21 +4872,21 @@
       </c>
       <c r="G124" s="6"/>
       <c r="H124" s="7" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A125" s="5" t="s">
-        <v>28</v>
+        <v>425</v>
       </c>
       <c r="B125" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C125" s="5" t="s">
-        <v>29</v>
+        <v>191</v>
       </c>
       <c r="D125" s="5" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="E125" s="6" t="s">
         <v>7</v>
@@ -4882,40 +4894,38 @@
       <c r="F125" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G125" s="6" t="s">
-        <v>31</v>
-      </c>
+      <c r="G125" s="6"/>
       <c r="H125" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" s="5" t="s">
-        <v>400</v>
+        <v>434</v>
       </c>
       <c r="B126" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>29</v>
+        <v>191</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="E126" s="6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F126" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G126" s="6"/>
       <c r="H126" s="7" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A127" s="5" t="s">
-        <v>402</v>
+        <v>28</v>
       </c>
       <c r="B127" s="6" t="s">
         <v>6</v>
@@ -4924,22 +4934,24 @@
         <v>29</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="E127" s="6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F127" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G127" s="6"/>
+      <c r="G127" s="6" t="s">
+        <v>31</v>
+      </c>
       <c r="H127" s="7" t="s">
-        <v>401</v>
+        <v>27</v>
       </c>
     </row>
     <row r="128" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A128" s="5" t="s">
-        <v>62</v>
+        <v>400</v>
       </c>
       <c r="B128" s="6" t="s">
         <v>6</v>
@@ -4948,24 +4960,22 @@
         <v>29</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="E128" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F128" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G128" s="6" t="s">
-        <v>64</v>
-      </c>
+      <c r="G128" s="6"/>
       <c r="H128" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A129" s="5" t="s">
-        <v>241</v>
+        <v>402</v>
       </c>
       <c r="B129" s="6" t="s">
         <v>6</v>
@@ -4974,31 +4984,31 @@
         <v>29</v>
       </c>
       <c r="D129" s="5" t="s">
-        <v>242</v>
+        <v>13</v>
       </c>
       <c r="E129" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F129" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G129" s="6"/>
       <c r="H129" s="7" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A130" s="5" t="s">
-        <v>412</v>
+        <v>62</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="E130" s="6" t="s">
         <v>7</v>
@@ -5006,23 +5016,25 @@
       <c r="F130" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G130" s="6"/>
+      <c r="G130" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="H130" s="7" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
     </row>
     <row r="131" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A131" s="5" t="s">
-        <v>70</v>
+        <v>241</v>
       </c>
       <c r="B131" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D131" s="5" t="s">
-        <v>71</v>
+        <v>242</v>
       </c>
       <c r="E131" s="6" t="s">
         <v>7</v>
@@ -5030,16 +5042,14 @@
       <c r="F131" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G131" s="6" t="s">
-        <v>72</v>
-      </c>
+      <c r="G131" s="6"/>
       <c r="H131" s="7" t="s">
-        <v>69</v>
+        <v>240</v>
       </c>
     </row>
     <row r="132" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A132" s="5" t="s">
-        <v>208</v>
+        <v>412</v>
       </c>
       <c r="B132" s="6" t="s">
         <v>6</v>
@@ -5048,7 +5058,7 @@
         <v>10</v>
       </c>
       <c r="D132" s="5" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E132" s="6" t="s">
         <v>7</v>
@@ -5058,12 +5068,12 @@
       </c>
       <c r="G132" s="6"/>
       <c r="H132" s="7" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A133" s="5" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B133" s="6" t="s">
         <v>6</v>
@@ -5072,7 +5082,7 @@
         <v>10</v>
       </c>
       <c r="D133" s="5" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="E133" s="6" t="s">
         <v>7</v>
@@ -5081,15 +5091,15 @@
         <v>7</v>
       </c>
       <c r="G133" s="6" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="H133" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A134" s="5" t="s">
-        <v>86</v>
+        <v>208</v>
       </c>
       <c r="B134" s="6" t="s">
         <v>6</v>
@@ -5098,7 +5108,7 @@
         <v>10</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="E134" s="6" t="s">
         <v>7</v>
@@ -5106,16 +5116,14 @@
       <c r="F134" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G134" s="6" t="s">
-        <v>87</v>
-      </c>
+      <c r="G134" s="6"/>
       <c r="H134" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A135" s="5" t="s">
-        <v>359</v>
+        <v>82</v>
       </c>
       <c r="B135" s="6" t="s">
         <v>6</v>
@@ -5132,14 +5140,16 @@
       <c r="F135" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G135" s="6"/>
+      <c r="G135" s="6" t="s">
+        <v>84</v>
+      </c>
       <c r="H135" s="7" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A136" s="5" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="B136" s="6" t="s">
         <v>6</v>
@@ -5148,7 +5158,7 @@
         <v>10</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E136" s="6" t="s">
         <v>7</v>
@@ -5156,14 +5166,16 @@
       <c r="F136" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G136" s="6"/>
+      <c r="G136" s="6" t="s">
+        <v>87</v>
+      </c>
       <c r="H136" s="7" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="137" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A137" s="5" t="s">
-        <v>206</v>
+        <v>359</v>
       </c>
       <c r="B137" s="6" t="s">
         <v>6</v>
@@ -5172,7 +5184,7 @@
         <v>10</v>
       </c>
       <c r="D137" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E137" s="6" t="s">
         <v>7</v>
@@ -5182,12 +5194,12 @@
       </c>
       <c r="G137" s="6"/>
       <c r="H137" s="7" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A138" s="5" t="s">
-        <v>203</v>
+        <v>79</v>
       </c>
       <c r="B138" s="6" t="s">
         <v>6</v>
@@ -5196,7 +5208,7 @@
         <v>10</v>
       </c>
       <c r="D138" s="5" t="s">
-        <v>204</v>
+        <v>80</v>
       </c>
       <c r="E138" s="6" t="s">
         <v>7</v>
@@ -5206,12 +5218,12 @@
       </c>
       <c r="G138" s="6"/>
       <c r="H138" s="7" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A139" s="5" t="s">
-        <v>33</v>
+        <v>206</v>
       </c>
       <c r="B139" s="6" t="s">
         <v>6</v>
@@ -5220,7 +5232,7 @@
         <v>10</v>
       </c>
       <c r="D139" s="5" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="E139" s="6" t="s">
         <v>7</v>
@@ -5228,16 +5240,14 @@
       <c r="F139" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G139" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="G139" s="6"/>
       <c r="H139" s="7" t="s">
-        <v>32</v>
+        <v>205</v>
       </c>
     </row>
     <row r="140" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A140" s="5" t="s">
-        <v>37</v>
+        <v>203</v>
       </c>
       <c r="B140" s="6" t="s">
         <v>6</v>
@@ -5246,7 +5256,7 @@
         <v>10</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>34</v>
+        <v>204</v>
       </c>
       <c r="E140" s="6" t="s">
         <v>7</v>
@@ -5254,16 +5264,14 @@
       <c r="F140" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G140" s="6" t="s">
-        <v>38</v>
-      </c>
+      <c r="G140" s="6"/>
       <c r="H140" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A141" s="5" t="s">
-        <v>281</v>
+        <v>33</v>
       </c>
       <c r="B141" s="6" t="s">
         <v>6</v>
@@ -5272,7 +5280,7 @@
         <v>10</v>
       </c>
       <c r="D141" s="5" t="s">
-        <v>282</v>
+        <v>34</v>
       </c>
       <c r="E141" s="6" t="s">
         <v>7</v>
@@ -5280,14 +5288,16 @@
       <c r="F141" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G141" s="6"/>
+      <c r="G141" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="H141" s="7" t="s">
-        <v>280</v>
+        <v>32</v>
       </c>
     </row>
     <row r="142" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A142" s="5" t="s">
-        <v>284</v>
+        <v>37</v>
       </c>
       <c r="B142" s="6" t="s">
         <v>6</v>
@@ -5296,25 +5306,75 @@
         <v>10</v>
       </c>
       <c r="D142" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E142" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F142" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G142" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H142" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A143" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="B143" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C143" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D143" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="E143" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F143" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G143" s="6"/>
+      <c r="H143" s="7" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A144" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B144" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C144" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D144" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="E142" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F142" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G142" s="6"/>
-      <c r="H142" s="7" t="s">
+      <c r="E144" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F144" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G144" s="6"/>
+      <c r="H144" s="7" t="s">
         <v>283</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:Q10" xr:uid="{B9FACE88-1C57-4099-A43D-8DA482706A91}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H142">
-    <sortCondition ref="C8:C142"/>
-    <sortCondition ref="D8:D142"/>
-    <sortCondition ref="H8:H142"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H144">
+    <sortCondition ref="C8:C144"/>
+    <sortCondition ref="D8:D144"/>
+    <sortCondition ref="H8:H144"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added and changed rules according to #408
</commit_message>
<xml_diff>
--- a/Deliverables/RULES/USDM_CORE_Rules.xlsx
+++ b/Deliverables/RULES/USDM_CORE_Rules.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stack\CL027\Publish\CORE\3.3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stack\CL027\Publish\CORE\3.4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378E6348-74D3-4D1C-9DAB-DFB8F678266F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F7EA55-2090-4D48-9295-436772E66DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8310" yWindow="-18930" windowWidth="23010" windowHeight="18330" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
+    <workbookView xWindow="7215" yWindow="-17760" windowWidth="24555" windowHeight="15225" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
   </bookViews>
   <sheets>
-    <sheet name="Release 3.3 CORE rules" sheetId="1" r:id="rId1"/>
+    <sheet name="Release 3.0 and 3.4 CORE rules" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Release 3.3 CORE rules'!$A$1:$Q$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Release 3.0 and 3.4 CORE rules'!$A$1:$Q$165</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="493">
   <si>
     <t>Textual statement of rule</t>
   </si>
@@ -641,9 +641,6 @@
     <t>CHK0105</t>
   </si>
   <si>
-    <t>Within a study protocol document version, the section numbers for narrative content specified must be unique.</t>
-  </si>
-  <si>
     <t>sectionNumber</t>
   </si>
   <si>
@@ -1007,9 +1004,6 @@
     <t>CHK0120</t>
   </si>
   <si>
-    <t>For  a specified range at least a minimum or maximum value is expected.</t>
-  </si>
-  <si>
     <t>minValue, maxValue</t>
   </si>
   <si>
@@ -1052,9 +1046,6 @@
     <t>CHK0056</t>
   </si>
   <si>
-    <t>A study cell must at least refer one element defined wihtin the same study design.</t>
-  </si>
-  <si>
     <t>CHK0091</t>
   </si>
   <si>
@@ -1391,9 +1382,6 @@
     <t>DDF00019</t>
   </si>
   <si>
-    <t>BiomedicalConceptCategory, StudyProtocolDocumentVersion, NarrativeContent, Activity</t>
-  </si>
-  <si>
     <t>DDF00018</t>
   </si>
   <si>
@@ -1419,6 +1407,117 @@
   </si>
   <si>
     <t>CHK0179</t>
+  </si>
+  <si>
+    <t>DDF00042</t>
+  </si>
+  <si>
+    <t>BiomedicalConceptCategory, StudyProtocolDocumentVersion, StudyDefinitionDocumentVersion, NarrativeContent, Activity</t>
+  </si>
+  <si>
+    <t>A study cell must only reference elements that are defined within the same study design as the study cell.</t>
+  </si>
+  <si>
+    <t>DDF00045</t>
+  </si>
+  <si>
+    <t>Within a document version, the specified section numbers for narrative content must be unique.</t>
+  </si>
+  <si>
+    <t>DDF00044</t>
+  </si>
+  <si>
+    <t>For a specified range at least a minimum or maximum value is expected.</t>
+  </si>
+  <si>
+    <t>DDF00043</t>
+  </si>
+  <si>
+    <t>A study cell must refer to at least one element.</t>
+  </si>
+  <si>
+    <t>CHK0180</t>
+  </si>
+  <si>
+    <t>NarrativeContentItem</t>
+  </si>
+  <si>
+    <t>CHK0181</t>
+  </si>
+  <si>
+    <t>Narrative content is expected to point to a child and/or to a content item text.</t>
+  </si>
+  <si>
+    <t>children, contentItem</t>
+  </si>
+  <si>
+    <t>CHK0182</t>
+  </si>
+  <si>
+    <t>If a section number is to be displayed then a number must be specified and vice versa.</t>
+  </si>
+  <si>
+    <t>sectionNumber, displaySectionNumber</t>
+  </si>
+  <si>
+    <t>CHK0183</t>
+  </si>
+  <si>
+    <t>If a section title is to be displayed then a title must be specified and vice versa.</t>
+  </si>
+  <si>
+    <t>sectionTitle, displaySectionTitle</t>
+  </si>
+  <si>
+    <t>CHK0184</t>
+  </si>
+  <si>
+    <t>A study definition document type must be specifed using the XXX (Cnnn) DDF codelist.</t>
+  </si>
+  <si>
+    <t>StudyDefinitionDocument</t>
+  </si>
+  <si>
+    <t>CHK0185</t>
+  </si>
+  <si>
+    <t>A study definition document language must be specifed using the XXX (Cnnn) codelist.</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>CHK0186</t>
+  </si>
+  <si>
+    <t>A study definition document version must not be referenced more than once by the same study version.</t>
+  </si>
+  <si>
+    <t>documentVersions</t>
+  </si>
+  <si>
+    <t>CHK0187</t>
+  </si>
+  <si>
+    <t>A piece of narrative content must only reference narrative content items that have been defined within the study version as the narrative content.</t>
+  </si>
+  <si>
+    <t>contentItem</t>
+  </si>
+  <si>
+    <t>CHK0188</t>
+  </si>
+  <si>
+    <t>A study definition document version's status must be specifed using the status Value Set Terminology (XXX) DDF codelist.</t>
+  </si>
+  <si>
+    <t>StudyDefinitionDocumentVersion</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>CHK0189</t>
   </si>
 </sst>
 </file>
@@ -1483,7 +1582,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1498,6 +1597,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1832,10 +1936,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FACE88-1C57-4099-A43D-8DA482706A91}">
-  <dimension ref="A1:H144"/>
+  <dimension ref="A1:H163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1854,10 +1958,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>406</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>409</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>1</v>
@@ -1869,15 +1973,15 @@
         <v>3</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
@@ -1901,7 +2005,7 @@
     </row>
     <row r="3" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>6</v>
@@ -1925,7 +2029,7 @@
     </row>
     <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>6</v>
@@ -1944,12 +2048,12 @@
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>6</v>
@@ -1968,7 +2072,7 @@
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -2023,7 +2127,7 @@
     </row>
     <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>6</v>
@@ -2042,7 +2146,7 @@
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -2119,7 +2223,7 @@
     </row>
     <row r="12" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>6</v>
@@ -2138,7 +2242,7 @@
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="7" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -2167,7 +2271,7 @@
     </row>
     <row r="14" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>115</v>
@@ -2176,7 +2280,7 @@
         <v>141</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>7</v>
@@ -2186,12 +2290,12 @@
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>6</v>
@@ -2210,7 +2314,7 @@
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="7" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -2265,7 +2369,7 @@
     </row>
     <row r="18" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>6</v>
@@ -2306,7 +2410,9 @@
       <c r="F19" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="6"/>
+      <c r="G19" s="6" t="s">
+        <v>459</v>
+      </c>
       <c r="H19" s="7" t="s">
         <v>159</v>
       </c>
@@ -2339,7 +2445,7 @@
     </row>
     <row r="21" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>6</v>
@@ -2348,7 +2454,7 @@
         <v>41</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>7</v>
@@ -2357,24 +2463,24 @@
         <v>7</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="5" t="s">
+      <c r="D22" s="5" t="s">
         <v>235</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>236</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>7</v>
@@ -2384,21 +2490,21 @@
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>7</v>
@@ -2408,7 +2514,7 @@
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="7" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -2437,7 +2543,7 @@
     </row>
     <row r="25" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>115</v>
@@ -2456,21 +2562,21 @@
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="7" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>115</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>7</v>
@@ -2480,7 +2586,7 @@
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -2503,13 +2609,13 @@
         <v>7</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="H27" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>133</v>
       </c>
@@ -2517,7 +2623,7 @@
         <v>6</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>450</v>
+        <v>457</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>134</v>
@@ -2529,7 +2635,7 @@
         <v>7</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="H28" s="7" t="s">
         <v>132</v>
@@ -2563,42 +2669,42 @@
     </row>
     <row r="30" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>115</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D30" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>309</v>
-      </c>
       <c r="H30" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>115</v>
       </c>
       <c r="C31" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>290</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>291</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>7</v>
@@ -2608,21 +2714,21 @@
       </c>
       <c r="G31" s="6"/>
       <c r="H31" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C32" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>290</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>291</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>7</v>
@@ -2632,7 +2738,7 @@
       </c>
       <c r="G32" s="6"/>
       <c r="H32" s="7" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -2685,7 +2791,7 @@
     </row>
     <row r="35" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>6</v>
@@ -2704,36 +2810,38 @@
       </c>
       <c r="G35" s="6"/>
       <c r="H35" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="B36" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" s="5" t="s">
+      <c r="D36" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>317</v>
-      </c>
       <c r="E36" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G36" s="6"/>
+      <c r="G36" s="6" t="s">
+        <v>461</v>
+      </c>
       <c r="H36" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>6</v>
@@ -2742,7 +2850,7 @@
         <v>185</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>7</v>
@@ -2752,7 +2860,7 @@
       </c>
       <c r="G37" s="6"/>
       <c r="H37" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
@@ -2807,7 +2915,7 @@
     </row>
     <row r="40" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>6</v>
@@ -2816,7 +2924,7 @@
         <v>114</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>7</v>
@@ -2826,12 +2934,12 @@
       </c>
       <c r="G40" s="6"/>
       <c r="H40" s="7" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>6</v>
@@ -2840,7 +2948,7 @@
         <v>114</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>7</v>
@@ -2850,12 +2958,12 @@
       </c>
       <c r="G41" s="6"/>
       <c r="H41" s="7" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>6</v>
@@ -2864,7 +2972,7 @@
         <v>114</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>7</v>
@@ -2874,12 +2982,12 @@
       </c>
       <c r="G42" s="6"/>
       <c r="H42" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>6</v>
@@ -2888,7 +2996,7 @@
         <v>114</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>7</v>
@@ -2898,12 +3006,12 @@
       </c>
       <c r="G43" s="6"/>
       <c r="H43" s="7" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>6</v>
@@ -2912,7 +3020,7 @@
         <v>114</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>14</v>
@@ -2922,12 +3030,12 @@
       </c>
       <c r="G44" s="6"/>
       <c r="H44" s="7" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>6</v>
@@ -2936,7 +3044,7 @@
         <v>114</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>14</v>
@@ -2946,7 +3054,7 @@
       </c>
       <c r="G45" s="6"/>
       <c r="H45" s="7" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="58" x14ac:dyDescent="0.35">
@@ -2975,7 +3083,7 @@
     </row>
     <row r="47" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>6</v>
@@ -2984,7 +3092,7 @@
         <v>114</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>7</v>
@@ -2994,7 +3102,7 @@
       </c>
       <c r="G47" s="6"/>
       <c r="H47" s="7" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -3025,7 +3133,7 @@
     </row>
     <row r="49" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>6</v>
@@ -3049,16 +3157,16 @@
     </row>
     <row r="50" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>115</v>
       </c>
       <c r="C50" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="D50" s="5" t="s">
         <v>305</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>306</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>7</v>
@@ -3068,7 +3176,7 @@
       </c>
       <c r="G50" s="6"/>
       <c r="H50" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -3169,16 +3277,16 @@
     </row>
     <row r="55" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>7</v>
@@ -3188,21 +3296,21 @@
       </c>
       <c r="G55" s="6"/>
       <c r="H55" s="7" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="B56" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>267</v>
-      </c>
       <c r="D56" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>7</v>
@@ -3212,69 +3320,69 @@
       </c>
       <c r="G56" s="6"/>
       <c r="H56" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
-        <v>200</v>
+        <v>468</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>128</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>201</v>
+        <v>469</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G57" s="6"/>
       <c r="H57" s="7" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
-        <v>311</v>
+        <v>486</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>128</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>201</v>
+        <v>487</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F58" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G58" s="6"/>
       <c r="H58" s="7" t="s">
-        <v>310</v>
+        <v>488</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
-        <v>313</v>
+        <v>460</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>128</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E59" s="6" t="s">
         <v>7</v>
@@ -3284,12 +3392,12 @@
       </c>
       <c r="G59" s="6"/>
       <c r="H59" s="7" t="s">
-        <v>312</v>
+        <v>199</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
-        <v>328</v>
+        <v>310</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>115</v>
@@ -3298,7 +3406,7 @@
         <v>128</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>329</v>
+        <v>200</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>7</v>
@@ -3308,21 +3416,21 @@
       </c>
       <c r="G60" s="6"/>
       <c r="H60" s="7" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
-        <v>127</v>
+        <v>312</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>128</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>122</v>
+        <v>200</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>7</v>
@@ -3332,12 +3440,12 @@
       </c>
       <c r="G61" s="6"/>
       <c r="H61" s="7" t="s">
-        <v>126</v>
+        <v>311</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
-        <v>353</v>
+        <v>471</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>6</v>
@@ -3346,31 +3454,31 @@
         <v>128</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>122</v>
+        <v>472</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F62" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G62" s="6"/>
       <c r="H62" s="7" t="s">
-        <v>352</v>
+        <v>473</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
-        <v>93</v>
+        <v>326</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>95</v>
+        <v>327</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>7</v>
@@ -3380,69 +3488,69 @@
       </c>
       <c r="G63" s="6"/>
       <c r="H63" s="7" t="s">
-        <v>92</v>
+        <v>325</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
-        <v>244</v>
+        <v>474</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>95</v>
+        <v>475</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F64" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G64" s="6"/>
       <c r="H64" s="7" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
-        <v>269</v>
+        <v>127</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>270</v>
+        <v>128</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>271</v>
+        <v>122</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="G65" s="6"/>
       <c r="H65" s="7" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="116" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
-        <v>405</v>
+        <v>350</v>
       </c>
       <c r="B66" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>270</v>
+        <v>128</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>271</v>
+        <v>122</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>7</v>
@@ -3452,45 +3560,45 @@
       </c>
       <c r="G66" s="6"/>
       <c r="H66" s="7" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
-        <v>422</v>
+        <v>127</v>
       </c>
       <c r="B67" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>157</v>
+        <v>466</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>158</v>
+        <v>122</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F67" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G67" s="6"/>
       <c r="H67" s="7" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
-        <v>426</v>
+        <v>93</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>157</v>
+        <v>94</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>158</v>
+        <v>95</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>7</v>
@@ -3500,21 +3608,21 @@
       </c>
       <c r="G68" s="6"/>
       <c r="H68" s="7" t="s">
-        <v>192</v>
+        <v>92</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
-        <v>48</v>
+        <v>243</v>
       </c>
       <c r="B69" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="E69" s="6" t="s">
         <v>7</v>
@@ -3522,25 +3630,23 @@
       <c r="F69" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G69" s="6" t="s">
-        <v>452</v>
-      </c>
+      <c r="G69" s="6"/>
       <c r="H69" s="7" t="s">
-        <v>47</v>
+        <v>242</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
-        <v>437</v>
+        <v>268</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>224</v>
+        <v>269</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>299</v>
+        <v>270</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>7</v>
@@ -3550,45 +3656,45 @@
       </c>
       <c r="G70" s="6"/>
       <c r="H70" s="7" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="116" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
-        <v>322</v>
+        <v>402</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>224</v>
+        <v>269</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>323</v>
+        <v>270</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G71" s="6"/>
       <c r="H71" s="7" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
-        <v>432</v>
+        <v>419</v>
       </c>
       <c r="B72" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>224</v>
+        <v>157</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>50</v>
+        <v>158</v>
       </c>
       <c r="E72" s="6" t="s">
         <v>7</v>
@@ -3598,21 +3704,21 @@
       </c>
       <c r="G72" s="6"/>
       <c r="H72" s="7" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
-        <v>433</v>
+        <v>423</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>224</v>
+        <v>157</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>50</v>
+        <v>158</v>
       </c>
       <c r="E73" s="6" t="s">
         <v>7</v>
@@ -3622,21 +3728,21 @@
       </c>
       <c r="G73" s="6"/>
       <c r="H73" s="7" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A74" s="5" t="s">
-        <v>429</v>
+        <v>48</v>
       </c>
       <c r="B74" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>212</v>
+        <v>50</v>
       </c>
       <c r="E74" s="6" t="s">
         <v>7</v>
@@ -3644,23 +3750,25 @@
       <c r="F74" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G74" s="6"/>
+      <c r="G74" s="6" t="s">
+        <v>448</v>
+      </c>
       <c r="H74" s="7" t="s">
-        <v>211</v>
+        <v>47</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
-        <v>188</v>
+        <v>434</v>
       </c>
       <c r="B75" s="6" t="s">
         <v>115</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>53</v>
+        <v>223</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>189</v>
+        <v>298</v>
       </c>
       <c r="E75" s="6" t="s">
         <v>7</v>
@@ -3668,49 +3776,49 @@
       <c r="F75" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G75" s="6"/>
+      <c r="G75" s="6" t="s">
+        <v>456</v>
+      </c>
       <c r="H75" s="7" t="s">
-        <v>187</v>
+        <v>297</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
-        <v>194</v>
+        <v>462</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>53</v>
+        <v>223</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>195</v>
+        <v>321</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G76" s="6" t="s">
-        <v>454</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="G76" s="6"/>
       <c r="H76" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A77" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B77" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>53</v>
+        <v>223</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>195</v>
+        <v>50</v>
       </c>
       <c r="E77" s="6" t="s">
         <v>7</v>
@@ -3718,23 +3826,25 @@
       <c r="F77" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G77" s="6"/>
+      <c r="G77" s="6" t="s">
+        <v>463</v>
+      </c>
       <c r="H77" s="7" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
-        <v>89</v>
+        <v>430</v>
       </c>
       <c r="B78" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>53</v>
+        <v>223</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="E78" s="6" t="s">
         <v>7</v>
@@ -3742,16 +3852,14 @@
       <c r="F78" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G78" s="6" t="s">
-        <v>91</v>
-      </c>
+      <c r="G78" s="6"/>
       <c r="H78" s="7" t="s">
-        <v>88</v>
+        <v>227</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
-        <v>439</v>
+        <v>426</v>
       </c>
       <c r="B79" s="6" t="s">
         <v>6</v>
@@ -3760,7 +3868,7 @@
         <v>53</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>90</v>
+        <v>211</v>
       </c>
       <c r="E79" s="6" t="s">
         <v>7</v>
@@ -3770,21 +3878,21 @@
       </c>
       <c r="G79" s="6"/>
       <c r="H79" s="7" t="s">
-        <v>332</v>
+        <v>210</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
-        <v>52</v>
+        <v>188</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>53</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>54</v>
+        <v>189</v>
       </c>
       <c r="E80" s="6" t="s">
         <v>7</v>
@@ -3792,25 +3900,23 @@
       <c r="F80" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G80" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="G80" s="6"/>
       <c r="H80" s="7" t="s">
-        <v>51</v>
+        <v>187</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
-        <v>278</v>
+        <v>194</v>
       </c>
       <c r="B81" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>210</v>
+        <v>53</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>279</v>
+        <v>195</v>
       </c>
       <c r="E81" s="6" t="s">
         <v>7</v>
@@ -3819,24 +3925,24 @@
         <v>7</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="H81" s="7" t="s">
-        <v>277</v>
+        <v>193</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B82" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>210</v>
+        <v>53</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="E82" s="6" t="s">
         <v>7</v>
@@ -3846,21 +3952,21 @@
       </c>
       <c r="G82" s="6"/>
       <c r="H82" s="7" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
-        <v>331</v>
+        <v>89</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>210</v>
+        <v>53</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>189</v>
+        <v>90</v>
       </c>
       <c r="E83" s="6" t="s">
         <v>7</v>
@@ -3868,119 +3974,125 @@
       <c r="F83" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G83" s="6"/>
+      <c r="G83" s="6" t="s">
+        <v>91</v>
+      </c>
       <c r="H83" s="7" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
-        <v>389</v>
+        <v>436</v>
       </c>
       <c r="B84" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>387</v>
+        <v>53</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>279</v>
+        <v>90</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F84" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G84" s="6"/>
       <c r="H84" s="7" t="s">
-        <v>388</v>
+        <v>330</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
-        <v>398</v>
+        <v>52</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>387</v>
+        <v>53</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>279</v>
+        <v>54</v>
       </c>
       <c r="E85" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F85" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G85" s="6"/>
+        <v>7</v>
+      </c>
+      <c r="G85" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="H85" s="7" t="s">
-        <v>397</v>
+        <v>51</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
-        <v>391</v>
+        <v>277</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>387</v>
+        <v>209</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>195</v>
+        <v>278</v>
       </c>
       <c r="E86" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F86" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G86" s="6"/>
+        <v>7</v>
+      </c>
+      <c r="G86" s="6" t="s">
+        <v>446</v>
+      </c>
       <c r="H86" s="7" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
-        <v>386</v>
+        <v>425</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>387</v>
+        <v>209</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>90</v>
+        <v>189</v>
       </c>
       <c r="E87" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F87" s="6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G87" s="6"/>
       <c r="H87" s="7" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
-        <v>215</v>
+        <v>329</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>75</v>
+        <v>209</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>216</v>
+        <v>189</v>
       </c>
       <c r="E88" s="6" t="s">
         <v>7</v>
@@ -3990,123 +4102,117 @@
       </c>
       <c r="G88" s="6"/>
       <c r="H88" s="7" t="s">
-        <v>214</v>
+        <v>328</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
-        <v>74</v>
+        <v>386</v>
       </c>
       <c r="B89" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>75</v>
+        <v>384</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>76</v>
+        <v>278</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F89" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G89" s="6" t="s">
-        <v>77</v>
-      </c>
+      <c r="G89" s="6"/>
       <c r="H89" s="7" t="s">
-        <v>73</v>
+        <v>385</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
-        <v>180</v>
+        <v>395</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>75</v>
+        <v>384</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>76</v>
+        <v>278</v>
       </c>
       <c r="E90" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F90" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G90" s="6" t="s">
-        <v>181</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="G90" s="6"/>
       <c r="H90" s="7" t="s">
-        <v>179</v>
+        <v>394</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A91" s="5" t="s">
-        <v>417</v>
+        <v>388</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>418</v>
+        <v>384</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>419</v>
+        <v>195</v>
       </c>
       <c r="E91" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F91" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F91" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G91" s="6" t="s">
-        <v>420</v>
-      </c>
+      <c r="G91" s="6"/>
       <c r="H91" s="7" t="s">
-        <v>416</v>
+        <v>387</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
-        <v>424</v>
+        <v>383</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>183</v>
+        <v>384</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>184</v>
+        <v>90</v>
       </c>
       <c r="E92" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F92" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="G92" s="6"/>
       <c r="H92" s="7" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A93" s="5" t="s">
-        <v>334</v>
+        <v>214</v>
       </c>
       <c r="B93" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>335</v>
+        <v>215</v>
       </c>
       <c r="E93" s="6" t="s">
         <v>7</v>
@@ -4116,21 +4222,21 @@
       </c>
       <c r="G93" s="6"/>
       <c r="H93" s="7" t="s">
-        <v>333</v>
+        <v>213</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A94" s="5" t="s">
-        <v>440</v>
+        <v>74</v>
       </c>
       <c r="B94" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>335</v>
+        <v>76</v>
       </c>
       <c r="E94" s="6" t="s">
         <v>7</v>
@@ -4138,23 +4244,25 @@
       <c r="F94" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G94" s="6"/>
+      <c r="G94" s="6" t="s">
+        <v>77</v>
+      </c>
       <c r="H94" s="7" t="s">
-        <v>338</v>
+        <v>73</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A95" s="5" t="s">
-        <v>446</v>
+        <v>180</v>
       </c>
       <c r="B95" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="E95" s="6" t="s">
         <v>7</v>
@@ -4163,48 +4271,50 @@
         <v>7</v>
       </c>
       <c r="G95" s="6" t="s">
-        <v>103</v>
+        <v>181</v>
       </c>
       <c r="H95" s="7" t="s">
-        <v>100</v>
+        <v>179</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A96" s="5" t="s">
-        <v>337</v>
+        <v>414</v>
       </c>
       <c r="B96" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>101</v>
+        <v>415</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>102</v>
+        <v>416</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F96" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G96" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="G96" s="6" t="s">
+        <v>417</v>
+      </c>
       <c r="H96" s="7" t="s">
-        <v>336</v>
+        <v>413</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A97" s="5" t="s">
-        <v>260</v>
+        <v>421</v>
       </c>
       <c r="B97" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>251</v>
+        <v>183</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>261</v>
+        <v>184</v>
       </c>
       <c r="E97" s="6" t="s">
         <v>7</v>
@@ -4214,21 +4324,21 @@
       </c>
       <c r="G97" s="6"/>
       <c r="H97" s="7" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" s="5" t="s">
-        <v>263</v>
+        <v>332</v>
       </c>
       <c r="B98" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>251</v>
+        <v>101</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>264</v>
+        <v>333</v>
       </c>
       <c r="E98" s="6" t="s">
         <v>7</v>
@@ -4238,21 +4348,21 @@
       </c>
       <c r="G98" s="6"/>
       <c r="H98" s="7" t="s">
-        <v>262</v>
+        <v>331</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A99" s="5" t="s">
-        <v>367</v>
+        <v>437</v>
       </c>
       <c r="B99" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>251</v>
+        <v>101</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>264</v>
+        <v>333</v>
       </c>
       <c r="E99" s="6" t="s">
         <v>7</v>
@@ -4262,21 +4372,21 @@
       </c>
       <c r="G99" s="6"/>
       <c r="H99" s="7" t="s">
-        <v>366</v>
+        <v>335</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A100" s="5" t="s">
-        <v>257</v>
+        <v>443</v>
       </c>
       <c r="B100" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>251</v>
+        <v>101</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>258</v>
+        <v>102</v>
       </c>
       <c r="E100" s="6" t="s">
         <v>7</v>
@@ -4284,23 +4394,25 @@
       <c r="F100" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G100" s="6"/>
+      <c r="G100" s="6" t="s">
+        <v>103</v>
+      </c>
       <c r="H100" s="7" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A101" s="5" t="s">
-        <v>293</v>
+        <v>458</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>251</v>
+        <v>101</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>219</v>
+        <v>102</v>
       </c>
       <c r="E101" s="6" t="s">
         <v>7</v>
@@ -4310,117 +4422,117 @@
       </c>
       <c r="G101" s="6"/>
       <c r="H101" s="7" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
-        <v>371</v>
+        <v>464</v>
       </c>
       <c r="B102" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>251</v>
+        <v>101</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>372</v>
+        <v>102</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F102" s="6" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="G102" s="6"/>
       <c r="H102" s="7" t="s">
-        <v>370</v>
+        <v>465</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A103" s="5" t="s">
-        <v>250</v>
+        <v>480</v>
       </c>
       <c r="B103" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>251</v>
+        <v>478</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>252</v>
+        <v>481</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F103" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G103" s="6"/>
       <c r="H103" s="7" t="s">
-        <v>249</v>
+        <v>482</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A104" s="5" t="s">
-        <v>374</v>
+        <v>477</v>
       </c>
       <c r="B104" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>251</v>
+        <v>478</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>252</v>
+        <v>80</v>
       </c>
       <c r="E104" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F104" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G104" s="6"/>
       <c r="H104" s="7" t="s">
-        <v>373</v>
+        <v>479</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A105" s="5" t="s">
-        <v>254</v>
+        <v>489</v>
       </c>
       <c r="B105" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>251</v>
+        <v>490</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>255</v>
+        <v>491</v>
       </c>
       <c r="E105" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F105" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G105" s="6"/>
       <c r="H105" s="7" t="s">
-        <v>253</v>
+        <v>492</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A106" s="5" t="s">
-        <v>369</v>
+        <v>259</v>
       </c>
       <c r="B106" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="E106" s="6" t="s">
         <v>7</v>
@@ -4430,45 +4542,45 @@
       </c>
       <c r="G106" s="6"/>
       <c r="H106" s="7" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A107" s="5" t="s">
-        <v>414</v>
+        <v>262</v>
       </c>
       <c r="B107" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>12</v>
+        <v>250</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>13</v>
+        <v>263</v>
       </c>
       <c r="E107" s="6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F107" s="6" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G107" s="6"/>
       <c r="H107" s="7" t="s">
-        <v>413</v>
+        <v>261</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A108" s="5" t="s">
-        <v>45</v>
+        <v>364</v>
       </c>
       <c r="B108" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>12</v>
+        <v>250</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>46</v>
+        <v>263</v>
       </c>
       <c r="E108" s="6" t="s">
         <v>7</v>
@@ -4478,21 +4590,21 @@
       </c>
       <c r="G108" s="6"/>
       <c r="H108" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A109" s="5" t="s">
-        <v>361</v>
+        <v>256</v>
       </c>
       <c r="B109" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>12</v>
+        <v>250</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>362</v>
+        <v>257</v>
       </c>
       <c r="E109" s="6" t="s">
         <v>7</v>
@@ -4502,21 +4614,21 @@
       </c>
       <c r="G109" s="6"/>
       <c r="H109" s="7" t="s">
-        <v>360</v>
+        <v>255</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A110" s="5" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>12</v>
+        <v>250</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>302</v>
+        <v>218</v>
       </c>
       <c r="E110" s="6" t="s">
         <v>7</v>
@@ -4526,21 +4638,21 @@
       </c>
       <c r="G110" s="6"/>
       <c r="H110" s="7" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A111" s="5" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="B111" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>12</v>
+        <v>250</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="E111" s="6" t="s">
         <v>7</v>
@@ -4550,21 +4662,21 @@
       </c>
       <c r="G111" s="6"/>
       <c r="H111" s="7" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A112" s="5" t="s">
-        <v>109</v>
+        <v>249</v>
       </c>
       <c r="B112" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>12</v>
+        <v>250</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>110</v>
+        <v>251</v>
       </c>
       <c r="E112" s="6" t="s">
         <v>7</v>
@@ -4574,21 +4686,21 @@
       </c>
       <c r="G112" s="6"/>
       <c r="H112" s="7" t="s">
-        <v>108</v>
+        <v>248</v>
       </c>
     </row>
     <row r="113" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A113" s="5" t="s">
-        <v>431</v>
+        <v>371</v>
       </c>
       <c r="B113" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>218</v>
+        <v>250</v>
       </c>
       <c r="D113" s="5" t="s">
-        <v>219</v>
+        <v>251</v>
       </c>
       <c r="E113" s="6" t="s">
         <v>7</v>
@@ -4598,21 +4710,21 @@
       </c>
       <c r="G113" s="6"/>
       <c r="H113" s="7" t="s">
-        <v>217</v>
+        <v>370</v>
       </c>
     </row>
     <row r="114" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A114" s="5" t="s">
-        <v>438</v>
+        <v>253</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>319</v>
+        <v>250</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>320</v>
+        <v>254</v>
       </c>
       <c r="E114" s="6" t="s">
         <v>7</v>
@@ -4622,21 +4734,21 @@
       </c>
       <c r="G114" s="6"/>
       <c r="H114" s="7" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A115" s="5" t="s">
-        <v>117</v>
+        <v>366</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>118</v>
+        <v>250</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>107</v>
+        <v>254</v>
       </c>
       <c r="E115" s="6" t="s">
         <v>7</v>
@@ -4644,51 +4756,47 @@
       <c r="F115" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G115" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="G115" s="6"/>
       <c r="H115" s="7" t="s">
-        <v>116</v>
+        <v>365</v>
       </c>
     </row>
     <row r="116" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A116" s="5" t="s">
-        <v>447</v>
+        <v>411</v>
       </c>
       <c r="B116" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>275</v>
+        <v>12</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>276</v>
+        <v>13</v>
       </c>
       <c r="E116" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F116" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G116" s="6" t="s">
-        <v>448</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="G116" s="6"/>
       <c r="H116" s="7" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A117" s="5" t="s">
-        <v>442</v>
+        <v>45</v>
       </c>
       <c r="B117" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>130</v>
+        <v>12</v>
       </c>
       <c r="D117" s="5" t="s">
-        <v>131</v>
+        <v>46</v>
       </c>
       <c r="E117" s="6" t="s">
         <v>7</v>
@@ -4696,25 +4804,23 @@
       <c r="F117" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G117" s="6" t="s">
-        <v>443</v>
-      </c>
+      <c r="G117" s="6"/>
       <c r="H117" s="7" t="s">
-        <v>129</v>
+        <v>44</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A118" s="5" t="s">
-        <v>415</v>
+        <v>358</v>
       </c>
       <c r="B118" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>25</v>
+        <v>359</v>
       </c>
       <c r="E118" s="6" t="s">
         <v>7</v>
@@ -4722,25 +4828,23 @@
       <c r="F118" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G118" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="G118" s="6"/>
       <c r="H118" s="7" t="s">
-        <v>23</v>
+        <v>357</v>
       </c>
     </row>
     <row r="119" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A119" s="5" t="s">
-        <v>197</v>
+        <v>300</v>
       </c>
       <c r="B119" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D119" s="5" t="s">
-        <v>25</v>
+        <v>301</v>
       </c>
       <c r="E119" s="6" t="s">
         <v>7</v>
@@ -4748,25 +4852,23 @@
       <c r="F119" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G119" s="6" t="s">
-        <v>198</v>
-      </c>
+      <c r="G119" s="6"/>
       <c r="H119" s="7" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A120" s="5" t="s">
-        <v>380</v>
+        <v>361</v>
       </c>
       <c r="B120" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>231</v>
+        <v>12</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
       <c r="E120" s="6" t="s">
         <v>7</v>
@@ -4776,21 +4878,21 @@
       </c>
       <c r="G120" s="6"/>
       <c r="H120" s="7" t="s">
-        <v>379</v>
+        <v>360</v>
       </c>
     </row>
     <row r="121" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A121" s="5" t="s">
-        <v>347</v>
+        <v>109</v>
       </c>
       <c r="B121" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>231</v>
+        <v>12</v>
       </c>
       <c r="D121" s="5" t="s">
-        <v>348</v>
+        <v>110</v>
       </c>
       <c r="E121" s="6" t="s">
         <v>7</v>
@@ -4800,21 +4902,21 @@
       </c>
       <c r="G121" s="6"/>
       <c r="H121" s="7" t="s">
-        <v>346</v>
+        <v>108</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A122" s="5" t="s">
-        <v>230</v>
+        <v>428</v>
       </c>
       <c r="B122" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="D122" s="5" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="E122" s="6" t="s">
         <v>7</v>
@@ -4824,21 +4926,21 @@
       </c>
       <c r="G122" s="6"/>
       <c r="H122" s="7" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
     </row>
     <row r="123" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A123" s="5" t="s">
-        <v>345</v>
+        <v>435</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>231</v>
+        <v>318</v>
       </c>
       <c r="D123" s="5" t="s">
-        <v>80</v>
+        <v>319</v>
       </c>
       <c r="E123" s="6" t="s">
         <v>7</v>
@@ -4848,21 +4950,21 @@
       </c>
       <c r="G123" s="6"/>
       <c r="H123" s="7" t="s">
-        <v>344</v>
+        <v>317</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A124" s="5" t="s">
-        <v>246</v>
+        <v>117</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>247</v>
+        <v>118</v>
       </c>
       <c r="D124" s="5" t="s">
-        <v>248</v>
+        <v>107</v>
       </c>
       <c r="E124" s="6" t="s">
         <v>7</v>
@@ -4870,23 +4972,25 @@
       <c r="F124" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G124" s="6"/>
+      <c r="G124" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="H124" s="7" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A125" s="5" t="s">
-        <v>425</v>
+        <v>444</v>
       </c>
       <c r="B125" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C125" s="5" t="s">
-        <v>191</v>
+        <v>274</v>
       </c>
       <c r="D125" s="5" t="s">
-        <v>80</v>
+        <v>275</v>
       </c>
       <c r="E125" s="6" t="s">
         <v>7</v>
@@ -4894,23 +4998,25 @@
       <c r="F125" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G125" s="6"/>
+      <c r="G125" s="6" t="s">
+        <v>445</v>
+      </c>
       <c r="H125" s="7" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A126" s="5" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
       <c r="B126" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>191</v>
+        <v>130</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>80</v>
+        <v>131</v>
       </c>
       <c r="E126" s="6" t="s">
         <v>7</v>
@@ -4918,23 +5024,25 @@
       <c r="F126" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G126" s="6"/>
+      <c r="G126" s="6" t="s">
+        <v>440</v>
+      </c>
       <c r="H126" s="7" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A127" s="5" t="s">
-        <v>28</v>
+        <v>412</v>
       </c>
       <c r="B127" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C127" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E127" s="6" t="s">
         <v>7</v>
@@ -4943,72 +5051,74 @@
         <v>7</v>
       </c>
       <c r="G127" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H127" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A128" s="5" t="s">
-        <v>400</v>
+        <v>197</v>
       </c>
       <c r="B128" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="E128" s="6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F128" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G128" s="6"/>
+      <c r="G128" s="6" t="s">
+        <v>198</v>
+      </c>
       <c r="H128" s="7" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A129" s="5" t="s">
-        <v>402</v>
+        <v>377</v>
       </c>
       <c r="B129" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>29</v>
+        <v>230</v>
       </c>
       <c r="D129" s="5" t="s">
-        <v>13</v>
+        <v>375</v>
       </c>
       <c r="E129" s="6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F129" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G129" s="6"/>
       <c r="H129" s="7" t="s">
-        <v>401</v>
+        <v>376</v>
       </c>
     </row>
     <row r="130" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A130" s="5" t="s">
-        <v>62</v>
+        <v>344</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>29</v>
+        <v>230</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>63</v>
+        <v>345</v>
       </c>
       <c r="E130" s="6" t="s">
         <v>7</v>
@@ -5016,25 +5126,23 @@
       <c r="F130" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G130" s="6" t="s">
-        <v>64</v>
-      </c>
+      <c r="G130" s="6"/>
       <c r="H130" s="7" t="s">
-        <v>61</v>
+        <v>343</v>
       </c>
     </row>
     <row r="131" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A131" s="5" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="B131" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>29</v>
+        <v>230</v>
       </c>
       <c r="D131" s="5" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="E131" s="6" t="s">
         <v>7</v>
@@ -5044,21 +5152,21 @@
       </c>
       <c r="G131" s="6"/>
       <c r="H131" s="7" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A132" s="5" t="s">
-        <v>412</v>
+        <v>342</v>
       </c>
       <c r="B132" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>10</v>
+        <v>230</v>
       </c>
       <c r="D132" s="5" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="E132" s="6" t="s">
         <v>7</v>
@@ -5068,47 +5176,45 @@
       </c>
       <c r="G132" s="6"/>
       <c r="H132" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A133" s="5" t="s">
-        <v>70</v>
+        <v>245</v>
       </c>
       <c r="B133" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="D133" s="5" t="s">
-        <v>71</v>
+        <v>247</v>
       </c>
       <c r="E133" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F133" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G133" s="6" t="s">
-        <v>72</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="G133" s="6"/>
       <c r="H133" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A134" s="5" t="s">
-        <v>208</v>
+        <v>422</v>
       </c>
       <c r="B134" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>10</v>
+        <v>191</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E134" s="6" t="s">
         <v>7</v>
@@ -5118,21 +5224,21 @@
       </c>
       <c r="G134" s="6"/>
       <c r="H134" s="7" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A135" s="5" t="s">
-        <v>82</v>
+        <v>431</v>
       </c>
       <c r="B135" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>10</v>
+        <v>191</v>
       </c>
       <c r="D135" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E135" s="6" t="s">
         <v>7</v>
@@ -5140,25 +5246,23 @@
       <c r="F135" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G135" s="6" t="s">
-        <v>84</v>
-      </c>
+      <c r="G135" s="6"/>
       <c r="H135" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A136" s="5" t="s">
-        <v>86</v>
+        <v>28</v>
       </c>
       <c r="B136" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>83</v>
+        <v>30</v>
       </c>
       <c r="E136" s="6" t="s">
         <v>7</v>
@@ -5167,96 +5271,96 @@
         <v>7</v>
       </c>
       <c r="G136" s="6" t="s">
-        <v>87</v>
+        <v>31</v>
       </c>
       <c r="H136" s="7" t="s">
-        <v>85</v>
+        <v>27</v>
       </c>
     </row>
     <row r="137" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A137" s="5" t="s">
-        <v>359</v>
+        <v>397</v>
       </c>
       <c r="B137" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C137" s="5" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D137" s="5" t="s">
-        <v>83</v>
+        <v>13</v>
       </c>
       <c r="E137" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F137" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G137" s="6"/>
       <c r="H137" s="7" t="s">
-        <v>358</v>
+        <v>396</v>
       </c>
     </row>
     <row r="138" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A138" s="5" t="s">
-        <v>79</v>
+        <v>399</v>
       </c>
       <c r="B138" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C138" s="5" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D138" s="5" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="E138" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F138" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G138" s="6"/>
       <c r="H138" s="7" t="s">
-        <v>78</v>
+        <v>398</v>
       </c>
     </row>
     <row r="139" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A139" s="5" t="s">
-        <v>206</v>
+        <v>483</v>
       </c>
       <c r="B139" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C139" s="5" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D139" s="5" t="s">
-        <v>80</v>
+        <v>484</v>
       </c>
       <c r="E139" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F139" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G139" s="6"/>
       <c r="H139" s="7" t="s">
-        <v>205</v>
+        <v>485</v>
       </c>
     </row>
     <row r="140" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A140" s="5" t="s">
-        <v>203</v>
+        <v>62</v>
       </c>
       <c r="B140" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>204</v>
+        <v>63</v>
       </c>
       <c r="E140" s="6" t="s">
         <v>7</v>
@@ -5264,23 +5368,25 @@
       <c r="F140" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G140" s="6"/>
+      <c r="G140" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="H140" s="7" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A141" s="5" t="s">
-        <v>33</v>
+        <v>240</v>
       </c>
       <c r="B141" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C141" s="5" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D141" s="5" t="s">
-        <v>34</v>
+        <v>241</v>
       </c>
       <c r="E141" s="6" t="s">
         <v>7</v>
@@ -5288,16 +5394,14 @@
       <c r="F141" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G141" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="G141" s="6"/>
       <c r="H141" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A142" s="5" t="s">
-        <v>37</v>
+        <v>409</v>
       </c>
       <c r="B142" s="6" t="s">
         <v>6</v>
@@ -5306,7 +5410,7 @@
         <v>10</v>
       </c>
       <c r="D142" s="5" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="E142" s="6" t="s">
         <v>7</v>
@@ -5314,16 +5418,14 @@
       <c r="F142" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G142" s="6" t="s">
-        <v>38</v>
-      </c>
+      <c r="G142" s="6"/>
       <c r="H142" s="7" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
     </row>
     <row r="143" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A143" s="5" t="s">
-        <v>281</v>
+        <v>70</v>
       </c>
       <c r="B143" s="6" t="s">
         <v>6</v>
@@ -5332,7 +5434,7 @@
         <v>10</v>
       </c>
       <c r="D143" s="5" t="s">
-        <v>282</v>
+        <v>71</v>
       </c>
       <c r="E143" s="6" t="s">
         <v>7</v>
@@ -5340,14 +5442,16 @@
       <c r="F143" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G143" s="6"/>
+      <c r="G143" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="H143" s="7" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A144" s="5" t="s">
-        <v>284</v>
+        <v>207</v>
       </c>
       <c r="B144" s="6" t="s">
         <v>6</v>
@@ -5356,7 +5460,7 @@
         <v>10</v>
       </c>
       <c r="D144" s="5" t="s">
-        <v>285</v>
+        <v>71</v>
       </c>
       <c r="E144" s="6" t="s">
         <v>7</v>
@@ -5366,15 +5470,353 @@
       </c>
       <c r="G144" s="6"/>
       <c r="H144" s="7" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A145" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B145" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C145" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D145" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E145" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F145" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G145" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="H145" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A146" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B146" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C146" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D146" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E146" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F146" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G146" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="H146" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A147" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="B147" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C147" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D147" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E147" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F147" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G147" s="9"/>
+      <c r="H147" s="10" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A148" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B148" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C148" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D148" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E148" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F148" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G148" s="9"/>
+      <c r="H148" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A149" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="B149" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C149" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D149" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E149" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F149" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G149" s="9"/>
+      <c r="H149" s="10" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A150" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="B150" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C150" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D150" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="E150" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F150" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G150" s="9"/>
+      <c r="H150" s="10" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A151" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B151" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C151" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D151" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E151" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F151" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G151" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H151" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A152" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B152" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C152" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D152" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E152" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F152" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G152" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H152" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A153" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="B153" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C153" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D153" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="E153" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F153" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G153" s="9"/>
+      <c r="H153" s="10" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A154" s="8" t="s">
         <v>283</v>
       </c>
+      <c r="B154" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C154" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D154" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="E154" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F154" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G154" s="9"/>
+      <c r="H154" s="10" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A155" s="8"/>
+      <c r="B155" s="9"/>
+      <c r="C155" s="8"/>
+      <c r="D155" s="8"/>
+      <c r="E155" s="9"/>
+      <c r="F155" s="9"/>
+      <c r="G155" s="9"/>
+      <c r="H155" s="10"/>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A156" s="8"/>
+      <c r="B156" s="9"/>
+      <c r="C156" s="8"/>
+      <c r="D156" s="8"/>
+      <c r="E156" s="9"/>
+      <c r="F156" s="9"/>
+      <c r="G156" s="9"/>
+      <c r="H156" s="10"/>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A157" s="8"/>
+      <c r="B157" s="9"/>
+      <c r="C157" s="8"/>
+      <c r="D157" s="8"/>
+      <c r="E157" s="9"/>
+      <c r="F157" s="9"/>
+      <c r="G157" s="9"/>
+      <c r="H157" s="10"/>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A158" s="8"/>
+      <c r="B158" s="9"/>
+      <c r="C158" s="8"/>
+      <c r="D158" s="8"/>
+      <c r="E158" s="9"/>
+      <c r="F158" s="9"/>
+      <c r="G158" s="9"/>
+      <c r="H158" s="10"/>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A159" s="8"/>
+      <c r="B159" s="9"/>
+      <c r="C159" s="8"/>
+      <c r="D159" s="8"/>
+      <c r="E159" s="9"/>
+      <c r="F159" s="9"/>
+      <c r="G159" s="9"/>
+      <c r="H159" s="10"/>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A160" s="8"/>
+      <c r="B160" s="9"/>
+      <c r="C160" s="8"/>
+      <c r="D160" s="8"/>
+      <c r="E160" s="9"/>
+      <c r="F160" s="9"/>
+      <c r="G160" s="9"/>
+      <c r="H160" s="10"/>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A161" s="8"/>
+      <c r="B161" s="9"/>
+      <c r="C161" s="8"/>
+      <c r="D161" s="8"/>
+      <c r="E161" s="9"/>
+      <c r="F161" s="9"/>
+      <c r="G161" s="9"/>
+      <c r="H161" s="10"/>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A162" s="8"/>
+      <c r="B162" s="9"/>
+      <c r="C162" s="8"/>
+      <c r="D162" s="8"/>
+      <c r="E162" s="9"/>
+      <c r="F162" s="9"/>
+      <c r="G162" s="9"/>
+      <c r="H162" s="10"/>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A163" s="8"/>
+      <c r="B163" s="9"/>
+      <c r="C163" s="8"/>
+      <c r="D163" s="8"/>
+      <c r="E163" s="9"/>
+      <c r="F163" s="9"/>
+      <c r="G163" s="9"/>
+      <c r="H163" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q10" xr:uid="{B9FACE88-1C57-4099-A43D-8DA482706A91}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H144">
-    <sortCondition ref="C8:C144"/>
-    <sortCondition ref="D8:D144"/>
-    <sortCondition ref="H8:H144"/>
+  <autoFilter ref="A1:Q165" xr:uid="{B9FACE88-1C57-4099-A43D-8DA482706A91}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H165">
+    <sortCondition ref="C8:C165"/>
+    <sortCondition ref="D8:D165"/>
+    <sortCondition ref="H8:H165"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated rules based on #461, #466, #464 and #453
</commit_message>
<xml_diff>
--- a/Deliverables/RULES/USDM_CORE_Rules.xlsx
+++ b/Deliverables/RULES/USDM_CORE_Rules.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stack\CL027\Publish\CORE\3.6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E7272E-D78E-4FB7-A5F3-6E0C59E2299F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0DDF6B-2FC5-41B3-81C7-A1C627AE7030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9780" yWindow="-20040" windowWidth="22170" windowHeight="18135" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
   </bookViews>
   <sheets>
-    <sheet name="Release 3.0 and 3.6 CORE rules" sheetId="1" r:id="rId1"/>
+    <sheet name="Version 3.0 and 3.6 CORE rules" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Release 3.0 and 3.6 CORE rules'!$A$1:$H$182</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Version 3.0 and 3.6 CORE rules'!$A$1:$H$182</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1365" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="610">
   <si>
     <t>Textual statement of rule</t>
   </si>
@@ -587,9 +587,6 @@
     <t>CHK0108</t>
   </si>
   <si>
-    <t>The value for each timing must be specified in ISO 8601 duration format.</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
@@ -788,18 +785,12 @@
     <t>CHK0143</t>
   </si>
   <si>
-    <t>The lower limit of a timing window must be specified in ISO 8601 duration format.</t>
-  </si>
-  <si>
     <t>windowLower</t>
   </si>
   <si>
     <t>CHK0144</t>
   </si>
   <si>
-    <t>The upper limit of a timing window must be specified in ISO 8601 duration format.</t>
-  </si>
-  <si>
     <t>windowUpper</t>
   </si>
   <si>
@@ -1715,9 +1706,6 @@
     <t>Within a study version, if more than 1 business therapeutic area is defined then they must be distinct.</t>
   </si>
   <si>
-    <t>A window must not be defined for an anchor timing (e.g. type is "Fixed Reference".</t>
-  </si>
-  <si>
     <t>Within a study design, there must be exactly one scheduled timeline which identifies as the main Timeline.</t>
   </si>
   <si>
@@ -1815,6 +1803,72 @@
   </si>
   <si>
     <t>Narrative content item text is expected to be HTML formatted.</t>
+  </si>
+  <si>
+    <t>A window must not be defined for an anchor timing (i.e., type is "Fixed Reference").</t>
+  </si>
+  <si>
+    <t>The value for each timing must be a non-negative duration specified in ISO 8601 format.</t>
+  </si>
+  <si>
+    <t>When specified, the lower limit of a timing window must be a non-negative duration in ISO 8601 format.</t>
+  </si>
+  <si>
+    <t>When specified, the upper limit of a timing window must be a non-negative duration in ISO 8601 format.</t>
+  </si>
+  <si>
+    <t>CHK0232</t>
+  </si>
+  <si>
+    <t>A planned sex must ether include a single entry of male or female or both female and male as entries.</t>
+  </si>
+  <si>
+    <t>CHK0233</t>
+  </si>
+  <si>
+    <t>Every study role must apply to either a study version or at least one study design, but not both.</t>
+  </si>
+  <si>
+    <t>StudyRole</t>
+  </si>
+  <si>
+    <t>CHK0234</t>
+  </si>
+  <si>
+    <t>A study role must not reference both assigned persons and organizations.</t>
+  </si>
+  <si>
+    <t>assignedPersons, organizations</t>
+  </si>
+  <si>
+    <t>CHK0235</t>
+  </si>
+  <si>
+    <t>A masking is not expected to be defined for any study role in a study design with an open label blinding schema.</t>
+  </si>
+  <si>
+    <t>masking</t>
+  </si>
+  <si>
+    <t>CHK0236</t>
+  </si>
+  <si>
+    <t>A masking is expected to be defined for at least two study roles in a study design with a double blind blinding schema.</t>
+  </si>
+  <si>
+    <t>CHK0237</t>
+  </si>
+  <si>
+    <t>A masking is expected to be defined for at least one study role in a study design with a blinding schema that is not open label or double blind.</t>
+  </si>
+  <si>
+    <t>DDF00060</t>
+  </si>
+  <si>
+    <t>DDF00061</t>
+  </si>
+  <si>
+    <t>DDF00062</t>
   </si>
 </sst>
 </file>
@@ -1923,6 +1977,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2242,10 +2300,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FACE88-1C57-4099-A43D-8DA482706A91}">
-  <dimension ref="A1:H188"/>
+  <dimension ref="A1:H194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
-      <selection activeCell="A178" sqref="A178"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2264,10 +2322,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>353</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>356</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>1</v>
@@ -2279,15 +2337,15 @@
         <v>3</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
@@ -2311,7 +2369,7 @@
     </row>
     <row r="3" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>6</v>
@@ -2335,7 +2393,7 @@
     </row>
     <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>6</v>
@@ -2354,12 +2412,12 @@
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="7" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>6</v>
@@ -2378,7 +2436,7 @@
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="7" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -2433,16 +2491,16 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>14</v>
@@ -2452,21 +2510,21 @@
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="7" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>107</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>14</v>
@@ -2476,12 +2534,12 @@
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="7" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>6</v>
@@ -2500,7 +2558,7 @@
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -2577,7 +2635,7 @@
     </row>
     <row r="14" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>6</v>
@@ -2596,7 +2654,7 @@
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="7" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -2625,7 +2683,7 @@
     </row>
     <row r="16" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>107</v>
@@ -2634,7 +2692,7 @@
         <v>131</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>7</v>
@@ -2644,12 +2702,12 @@
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="7" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>6</v>
@@ -2668,12 +2726,12 @@
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="7" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>6</v>
@@ -2692,12 +2750,12 @@
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="7" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>6</v>
@@ -2716,7 +2774,7 @@
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="7" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -2771,7 +2829,7 @@
     </row>
     <row r="22" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>6</v>
@@ -2813,7 +2871,7 @@
         <v>7</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="H23" s="7" t="s">
         <v>149</v>
@@ -2821,16 +2879,16 @@
     </row>
     <row r="24" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>14</v>
@@ -2840,18 +2898,18 @@
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="7" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>75</v>
@@ -2864,21 +2922,21 @@
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="7" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>14</v>
@@ -2888,21 +2946,21 @@
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="7" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>14</v>
@@ -2912,21 +2970,21 @@
       </c>
       <c r="G27" s="6"/>
       <c r="H27" s="7" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>107</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>14</v>
@@ -2936,21 +2994,21 @@
       </c>
       <c r="G28" s="6"/>
       <c r="H28" s="7" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>14</v>
@@ -2960,21 +3018,21 @@
       </c>
       <c r="G29" s="6"/>
       <c r="H29" s="7" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>14</v>
@@ -2984,7 +3042,7 @@
       </c>
       <c r="G30" s="6"/>
       <c r="H30" s="7" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -3015,7 +3073,7 @@
     </row>
     <row r="32" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>107</v>
@@ -3024,7 +3082,7 @@
         <v>39</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>7</v>
@@ -3033,24 +3091,24 @@
         <v>7</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C33" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>212</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>213</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>7</v>
@@ -3060,21 +3118,21 @@
       </c>
       <c r="G33" s="6"/>
       <c r="H33" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>7</v>
@@ -3084,12 +3142,12 @@
       </c>
       <c r="G34" s="6"/>
       <c r="H34" s="7" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>6</v>
@@ -3107,7 +3165,7 @@
         <v>7</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="H35" s="7" t="s">
         <v>152</v>
@@ -3115,7 +3173,7 @@
     </row>
     <row r="36" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>107</v>
@@ -3134,21 +3192,21 @@
       </c>
       <c r="G36" s="6"/>
       <c r="H36" s="7" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>107</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>7</v>
@@ -3158,7 +3216,7 @@
       </c>
       <c r="G37" s="6"/>
       <c r="H37" s="7" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -3181,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="H38" s="7" t="s">
         <v>125</v>
@@ -3195,7 +3253,7 @@
         <v>6</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>124</v>
@@ -3207,7 +3265,7 @@
         <v>7</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="H39" s="7" t="s">
         <v>122</v>
@@ -3241,16 +3299,16 @@
     </row>
     <row r="41" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>107</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>7</v>
@@ -3259,24 +3317,24 @@
         <v>7</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>107</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>7</v>
@@ -3286,21 +3344,21 @@
       </c>
       <c r="G42" s="6"/>
       <c r="H42" s="7" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>7</v>
@@ -3310,7 +3368,7 @@
       </c>
       <c r="G43" s="6"/>
       <c r="H43" s="7" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -3333,7 +3391,7 @@
         <v>7</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="H44" s="7" t="s">
         <v>61</v>
@@ -3365,7 +3423,7 @@
     </row>
     <row r="46" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>6</v>
@@ -3384,21 +3442,21 @@
       </c>
       <c r="G46" s="6"/>
       <c r="H46" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>7</v>
@@ -3407,15 +3465,15 @@
         <v>7</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>6</v>
@@ -3424,7 +3482,7 @@
         <v>168</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>7</v>
@@ -3434,7 +3492,7 @@
       </c>
       <c r="G48" s="6"/>
       <c r="H48" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
@@ -3465,7 +3523,7 @@
     </row>
     <row r="50" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>6</v>
@@ -3489,7 +3547,7 @@
     </row>
     <row r="51" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>107</v>
@@ -3508,12 +3566,12 @@
       </c>
       <c r="G51" s="6"/>
       <c r="H51" s="7" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>6</v>
@@ -3522,7 +3580,7 @@
         <v>106</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>7</v>
@@ -3531,15 +3589,15 @@
         <v>7</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>6</v>
@@ -3548,7 +3606,7 @@
         <v>106</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>7</v>
@@ -3558,12 +3616,12 @@
       </c>
       <c r="G53" s="6"/>
       <c r="H53" s="7" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>6</v>
@@ -3572,7 +3630,7 @@
         <v>106</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>7</v>
@@ -3581,15 +3639,15 @@
         <v>14</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>6</v>
@@ -3598,7 +3656,7 @@
         <v>106</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>7</v>
@@ -3608,12 +3666,12 @@
       </c>
       <c r="G55" s="6"/>
       <c r="H55" s="7" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>6</v>
@@ -3622,7 +3680,7 @@
         <v>106</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>14</v>
@@ -3632,12 +3690,12 @@
       </c>
       <c r="G56" s="6"/>
       <c r="H56" s="7" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>6</v>
@@ -3646,7 +3704,7 @@
         <v>106</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>14</v>
@@ -3656,12 +3714,12 @@
       </c>
       <c r="G57" s="6"/>
       <c r="H57" s="7" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>107</v>
@@ -3685,7 +3743,7 @@
     </row>
     <row r="59" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>6</v>
@@ -3704,12 +3762,12 @@
       </c>
       <c r="G59" s="6"/>
       <c r="H59" s="7" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>6</v>
@@ -3718,7 +3776,7 @@
         <v>106</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>7</v>
@@ -3728,12 +3786,12 @@
       </c>
       <c r="G60" s="6"/>
       <c r="H60" s="7" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>6</v>
@@ -3752,7 +3810,7 @@
       </c>
       <c r="G61" s="6"/>
       <c r="H61" s="7" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -3783,7 +3841,7 @@
     </row>
     <row r="63" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>6</v>
@@ -3807,7 +3865,7 @@
     </row>
     <row r="64" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>6</v>
@@ -3826,21 +3884,21 @@
       </c>
       <c r="G64" s="6"/>
       <c r="H64" s="7" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>107</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>7</v>
@@ -3850,18 +3908,18 @@
       </c>
       <c r="G65" s="6"/>
       <c r="H65" s="7" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="B66" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D66" s="5" t="s">
         <v>75</v>
@@ -3874,12 +3932,12 @@
       </c>
       <c r="G66" s="6"/>
       <c r="H66" s="7" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="B67" s="6" t="s">
         <v>6</v>
@@ -3888,7 +3946,7 @@
         <v>159</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>7</v>
@@ -3898,12 +3956,12 @@
       </c>
       <c r="G67" s="6"/>
       <c r="H67" s="7" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="B68" s="6" t="s">
         <v>6</v>
@@ -3922,21 +3980,21 @@
       </c>
       <c r="G68" s="6"/>
       <c r="H68" s="7" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B69" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="E69" s="6" t="s">
         <v>7</v>
@@ -3945,24 +4003,24 @@
         <v>7</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="H69" s="7" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="B70" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>7</v>
@@ -3972,12 +4030,12 @@
       </c>
       <c r="G70" s="6"/>
       <c r="H70" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B71" s="6" t="s">
         <v>107</v>
@@ -3986,7 +4044,7 @@
         <v>118</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="E71" s="6" t="s">
         <v>14</v>
@@ -3996,12 +4054,12 @@
       </c>
       <c r="G71" s="6"/>
       <c r="H71" s="7" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B72" s="6" t="s">
         <v>6</v>
@@ -4010,7 +4068,7 @@
         <v>118</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="E72" s="6" t="s">
         <v>14</v>
@@ -4020,12 +4078,12 @@
       </c>
       <c r="G72" s="6"/>
       <c r="H72" s="7" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B73" s="6" t="s">
         <v>6</v>
@@ -4049,7 +4107,7 @@
     </row>
     <row r="74" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A74" s="5" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B74" s="6" t="s">
         <v>6</v>
@@ -4058,7 +4116,7 @@
         <v>118</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="E74" s="6" t="s">
         <v>14</v>
@@ -4068,12 +4126,12 @@
       </c>
       <c r="G74" s="6"/>
       <c r="H74" s="7" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B75" s="6" t="s">
         <v>6</v>
@@ -4082,7 +4140,7 @@
         <v>118</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="E75" s="6" t="s">
         <v>14</v>
@@ -4092,12 +4150,12 @@
       </c>
       <c r="G75" s="6"/>
       <c r="H75" s="7" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="B76" s="6" t="s">
         <v>6</v>
@@ -4121,7 +4179,7 @@
     </row>
     <row r="77" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A77" s="5" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B77" s="6" t="s">
         <v>6</v>
@@ -4140,12 +4198,12 @@
       </c>
       <c r="G77" s="6"/>
       <c r="H77" s="7" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="B78" s="6" t="s">
         <v>107</v>
@@ -4164,7 +4222,7 @@
       </c>
       <c r="G78" s="6"/>
       <c r="H78" s="7" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
@@ -4175,7 +4233,7 @@
         <v>6</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>113</v>
@@ -4188,18 +4246,18 @@
       </c>
       <c r="G79" s="6"/>
       <c r="H79" s="7" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="B80" s="6" t="s">
         <v>107</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>113</v>
@@ -4212,12 +4270,12 @@
       </c>
       <c r="G80" s="6"/>
       <c r="H80" s="7" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="B81" s="6" t="s">
         <v>6</v>
@@ -4241,7 +4299,7 @@
     </row>
     <row r="82" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="B82" s="6" t="s">
         <v>6</v>
@@ -4260,21 +4318,21 @@
       </c>
       <c r="G82" s="6"/>
       <c r="H82" s="7" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="B83" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="E83" s="6" t="s">
         <v>7</v>
@@ -4284,21 +4342,21 @@
       </c>
       <c r="G83" s="6"/>
       <c r="H83" s="7" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="B84" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C84" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="D84" s="5" t="s">
         <v>238</v>
-      </c>
-      <c r="D84" s="5" t="s">
-        <v>239</v>
       </c>
       <c r="E84" s="6" t="s">
         <v>7</v>
@@ -4308,21 +4366,21 @@
       </c>
       <c r="G84" s="6"/>
       <c r="H84" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="116" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="B85" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C85" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="D85" s="5" t="s">
         <v>238</v>
-      </c>
-      <c r="D85" s="5" t="s">
-        <v>239</v>
       </c>
       <c r="E85" s="6" t="s">
         <v>7</v>
@@ -4332,12 +4390,12 @@
       </c>
       <c r="G85" s="6"/>
       <c r="H85" s="7" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="B86" s="6" t="s">
         <v>6</v>
@@ -4355,7 +4413,7 @@
         <v>7</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="H86" s="7" t="s">
         <v>146</v>
@@ -4363,7 +4421,7 @@
     </row>
     <row r="87" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B87" s="6" t="s">
         <v>107</v>
@@ -4387,16 +4445,16 @@
     </row>
     <row r="88" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B88" s="6" t="s">
         <v>107</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="E88" s="6" t="s">
         <v>7</v>
@@ -4405,24 +4463,24 @@
         <v>7</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="H88" s="7" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B89" s="6" t="s">
         <v>107</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="E89" s="6" t="s">
         <v>14</v>
@@ -4432,21 +4490,21 @@
       </c>
       <c r="G89" s="6"/>
       <c r="H89" s="7" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B90" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="E90" s="6" t="s">
         <v>7</v>
@@ -4456,18 +4514,18 @@
       </c>
       <c r="G90" s="6"/>
       <c r="H90" s="7" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A91" s="5" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="B91" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="D91" s="5" t="s">
         <v>47</v>
@@ -4480,18 +4538,18 @@
       </c>
       <c r="G91" s="6"/>
       <c r="H91" s="7" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="B92" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="D92" s="5" t="s">
         <v>75</v>
@@ -4504,12 +4562,12 @@
       </c>
       <c r="G92" s="6"/>
       <c r="H92" s="7" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A93" s="5" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B93" s="6" t="s">
         <v>6</v>
@@ -4518,7 +4576,7 @@
         <v>50</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E93" s="6" t="s">
         <v>7</v>
@@ -4528,7 +4586,7 @@
       </c>
       <c r="G93" s="6"/>
       <c r="H93" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -4557,7 +4615,7 @@
     </row>
     <row r="95" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A95" s="5" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="B95" s="6" t="s">
         <v>107</v>
@@ -4576,7 +4634,7 @@
       </c>
       <c r="G95" s="6"/>
       <c r="H95" s="7" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -4599,7 +4657,7 @@
         <v>7</v>
       </c>
       <c r="G96" s="6" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="H96" s="7" t="s">
         <v>176</v>
@@ -4607,7 +4665,7 @@
     </row>
     <row r="97" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A97" s="5" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B97" s="6" t="s">
         <v>6</v>
@@ -4626,7 +4684,7 @@
       </c>
       <c r="G97" s="6"/>
       <c r="H97" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -4657,7 +4715,7 @@
     </row>
     <row r="99" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A99" s="5" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B99" s="6" t="s">
         <v>6</v>
@@ -4676,7 +4734,7 @@
       </c>
       <c r="G99" s="6"/>
       <c r="H99" s="7" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -4707,17 +4765,17 @@
     </row>
     <row r="101" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A101" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D101" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="B101" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C101" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="D101" s="5" t="s">
-        <v>247</v>
-      </c>
       <c r="E101" s="6" t="s">
         <v>7</v>
       </c>
@@ -4725,21 +4783,21 @@
         <v>7</v>
       </c>
       <c r="G101" s="6" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="H101" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B102" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D102" s="5" t="s">
         <v>172</v>
@@ -4752,21 +4810,21 @@
       </c>
       <c r="G102" s="6"/>
       <c r="H102" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A103" s="5" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B103" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E103" s="6" t="s">
         <v>14</v>
@@ -4776,21 +4834,21 @@
       </c>
       <c r="G103" s="6"/>
       <c r="H103" s="7" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A104" s="5" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B104" s="6" t="s">
         <v>107</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E104" s="6" t="s">
         <v>7</v>
@@ -4800,18 +4858,18 @@
       </c>
       <c r="G104" s="6"/>
       <c r="H104" s="7" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A105" s="8" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B105" s="6" t="s">
         <v>107</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D105" s="5" t="s">
         <v>178</v>
@@ -4824,18 +4882,18 @@
       </c>
       <c r="G105" s="6"/>
       <c r="H105" s="7" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A106" s="5" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B106" s="6" t="s">
         <v>107</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D106" s="5" t="s">
         <v>84</v>
@@ -4848,12 +4906,12 @@
       </c>
       <c r="G106" s="6"/>
       <c r="H106" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A107" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B107" s="6" t="s">
         <v>6</v>
@@ -4862,7 +4920,7 @@
         <v>70</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E107" s="6" t="s">
         <v>7</v>
@@ -4872,12 +4930,12 @@
       </c>
       <c r="G107" s="6"/>
       <c r="H107" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A108" s="5" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="B108" s="6" t="s">
         <v>6</v>
@@ -4903,16 +4961,16 @@
     </row>
     <row r="109" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A109" s="5" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="B109" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="E109" s="6" t="s">
         <v>14</v>
@@ -4922,21 +4980,21 @@
       </c>
       <c r="G109" s="6"/>
       <c r="H109" s="7" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A110" s="5" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="B110" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E110" s="6" t="s">
         <v>7</v>
@@ -4946,21 +5004,21 @@
       </c>
       <c r="G110" s="6"/>
       <c r="H110" s="7" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A111" s="5" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B111" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="E111" s="6" t="s">
         <v>14</v>
@@ -4969,15 +5027,15 @@
         <v>15</v>
       </c>
       <c r="G111" s="6" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="H111" s="7" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A112" s="5" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B112" s="6" t="s">
         <v>6</v>
@@ -4986,7 +5044,7 @@
         <v>166</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="E112" s="6" t="s">
         <v>7</v>
@@ -4996,12 +5054,12 @@
       </c>
       <c r="G112" s="6"/>
       <c r="H112" s="7" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="113" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A113" s="5" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B113" s="6" t="s">
         <v>6</v>
@@ -5019,7 +5077,7 @@
         <v>7</v>
       </c>
       <c r="G113" s="6" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="H113" s="7" t="s">
         <v>165</v>
@@ -5027,7 +5085,7 @@
     </row>
     <row r="114" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A114" s="5" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B114" s="6" t="s">
         <v>6</v>
@@ -5045,15 +5103,15 @@
         <v>7</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="H114" s="7" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="115" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A115" s="5" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="B115" s="6" t="s">
         <v>6</v>
@@ -5062,7 +5120,7 @@
         <v>94</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="E115" s="6" t="s">
         <v>7</v>
@@ -5072,12 +5130,12 @@
       </c>
       <c r="G115" s="6"/>
       <c r="H115" s="7" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" s="5" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B116" s="6" t="s">
         <v>6</v>
@@ -5086,7 +5144,7 @@
         <v>94</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E116" s="6" t="s">
         <v>7</v>
@@ -5096,12 +5154,12 @@
       </c>
       <c r="G116" s="6"/>
       <c r="H116" s="7" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="117" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A117" s="5" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B117" s="6" t="s">
         <v>6</v>
@@ -5110,7 +5168,7 @@
         <v>94</v>
       </c>
       <c r="D117" s="5" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E117" s="6" t="s">
         <v>7</v>
@@ -5120,12 +5178,12 @@
       </c>
       <c r="G117" s="6"/>
       <c r="H117" s="7" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A118" s="5" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="B118" s="6" t="s">
         <v>6</v>
@@ -5151,7 +5209,7 @@
     </row>
     <row r="119" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A119" s="5" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B119" s="6" t="s">
         <v>6</v>
@@ -5169,15 +5227,15 @@
         <v>7</v>
       </c>
       <c r="G119" s="6" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="H119" s="7" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120" s="5" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B120" s="6" t="s">
         <v>6</v>
@@ -5196,12 +5254,12 @@
       </c>
       <c r="G120" s="6"/>
       <c r="H120" s="7" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="121" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A121" s="5" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="B121" s="6" t="s">
         <v>6</v>
@@ -5220,18 +5278,18 @@
       </c>
       <c r="G121" s="6"/>
       <c r="H121" s="7" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A122" s="5" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B122" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="D122" s="5" t="s">
         <v>75</v>
@@ -5244,7 +5302,7 @@
       </c>
       <c r="G122" s="6"/>
       <c r="H122" s="7" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="123" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -5255,10 +5313,10 @@
         <v>6</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D123" s="5" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="E123" s="6" t="s">
         <v>14</v>
@@ -5268,21 +5326,21 @@
       </c>
       <c r="G123" s="6"/>
       <c r="H123" s="7" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A124" s="5" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B124" s="6" t="s">
         <v>107</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D124" s="5" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="E124" s="6" t="s">
         <v>14</v>
@@ -5292,21 +5350,21 @@
       </c>
       <c r="G124" s="6"/>
       <c r="H124" s="7" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A125" s="5" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="B125" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C125" s="5" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D125" s="5" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="E125" s="6" t="s">
         <v>14</v>
@@ -5316,21 +5374,21 @@
       </c>
       <c r="G125" s="6"/>
       <c r="H125" s="7" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="126" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A126" s="5" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="B126" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E126" s="6" t="s">
         <v>7</v>
@@ -5340,21 +5398,21 @@
       </c>
       <c r="G126" s="6"/>
       <c r="H126" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="127" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A127" s="5" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="B127" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C127" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E127" s="6" t="s">
         <v>7</v>
@@ -5364,21 +5422,21 @@
       </c>
       <c r="G127" s="6"/>
       <c r="H127" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="128" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A128" s="5" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B128" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E128" s="6" t="s">
         <v>7</v>
@@ -5388,21 +5446,21 @@
       </c>
       <c r="G128" s="6"/>
       <c r="H128" s="7" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A129" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B129" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D129" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E129" s="6" t="s">
         <v>7</v>
@@ -5412,21 +5470,21 @@
       </c>
       <c r="G129" s="6"/>
       <c r="H129" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="130" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A130" s="5" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>107</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E130" s="6" t="s">
         <v>7</v>
@@ -5436,21 +5494,21 @@
       </c>
       <c r="G130" s="6"/>
       <c r="H130" s="7" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="131" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A131" s="5" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B131" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D131" s="5" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E131" s="6" t="s">
         <v>7</v>
@@ -5459,24 +5517,24 @@
         <v>7</v>
       </c>
       <c r="G131" s="6" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="H131" s="7" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="132" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A132" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="B132" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C132" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D132" s="5" t="s">
         <v>225</v>
-      </c>
-      <c r="D132" s="5" t="s">
-        <v>226</v>
       </c>
       <c r="E132" s="6" t="s">
         <v>7</v>
@@ -5486,22 +5544,22 @@
       </c>
       <c r="G132" s="6"/>
       <c r="H132" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="133" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A133" s="5" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B133" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C133" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D133" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="D133" s="5" t="s">
-        <v>226</v>
-      </c>
       <c r="E133" s="6" t="s">
         <v>7</v>
       </c>
@@ -5509,24 +5567,24 @@
         <v>7</v>
       </c>
       <c r="G133" s="6" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="H133" s="7" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="134" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A134" s="5" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B134" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E134" s="6" t="s">
         <v>7</v>
@@ -5536,21 +5594,21 @@
       </c>
       <c r="G134" s="6"/>
       <c r="H134" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="135" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A135" s="5" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B135" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D135" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E135" s="6" t="s">
         <v>7</v>
@@ -5559,15 +5617,15 @@
         <v>7</v>
       </c>
       <c r="G135" s="6" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="H135" s="7" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="136" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A136" s="5" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B136" s="6" t="s">
         <v>6</v>
@@ -5586,7 +5644,7 @@
       </c>
       <c r="G136" s="6"/>
       <c r="H136" s="7" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="137" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -5615,7 +5673,7 @@
     </row>
     <row r="138" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A138" s="5" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B138" s="6" t="s">
         <v>6</v>
@@ -5634,12 +5692,12 @@
       </c>
       <c r="G138" s="6"/>
       <c r="H138" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="139" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A139" s="5" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B139" s="6" t="s">
         <v>6</v>
@@ -5648,7 +5706,7 @@
         <v>12</v>
       </c>
       <c r="D139" s="5" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="E139" s="6" t="s">
         <v>7</v>
@@ -5658,12 +5716,12 @@
       </c>
       <c r="G139" s="6"/>
       <c r="H139" s="7" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="140" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A140" s="5" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B140" s="6" t="s">
         <v>6</v>
@@ -5672,7 +5730,7 @@
         <v>12</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="E140" s="6" t="s">
         <v>7</v>
@@ -5682,12 +5740,12 @@
       </c>
       <c r="G140" s="6"/>
       <c r="H140" s="7" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="141" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A141" s="5" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B141" s="6" t="s">
         <v>6</v>
@@ -5696,7 +5754,7 @@
         <v>12</v>
       </c>
       <c r="D141" s="5" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="E141" s="6" t="s">
         <v>7</v>
@@ -5705,10 +5763,10 @@
         <v>7</v>
       </c>
       <c r="G141" s="6" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="H141" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="142" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -5737,7 +5795,7 @@
     </row>
     <row r="143" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A143" s="5" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="B143" s="6" t="s">
         <v>6</v>
@@ -5756,45 +5814,45 @@
       </c>
       <c r="G143" s="6"/>
       <c r="H143" s="7" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="144" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A144" s="5" t="s">
-        <v>374</v>
+        <v>593</v>
       </c>
       <c r="B144" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>197</v>
+        <v>12</v>
       </c>
       <c r="D144" s="5" t="s">
-        <v>198</v>
+        <v>103</v>
       </c>
       <c r="E144" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F144" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G144" s="6"/>
       <c r="H144" s="7" t="s">
-        <v>196</v>
+        <v>592</v>
       </c>
     </row>
     <row r="145" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A145" s="5" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>107</v>
+        <v>6</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>279</v>
+        <v>196</v>
       </c>
       <c r="D145" s="5" t="s">
-        <v>280</v>
+        <v>197</v>
       </c>
       <c r="E145" s="6" t="s">
         <v>7</v>
@@ -5804,21 +5862,21 @@
       </c>
       <c r="G145" s="6"/>
       <c r="H145" s="7" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A146" s="5" t="s">
-        <v>563</v>
+        <v>377</v>
       </c>
       <c r="B146" s="6" t="s">
         <v>107</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>109</v>
+        <v>276</v>
       </c>
       <c r="D146" s="5" t="s">
-        <v>100</v>
+        <v>277</v>
       </c>
       <c r="E146" s="6" t="s">
         <v>7</v>
@@ -5826,19 +5884,17 @@
       <c r="F146" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G146" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="G146" s="6"/>
       <c r="H146" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A147" s="5" t="s">
-        <v>583</v>
+        <v>559</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="C147" s="5" t="s">
         <v>109</v>
@@ -5852,99 +5908,101 @@
       <c r="F147" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G147" s="6"/>
+      <c r="G147" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="H147" s="7" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A148" s="5" t="s">
-        <v>389</v>
+        <v>579</v>
       </c>
       <c r="B148" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C148" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D148" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E148" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F148" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G148" s="6"/>
+      <c r="H148" s="7" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A149" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="B149" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C149" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="D149" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="D148" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="E148" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F148" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G148" s="6" t="s">
-        <v>390</v>
-      </c>
-      <c r="H148" s="7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="149" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A149" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="B149" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C149" s="5" t="s">
+      <c r="E149" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F149" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G149" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="H149" s="7" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A150" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="B150" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C150" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D149" s="5" t="s">
+      <c r="D150" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="E149" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F149" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G149" s="6" t="s">
-        <v>385</v>
-      </c>
-      <c r="H149" s="7" t="s">
+      <c r="E150" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F150" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G150" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="H150" s="7" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="150" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A150" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="B150" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C150" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D150" s="5" t="s">
-        <v>486</v>
-      </c>
-      <c r="E150" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F150" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G150" s="6"/>
-      <c r="H150" s="7" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="151" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A151" s="5" t="s">
-        <v>493</v>
+        <v>448</v>
       </c>
       <c r="B151" s="6" t="s">
-        <v>107</v>
+        <v>6</v>
       </c>
       <c r="C151" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D151" s="5" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="E151" s="6" t="s">
         <v>14</v>
@@ -5954,36 +6012,36 @@
       </c>
       <c r="G151" s="6"/>
       <c r="H151" s="7" t="s">
-        <v>494</v>
+        <v>482</v>
       </c>
     </row>
     <row r="152" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A152" s="5" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="B152" s="6" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="C152" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D152" s="5" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="E152" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F152" s="6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G152" s="6"/>
       <c r="H152" s="7" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A153" s="5" t="s">
-        <v>451</v>
+        <v>485</v>
       </c>
       <c r="B153" s="6" t="s">
         <v>6</v>
@@ -5992,7 +6050,7 @@
         <v>24</v>
       </c>
       <c r="D153" s="5" t="s">
-        <v>25</v>
+        <v>486</v>
       </c>
       <c r="E153" s="6" t="s">
         <v>7</v>
@@ -6000,19 +6058,17 @@
       <c r="F153" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G153" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="G153" s="6"/>
       <c r="H153" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="154" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A154" s="5" t="s">
-        <v>493</v>
+        <v>448</v>
       </c>
       <c r="B154" s="6" t="s">
-        <v>107</v>
+        <v>6</v>
       </c>
       <c r="C154" s="5" t="s">
         <v>24</v>
@@ -6026,73 +6082,73 @@
       <c r="F154" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G154" s="6"/>
+      <c r="G154" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="H154" s="7" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="155" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A155" s="5" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="B155" s="6" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="C155" s="5" t="s">
-        <v>491</v>
+        <v>24</v>
       </c>
       <c r="D155" s="5" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="E155" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F155" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="F155" s="6" t="s">
-        <v>7</v>
       </c>
       <c r="G155" s="6"/>
       <c r="H155" s="7" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="156" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A156" s="5" t="s">
-        <v>331</v>
+        <v>485</v>
       </c>
       <c r="B156" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>209</v>
+        <v>488</v>
       </c>
       <c r="D156" s="5" t="s">
-        <v>329</v>
+        <v>113</v>
       </c>
       <c r="E156" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F156" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G156" s="6" t="s">
-        <v>479</v>
-      </c>
+      <c r="G156" s="6"/>
       <c r="H156" s="7" t="s">
-        <v>330</v>
+        <v>487</v>
       </c>
     </row>
     <row r="157" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A157" s="5" t="s">
-        <v>472</v>
+        <v>328</v>
       </c>
       <c r="B157" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D157" s="5" t="s">
-        <v>300</v>
+        <v>326</v>
       </c>
       <c r="E157" s="6" t="s">
         <v>7</v>
@@ -6100,23 +6156,25 @@
       <c r="F157" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G157" s="6"/>
+      <c r="G157" s="6" t="s">
+        <v>476</v>
+      </c>
       <c r="H157" s="7" t="s">
-        <v>299</v>
+        <v>327</v>
       </c>
     </row>
     <row r="158" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A158" s="5" t="s">
-        <v>463</v>
+        <v>469</v>
       </c>
       <c r="B158" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C158" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D158" s="5" t="s">
-        <v>210</v>
+        <v>297</v>
       </c>
       <c r="E158" s="6" t="s">
         <v>7</v>
@@ -6126,21 +6184,21 @@
       </c>
       <c r="G158" s="6"/>
       <c r="H158" s="7" t="s">
-        <v>208</v>
+        <v>296</v>
       </c>
     </row>
     <row r="159" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A159" s="5" t="s">
-        <v>298</v>
+        <v>460</v>
       </c>
       <c r="B159" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C159" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="D159" s="5" t="s">
         <v>209</v>
-      </c>
-      <c r="D159" s="5" t="s">
-        <v>75</v>
       </c>
       <c r="E159" s="6" t="s">
         <v>7</v>
@@ -6150,45 +6208,45 @@
       </c>
       <c r="G159" s="6"/>
       <c r="H159" s="7" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A160" s="5" t="s">
-        <v>158</v>
+        <v>295</v>
       </c>
       <c r="B160" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C160" s="5" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="D160" s="5" t="s">
-        <v>456</v>
+        <v>75</v>
       </c>
       <c r="E160" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F160" s="6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G160" s="6"/>
       <c r="H160" s="7" t="s">
-        <v>157</v>
+        <v>294</v>
       </c>
     </row>
     <row r="161" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A161" s="5" t="s">
-        <v>458</v>
+        <v>158</v>
       </c>
       <c r="B161" s="6" t="s">
-        <v>107</v>
+        <v>6</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D161" s="5" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="E161" s="6" t="s">
         <v>7</v>
@@ -6198,21 +6256,21 @@
       </c>
       <c r="G161" s="6"/>
       <c r="H161" s="7" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="162" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A162" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="B162" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C162" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="B162" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C162" s="5" t="s">
-        <v>222</v>
-      </c>
       <c r="D162" s="5" t="s">
-        <v>223</v>
+        <v>453</v>
       </c>
       <c r="E162" s="6" t="s">
         <v>7</v>
@@ -6222,71 +6280,69 @@
       </c>
       <c r="G162" s="6"/>
       <c r="H162" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A163" s="5" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="163" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A163" s="5" t="s">
-        <v>531</v>
-      </c>
       <c r="B163" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>174</v>
+        <v>221</v>
       </c>
       <c r="D163" s="5" t="s">
-        <v>75</v>
+        <v>222</v>
       </c>
       <c r="E163" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F163" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="G163" s="6"/>
       <c r="H163" s="7" t="s">
-        <v>530</v>
+        <v>219</v>
       </c>
     </row>
     <row r="164" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A164" s="5" t="s">
-        <v>557</v>
+        <v>595</v>
       </c>
       <c r="B164" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>28</v>
+        <v>596</v>
       </c>
       <c r="D164" s="5" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="E164" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F164" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G164" s="6" t="s">
-        <v>30</v>
-      </c>
+      <c r="G164" s="6"/>
       <c r="H164" s="7" t="s">
-        <v>27</v>
+        <v>594</v>
       </c>
     </row>
     <row r="165" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A165" s="5" t="s">
-        <v>348</v>
+        <v>598</v>
       </c>
       <c r="B165" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C165" s="5" t="s">
-        <v>28</v>
+        <v>596</v>
       </c>
       <c r="D165" s="5" t="s">
-        <v>13</v>
+        <v>599</v>
       </c>
       <c r="E165" s="6" t="s">
         <v>14</v>
@@ -6296,21 +6352,21 @@
       </c>
       <c r="G165" s="6"/>
       <c r="H165" s="7" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="166" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A166" s="5" t="s">
-        <v>350</v>
+        <v>601</v>
       </c>
       <c r="B166" s="6" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>28</v>
+        <v>596</v>
       </c>
       <c r="D166" s="5" t="s">
-        <v>13</v>
+        <v>602</v>
       </c>
       <c r="E166" s="6" t="s">
         <v>14</v>
@@ -6320,84 +6376,84 @@
       </c>
       <c r="G166" s="6"/>
       <c r="H166" s="7" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="167" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A167" s="5" t="s">
-        <v>161</v>
+        <v>604</v>
       </c>
       <c r="B167" s="6" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>28</v>
+        <v>596</v>
       </c>
       <c r="D167" s="5" t="s">
-        <v>456</v>
+        <v>602</v>
       </c>
       <c r="E167" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F167" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G167" s="6"/>
       <c r="H167" s="7" t="s">
-        <v>160</v>
+        <v>603</v>
       </c>
     </row>
     <row r="168" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A168" s="5" t="s">
-        <v>457</v>
+        <v>606</v>
       </c>
       <c r="B168" s="6" t="s">
         <v>107</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>28</v>
+        <v>596</v>
       </c>
       <c r="D168" s="5" t="s">
-        <v>456</v>
+        <v>602</v>
       </c>
       <c r="E168" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F168" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G168" s="6"/>
       <c r="H168" s="7" t="s">
-        <v>162</v>
+        <v>605</v>
       </c>
     </row>
     <row r="169" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A169" s="5" t="s">
-        <v>424</v>
+        <v>528</v>
       </c>
       <c r="B169" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>28</v>
+        <v>174</v>
       </c>
       <c r="D169" s="5" t="s">
-        <v>425</v>
+        <v>75</v>
       </c>
       <c r="E169" s="6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F169" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G169" s="6"/>
       <c r="H169" s="7" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="170" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A170" s="5" t="s">
-        <v>453</v>
+        <v>554</v>
       </c>
       <c r="B170" s="6" t="s">
         <v>6</v>
@@ -6406,7 +6462,7 @@
         <v>28</v>
       </c>
       <c r="D170" s="5" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="E170" s="6" t="s">
         <v>7</v>
@@ -6415,15 +6471,15 @@
         <v>7</v>
       </c>
       <c r="G170" s="6" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H170" s="7" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
     </row>
     <row r="171" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A171" s="5" t="s">
-        <v>218</v>
+        <v>345</v>
       </c>
       <c r="B171" s="6" t="s">
         <v>6</v>
@@ -6432,22 +6488,22 @@
         <v>28</v>
       </c>
       <c r="D171" s="5" t="s">
-        <v>219</v>
+        <v>13</v>
       </c>
       <c r="E171" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F171" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G171" s="6"/>
       <c r="H171" s="7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="172" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A172" s="5" t="s">
-        <v>369</v>
+        <v>347</v>
       </c>
       <c r="B172" s="6" t="s">
         <v>6</v>
@@ -6456,22 +6512,22 @@
         <v>28</v>
       </c>
       <c r="D172" s="5" t="s">
-        <v>459</v>
+        <v>13</v>
       </c>
       <c r="E172" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F172" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G172" s="6"/>
       <c r="H172" s="7" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="173" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A173" s="5" t="s">
-        <v>465</v>
+        <v>161</v>
       </c>
       <c r="B173" s="6" t="s">
         <v>6</v>
@@ -6480,7 +6536,7 @@
         <v>28</v>
       </c>
       <c r="D173" s="5" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="E173" s="6" t="s">
         <v>7</v>
@@ -6490,21 +6546,21 @@
       </c>
       <c r="G173" s="6"/>
       <c r="H173" s="7" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="174" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A174" s="5" t="s">
-        <v>46</v>
+        <v>454</v>
       </c>
       <c r="B174" s="6" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="C174" s="5" t="s">
-        <v>452</v>
+        <v>28</v>
       </c>
       <c r="D174" s="5" t="s">
-        <v>296</v>
+        <v>453</v>
       </c>
       <c r="E174" s="6" t="s">
         <v>7</v>
@@ -6512,25 +6568,23 @@
       <c r="F174" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G174" s="6" t="s">
-        <v>393</v>
-      </c>
+      <c r="G174" s="6"/>
       <c r="H174" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.35">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A175" s="5" t="s">
-        <v>545</v>
+        <v>421</v>
       </c>
       <c r="B175" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C175" s="5" t="s">
-        <v>546</v>
+        <v>28</v>
       </c>
       <c r="D175" s="5" t="s">
-        <v>547</v>
+        <v>422</v>
       </c>
       <c r="E175" s="6" t="s">
         <v>14</v>
@@ -6540,10 +6594,10 @@
       </c>
       <c r="G175" s="6"/>
       <c r="H175" s="7" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="176" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A176" s="5" t="s">
         <v>450</v>
       </c>
@@ -6551,10 +6605,10 @@
         <v>6</v>
       </c>
       <c r="C176" s="5" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D176" s="5" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="E176" s="6" t="s">
         <v>7</v>
@@ -6563,24 +6617,24 @@
         <v>7</v>
       </c>
       <c r="G176" s="6" t="s">
-        <v>433</v>
+        <v>60</v>
       </c>
       <c r="H176" s="7" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
     </row>
     <row r="177" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A177" s="5" t="s">
-        <v>66</v>
+        <v>217</v>
       </c>
       <c r="B177" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C177" s="5" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D177" s="5" t="s">
-        <v>67</v>
+        <v>218</v>
       </c>
       <c r="E177" s="6" t="s">
         <v>7</v>
@@ -6588,25 +6642,23 @@
       <c r="F177" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G177" s="6" t="s">
-        <v>68</v>
-      </c>
+      <c r="G177" s="6"/>
       <c r="H177" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="178" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A178" s="5" t="s">
-        <v>187</v>
+        <v>366</v>
       </c>
       <c r="B178" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C178" s="5" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D178" s="5" t="s">
-        <v>67</v>
+        <v>456</v>
       </c>
       <c r="E178" s="6" t="s">
         <v>7</v>
@@ -6616,21 +6668,21 @@
       </c>
       <c r="G178" s="6"/>
       <c r="H178" s="7" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="179" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A179" s="5" t="s">
-        <v>560</v>
+        <v>462</v>
       </c>
       <c r="B179" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C179" s="5" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D179" s="5" t="s">
-        <v>77</v>
+        <v>456</v>
       </c>
       <c r="E179" s="6" t="s">
         <v>7</v>
@@ -6638,25 +6690,23 @@
       <c r="F179" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G179" s="6" t="s">
-        <v>78</v>
-      </c>
+      <c r="G179" s="6"/>
       <c r="H179" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="180" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A180" s="5" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="B180" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C180" s="5" t="s">
-        <v>10</v>
+        <v>449</v>
       </c>
       <c r="D180" s="5" t="s">
-        <v>77</v>
+        <v>293</v>
       </c>
       <c r="E180" s="6" t="s">
         <v>7</v>
@@ -6665,39 +6715,39 @@
         <v>7</v>
       </c>
       <c r="G180" s="6" t="s">
-        <v>81</v>
+        <v>390</v>
       </c>
       <c r="H180" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="181" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A181" s="5" t="s">
-        <v>310</v>
+        <v>542</v>
       </c>
       <c r="B181" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C181" s="5" t="s">
-        <v>10</v>
+        <v>543</v>
       </c>
       <c r="D181" s="5" t="s">
-        <v>77</v>
+        <v>544</v>
       </c>
       <c r="E181" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F181" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G181" s="6"/>
       <c r="H181" s="7" t="s">
-        <v>309</v>
+        <v>541</v>
       </c>
     </row>
     <row r="182" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A182" s="5" t="s">
-        <v>74</v>
+        <v>447</v>
       </c>
       <c r="B182" s="6" t="s">
         <v>6</v>
@@ -6706,7 +6756,7 @@
         <v>10</v>
       </c>
       <c r="D182" s="5" t="s">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="E182" s="6" t="s">
         <v>7</v>
@@ -6714,14 +6764,16 @@
       <c r="F182" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G182" s="6"/>
+      <c r="G182" s="6" t="s">
+        <v>430</v>
+      </c>
       <c r="H182" s="7" t="s">
-        <v>73</v>
+        <v>9</v>
       </c>
     </row>
     <row r="183" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A183" s="5" t="s">
-        <v>185</v>
+        <v>66</v>
       </c>
       <c r="B183" s="6" t="s">
         <v>6</v>
@@ -6730,7 +6782,7 @@
         <v>10</v>
       </c>
       <c r="D183" s="5" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="E183" s="6" t="s">
         <v>7</v>
@@ -6739,15 +6791,15 @@
         <v>7</v>
       </c>
       <c r="G183" s="6" t="s">
-        <v>460</v>
+        <v>68</v>
       </c>
       <c r="H183" s="7" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="184" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A184" s="5" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B184" s="6" t="s">
         <v>6</v>
@@ -6756,7 +6808,7 @@
         <v>10</v>
       </c>
       <c r="D184" s="5" t="s">
-        <v>183</v>
+        <v>67</v>
       </c>
       <c r="E184" s="6" t="s">
         <v>7</v>
@@ -6766,12 +6818,12 @@
       </c>
       <c r="G184" s="6"/>
       <c r="H184" s="7" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="185" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A185" s="5" t="s">
-        <v>32</v>
+        <v>556</v>
       </c>
       <c r="B185" s="6" t="s">
         <v>6</v>
@@ -6780,7 +6832,7 @@
         <v>10</v>
       </c>
       <c r="D185" s="5" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="E185" s="6" t="s">
         <v>7</v>
@@ -6789,15 +6841,15 @@
         <v>7</v>
       </c>
       <c r="G185" s="6" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="H185" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="186" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A186" s="5" t="s">
-        <v>558</v>
+        <v>80</v>
       </c>
       <c r="B186" s="6" t="s">
         <v>6</v>
@@ -6806,7 +6858,7 @@
         <v>10</v>
       </c>
       <c r="D186" s="5" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="E186" s="6" t="s">
         <v>7</v>
@@ -6815,15 +6867,15 @@
         <v>7</v>
       </c>
       <c r="G186" s="6" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="H186" s="7" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
     </row>
     <row r="187" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A187" s="5" t="s">
-        <v>249</v>
+        <v>307</v>
       </c>
       <c r="B187" s="6" t="s">
         <v>6</v>
@@ -6832,7 +6884,7 @@
         <v>10</v>
       </c>
       <c r="D187" s="5" t="s">
-        <v>250</v>
+        <v>77</v>
       </c>
       <c r="E187" s="6" t="s">
         <v>7</v>
@@ -6842,12 +6894,12 @@
       </c>
       <c r="G187" s="6"/>
       <c r="H187" s="7" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="188" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A188" s="5" t="s">
-        <v>252</v>
+        <v>74</v>
       </c>
       <c r="B188" s="6" t="s">
         <v>6</v>
@@ -6856,7 +6908,7 @@
         <v>10</v>
       </c>
       <c r="D188" s="5" t="s">
-        <v>253</v>
+        <v>75</v>
       </c>
       <c r="E188" s="6" t="s">
         <v>7</v>
@@ -6866,15 +6918,171 @@
       </c>
       <c r="G188" s="6"/>
       <c r="H188" s="7" t="s">
-        <v>251</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A189" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B189" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C189" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D189" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E189" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F189" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G189" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="H189" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A190" s="5" t="s">
+        <v>589</v>
+      </c>
+      <c r="B190" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C190" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D190" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="E190" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F190" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G190" s="6" t="s">
+        <v>607</v>
+      </c>
+      <c r="H190" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A191" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B191" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C191" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D191" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E191" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F191" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G191" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H191" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A192" s="5" t="s">
+        <v>588</v>
+      </c>
+      <c r="B192" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C192" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D192" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E192" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F192" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G192" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H192" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A193" s="5" t="s">
+        <v>590</v>
+      </c>
+      <c r="B193" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C193" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D193" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="E193" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F193" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G193" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="H193" s="7" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A194" s="5" t="s">
+        <v>591</v>
+      </c>
+      <c r="B194" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C194" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D194" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="E194" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F194" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G194" s="6" t="s">
+        <v>609</v>
+      </c>
+      <c r="H194" s="7" t="s">
+        <v>249</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H182" xr:uid="{B9FACE88-1C57-4099-A43D-8DA482706A91}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H196">
-    <sortCondition ref="C8:C196"/>
-    <sortCondition ref="D8:D196"/>
-    <sortCondition ref="H8:H196"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H195">
+    <sortCondition ref="C8:C195"/>
+    <sortCondition ref="D8:D195"/>
+    <sortCondition ref="H8:H195"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated rules acc to last discussions Core v3.0 and #520
</commit_message>
<xml_diff>
--- a/Deliverables/RULES/USDM_CORE_Rules.xlsx
+++ b/Deliverables/RULES/USDM_CORE_Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stack\CL027\Publish\CORE\3.9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FABC3A2-5CDA-4516-8C6A-8FE333E7C6F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA4BC11-6FD8-4546-A434-20EBF7D6AE71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3210" yWindow="-19845" windowWidth="30285" windowHeight="19125" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
+    <workbookView xWindow="38040" yWindow="-10920" windowWidth="29040" windowHeight="15720" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
   </bookViews>
   <sheets>
     <sheet name="Version 3.0 and 3.9 CORE rules" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1632" uniqueCount="758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1639" uniqueCount="760">
   <si>
     <t>Textual statement of rule</t>
   </si>
@@ -2099,9 +2099,6 @@
     <t>DDF00128</t>
   </si>
   <si>
-    <t>A study intervention's product designation must be specified using the product Designation (C207418) DDF codelist.</t>
-  </si>
-  <si>
     <t>DDF00129</t>
   </si>
   <si>
@@ -2249,9 +2246,6 @@
     <t>administrableProduct</t>
   </si>
   <si>
-    <t>In case a medical device includes an embedded product then the sourcing information must be defined at the medical device level not at the embedded product level.</t>
-  </si>
-  <si>
     <t>AdminstrableProduct</t>
   </si>
   <si>
@@ -2309,10 +2303,22 @@
     <t>CHK0255</t>
   </si>
   <si>
-    <t>A product organization role is expected to either apply to at least a medical device or an administrable product.</t>
-  </si>
-  <si>
     <t>ProductOrganizationRole</t>
+  </si>
+  <si>
+    <t>A study intervention's product designation must be specified using the product designation (C207418) DDF codelist.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sourcing must not be defined for an administrable product which is only referenced as an embedded product for a medical device. </t>
+  </si>
+  <si>
+    <t>A product organization role is expected to apply to at least one medical device or administrable product.</t>
+  </si>
+  <si>
+    <t>CHK0256</t>
+  </si>
+  <si>
+    <t>If 'appliesTo' is specified for a product organization role, then the product organization role must only apply to medical devices or administrable products.</t>
   </si>
 </sst>
 </file>
@@ -2744,10 +2750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FACE88-1C57-4099-A43D-8DA482706A91}">
-  <dimension ref="A1:H212"/>
+  <dimension ref="A1:H213"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3207,7 +3213,7 @@
         <v>5</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>534</v>
@@ -3233,7 +3239,7 @@
         <v>5</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>539</v>
@@ -3393,7 +3399,7 @@
     </row>
     <row r="26" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>4</v>
@@ -3402,7 +3408,7 @@
         <v>472</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>12</v>
@@ -3412,7 +3418,7 @@
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="7" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="58" x14ac:dyDescent="0.35">
@@ -3441,7 +3447,7 @@
     </row>
     <row r="28" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>4</v>
@@ -3450,7 +3456,7 @@
         <v>463</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>12</v>
@@ -3460,7 +3466,7 @@
       </c>
       <c r="G28" s="6"/>
       <c r="H28" s="7" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -3489,7 +3495,7 @@
     </row>
     <row r="30" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>4</v>
@@ -3637,16 +3643,16 @@
     </row>
     <row r="36" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
+        <v>756</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>735</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>736</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>737</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>738</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>12</v>
@@ -3656,7 +3662,7 @@
       </c>
       <c r="G36" s="6"/>
       <c r="H36" s="7" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="58" x14ac:dyDescent="0.35">
@@ -3687,7 +3693,7 @@
     </row>
     <row r="38" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>4</v>
@@ -3705,7 +3711,7 @@
         <v>12</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="H38" s="7" t="s">
         <v>279</v>
@@ -3739,7 +3745,7 @@
     </row>
     <row r="40" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>99</v>
@@ -3765,7 +3771,7 @@
     </row>
     <row r="41" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>99</v>
@@ -3939,7 +3945,7 @@
         <v>5</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="H47" s="7" t="s">
         <v>328</v>
@@ -4171,7 +4177,7 @@
         <v>5</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="H56" s="7" t="s">
         <v>541</v>
@@ -4205,7 +4211,7 @@
     </row>
     <row r="58" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>4</v>
@@ -4223,7 +4229,7 @@
         <v>5</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="H58" s="7" t="s">
         <v>310</v>
@@ -4275,7 +4281,7 @@
         <v>12</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="H60" s="7" t="s">
         <v>309</v>
@@ -4375,7 +4381,7 @@
         <v>5</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="H64" s="7" t="s">
         <v>536</v>
@@ -4427,7 +4433,7 @@
         <v>5</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="H66" s="7" t="s">
         <v>503</v>
@@ -4505,7 +4511,7 @@
         <v>5</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="H69" s="7" t="s">
         <v>499</v>
@@ -4557,7 +4563,7 @@
         <v>5</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="H71" s="7" t="s">
         <v>488</v>
@@ -4583,7 +4589,7 @@
         <v>5</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="H72" s="7" t="s">
         <v>526</v>
@@ -4609,7 +4615,7 @@
         <v>5</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="H73" s="7" t="s">
         <v>484</v>
@@ -4669,16 +4675,16 @@
     </row>
     <row r="76" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B76" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>12</v>
@@ -4688,18 +4694,18 @@
       </c>
       <c r="G76" s="6"/>
       <c r="H76" s="7" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A77" s="5" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B77" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>70</v>
@@ -4712,7 +4718,7 @@
       </c>
       <c r="G77" s="6"/>
       <c r="H77" s="7" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -4765,7 +4771,7 @@
     </row>
     <row r="80" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B80" s="6" t="s">
         <v>4</v>
@@ -4774,7 +4780,7 @@
         <v>110</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E80" s="6" t="s">
         <v>12</v>
@@ -4784,7 +4790,7 @@
       </c>
       <c r="G80" s="6"/>
       <c r="H80" s="7" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -4905,7 +4911,7 @@
         <v>5</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="H85" s="7" t="s">
         <v>281</v>
@@ -4931,7 +4937,7 @@
         <v>12</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="H86" s="7" t="s">
         <v>543</v>
@@ -5031,7 +5037,7 @@
         <v>5</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="H90" s="7" t="s">
         <v>497</v>
@@ -5081,7 +5087,7 @@
         <v>12</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="H92" s="7" t="s">
         <v>477</v>
@@ -5089,7 +5095,7 @@
     </row>
     <row r="93" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A93" s="5" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B93" s="6" t="s">
         <v>4</v>
@@ -5115,7 +5121,7 @@
     </row>
     <row r="94" spans="1:8" ht="116" x14ac:dyDescent="0.35">
       <c r="A94" s="5" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="B94" s="6" t="s">
         <v>4</v>
@@ -5133,7 +5139,7 @@
         <v>5</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="H94" s="7" t="s">
         <v>329</v>
@@ -5193,13 +5199,13 @@
     </row>
     <row r="97" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A97" s="5" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="B97" s="6" t="s">
         <v>99</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="D97" s="5" t="s">
         <v>60</v>
@@ -5212,38 +5218,36 @@
       </c>
       <c r="G97" s="6"/>
       <c r="H97" s="7" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A98" s="5" t="s">
-        <v>354</v>
+        <v>759</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>192</v>
+        <v>754</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>248</v>
+        <v>60</v>
       </c>
       <c r="E98" s="6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F98" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G98" s="6" t="s">
-        <v>375</v>
-      </c>
+      <c r="G98" s="6"/>
       <c r="H98" s="7" t="s">
-        <v>247</v>
+        <v>758</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A99" s="5" t="s">
-        <v>381</v>
+        <v>354</v>
       </c>
       <c r="B99" s="6" t="s">
         <v>99</v>
@@ -5252,25 +5256,27 @@
         <v>192</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F99" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G99" s="6"/>
+        <v>5</v>
+      </c>
+      <c r="G99" s="6" t="s">
+        <v>375</v>
+      </c>
       <c r="H99" s="7" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A100" s="5" t="s">
-        <v>460</v>
+        <v>381</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="C100" s="5" t="s">
         <v>192</v>
@@ -5279,106 +5285,104 @@
         <v>263</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F100" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G100" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G100" s="6"/>
+      <c r="H100" s="7" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A101" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="E101" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F101" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G101" s="6" t="s">
         <v>593</v>
       </c>
-      <c r="H100" s="7" t="s">
+      <c r="H101" s="7" t="s">
         <v>459</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A101" s="5" t="s">
-        <v>752</v>
-      </c>
-      <c r="B101" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C101" s="5" t="s">
-        <v>491</v>
-      </c>
-      <c r="D101" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E101" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F101" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G101" s="6" t="s">
-        <v>717</v>
-      </c>
-      <c r="H101" s="7" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
+        <v>750</v>
+      </c>
+      <c r="B102" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>491</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E102" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F102" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G102" s="6" t="s">
+        <v>716</v>
+      </c>
+      <c r="H102" s="7" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A103" s="5" t="s">
         <v>495</v>
       </c>
-      <c r="B102" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C102" s="5" t="s">
+      <c r="B103" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C103" s="5" t="s">
         <v>496</v>
       </c>
-      <c r="D102" s="5" t="s">
+      <c r="D103" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E102" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F102" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G102" s="6"/>
-      <c r="H102" s="7" t="s">
+      <c r="E103" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F103" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G103" s="6"/>
+      <c r="H103" s="7" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A103" s="5" t="s">
+    <row r="104" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A104" s="5" t="s">
         <v>348</v>
       </c>
-      <c r="B103" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C103" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D103" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="E103" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F103" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G103" s="6" t="s">
-        <v>650</v>
-      </c>
-      <c r="H103" s="7" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A104" s="5" t="s">
-        <v>162</v>
-      </c>
       <c r="B104" s="6" t="s">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="C104" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>163</v>
+        <v>181</v>
       </c>
       <c r="E104" s="6" t="s">
         <v>5</v>
@@ -5387,15 +5391,15 @@
         <v>5</v>
       </c>
       <c r="G104" s="6" t="s">
-        <v>642</v>
+        <v>650</v>
       </c>
       <c r="H104" s="7" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A105" s="8" t="s">
-        <v>679</v>
+        <v>162</v>
       </c>
       <c r="B105" s="6" t="s">
         <v>99</v>
@@ -5413,24 +5417,24 @@
         <v>5</v>
       </c>
       <c r="G105" s="6" t="s">
-        <v>680</v>
+        <v>642</v>
       </c>
       <c r="H105" s="7" t="s">
-        <v>266</v>
+        <v>161</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A106" s="5" t="s">
-        <v>168</v>
+        <v>679</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="C106" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="E106" s="6" t="s">
         <v>5</v>
@@ -5439,15 +5443,15 @@
         <v>5</v>
       </c>
       <c r="G106" s="6" t="s">
-        <v>369</v>
+        <v>680</v>
       </c>
       <c r="H106" s="7" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A107" s="5" t="s">
-        <v>349</v>
+        <v>168</v>
       </c>
       <c r="B107" s="6" t="s">
         <v>4</v>
@@ -5465,15 +5469,15 @@
         <v>5</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>651</v>
+        <v>369</v>
       </c>
       <c r="H107" s="7" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A108" s="5" t="s">
-        <v>77</v>
+        <v>349</v>
       </c>
       <c r="B108" s="6" t="s">
         <v>4</v>
@@ -5482,7 +5486,7 @@
         <v>46</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>78</v>
+        <v>169</v>
       </c>
       <c r="E108" s="6" t="s">
         <v>5</v>
@@ -5491,15 +5495,15 @@
         <v>5</v>
       </c>
       <c r="G108" s="6" t="s">
-        <v>79</v>
+        <v>651</v>
       </c>
       <c r="H108" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A109" s="5" t="s">
-        <v>356</v>
+        <v>77</v>
       </c>
       <c r="B109" s="6" t="s">
         <v>4</v>
@@ -5517,15 +5521,15 @@
         <v>5</v>
       </c>
       <c r="G109" s="6" t="s">
-        <v>646</v>
+        <v>79</v>
       </c>
       <c r="H109" s="7" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A110" s="5" t="s">
-        <v>45</v>
+        <v>356</v>
       </c>
       <c r="B110" s="6" t="s">
         <v>4</v>
@@ -5534,7 +5538,7 @@
         <v>46</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="E110" s="6" t="s">
         <v>5</v>
@@ -5543,41 +5547,41 @@
         <v>5</v>
       </c>
       <c r="G110" s="6" t="s">
-        <v>48</v>
+        <v>646</v>
       </c>
       <c r="H110" s="7" t="s">
-        <v>44</v>
+        <v>267</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A111" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B111" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D111" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E111" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F111" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G111" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H111" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A112" s="5" t="s">
         <v>232</v>
-      </c>
-      <c r="B111" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C111" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="D111" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="E111" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F111" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G111" s="6" t="s">
-        <v>365</v>
-      </c>
-      <c r="H111" s="7" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A112" s="5" t="s">
-        <v>347</v>
       </c>
       <c r="B112" s="6" t="s">
         <v>4</v>
@@ -5586,51 +5590,53 @@
         <v>179</v>
       </c>
       <c r="D112" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="E112" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F112" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G112" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="H112" s="7" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A113" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C113" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D113" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="E112" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F112" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G112" s="6" t="s">
+      <c r="E113" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F113" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G113" s="6" t="s">
         <v>649</v>
       </c>
-      <c r="H112" s="7" t="s">
+      <c r="H113" s="7" t="s">
         <v>178</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A113" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="B113" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C113" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="D113" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="E113" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F113" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G113" s="6"/>
-      <c r="H113" s="7" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="114" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A114" s="5" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="C114" s="5" t="s">
         <v>313</v>
@@ -5639,21 +5645,19 @@
         <v>233</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F114" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G114" s="6" t="s">
-        <v>590</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G114" s="6"/>
       <c r="H114" s="7" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
     </row>
     <row r="115" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A115" s="5" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="B115" s="6" t="s">
         <v>99</v>
@@ -5662,7 +5666,7 @@
         <v>313</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>169</v>
+        <v>233</v>
       </c>
       <c r="E115" s="6" t="s">
         <v>5</v>
@@ -5671,15 +5675,15 @@
         <v>12</v>
       </c>
       <c r="G115" s="6" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="H115" s="7" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
     </row>
     <row r="116" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A116" s="5" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="B116" s="6" t="s">
         <v>99</v>
@@ -5688,50 +5692,50 @@
         <v>313</v>
       </c>
       <c r="D116" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E116" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F116" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G116" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="H116" s="7" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A117" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="B117" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C117" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="D117" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E116" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F116" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G116" s="6" t="s">
+      <c r="E117" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F117" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G117" s="6" t="s">
         <v>588</v>
       </c>
-      <c r="H116" s="7" t="s">
+      <c r="H117" s="7" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A117" s="5" t="s">
-        <v>748</v>
-      </c>
-      <c r="B117" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C117" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D117" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="E117" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F117" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G117" s="6" t="s">
-        <v>652</v>
-      </c>
-      <c r="H117" s="7" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A118" s="5" t="s">
-        <v>518</v>
+        <v>746</v>
       </c>
       <c r="B118" s="6" t="s">
         <v>4</v>
@@ -5740,7 +5744,7 @@
         <v>65</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>66</v>
+        <v>184</v>
       </c>
       <c r="E118" s="6" t="s">
         <v>5</v>
@@ -5749,48 +5753,50 @@
         <v>5</v>
       </c>
       <c r="G118" s="6" t="s">
-        <v>67</v>
+        <v>652</v>
       </c>
       <c r="H118" s="7" t="s">
-        <v>64</v>
+        <v>183</v>
       </c>
     </row>
     <row r="119" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A119" s="5" t="s">
+        <v>518</v>
+      </c>
+      <c r="B119" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C119" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D119" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E119" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F119" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G119" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H119" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A120" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="B119" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C119" s="5" t="s">
+      <c r="B120" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C120" s="5" t="s">
         <v>512</v>
       </c>
-      <c r="D119" s="5" t="s">
+      <c r="D120" s="5" t="s">
         <v>513</v>
-      </c>
-      <c r="E119" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F119" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G119" s="6"/>
-      <c r="H119" s="7" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A120" s="5" t="s">
-        <v>598</v>
-      </c>
-      <c r="B120" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C120" s="5" t="s">
-        <v>599</v>
-      </c>
-      <c r="D120" s="5" t="s">
-        <v>70</v>
       </c>
       <c r="E120" s="6" t="s">
         <v>12</v>
@@ -5800,38 +5806,36 @@
       </c>
       <c r="G120" s="6"/>
       <c r="H120" s="7" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A121" s="5" t="s">
+        <v>598</v>
+      </c>
+      <c r="B121" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C121" s="5" t="s">
+        <v>599</v>
+      </c>
+      <c r="D121" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E121" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F121" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G121" s="6"/>
+      <c r="H121" s="7" t="s">
         <v>597</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A121" s="5" t="s">
-        <v>487</v>
-      </c>
-      <c r="B121" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C121" s="5" t="s">
-        <v>340</v>
-      </c>
-      <c r="D121" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="E121" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F121" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G121" s="6" t="s">
-        <v>715</v>
-      </c>
-      <c r="H121" s="7" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A122" s="5" t="s">
-        <v>339</v>
+        <v>487</v>
       </c>
       <c r="B122" s="6" t="s">
         <v>4</v>
@@ -5840,50 +5844,50 @@
         <v>340</v>
       </c>
       <c r="D122" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="E122" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F122" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G122" s="6" t="s">
+        <v>714</v>
+      </c>
+      <c r="H122" s="7" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A123" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="B123" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C123" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="D123" s="5" t="s">
         <v>341</v>
       </c>
-      <c r="E122" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F122" s="6" t="s">
+      <c r="E123" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F123" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G122" s="6" t="s">
+      <c r="G123" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="H122" s="7" t="s">
+      <c r="H123" s="7" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A123" s="5" t="s">
-        <v>753</v>
-      </c>
-      <c r="B123" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C123" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="D123" s="5" t="s">
-        <v>502</v>
-      </c>
-      <c r="E123" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F123" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G123" s="6" t="s">
-        <v>721</v>
-      </c>
-      <c r="H123" s="7" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A124" s="5" t="s">
-        <v>411</v>
+        <v>751</v>
       </c>
       <c r="B124" s="6" t="s">
         <v>4</v>
@@ -5892,7 +5896,7 @@
         <v>157</v>
       </c>
       <c r="D124" s="5" t="s">
-        <v>158</v>
+        <v>502</v>
       </c>
       <c r="E124" s="6" t="s">
         <v>5</v>
@@ -5901,15 +5905,15 @@
         <v>5</v>
       </c>
       <c r="G124" s="6" t="s">
-        <v>412</v>
+        <v>720</v>
       </c>
       <c r="H124" s="7" t="s">
-        <v>156</v>
+        <v>501</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A125" s="5" t="s">
-        <v>708</v>
+        <v>411</v>
       </c>
       <c r="B125" s="6" t="s">
         <v>4</v>
@@ -5927,41 +5931,41 @@
         <v>5</v>
       </c>
       <c r="G125" s="6" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="H125" s="7" t="s">
-        <v>415</v>
+        <v>156</v>
       </c>
     </row>
     <row r="126" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A126" s="5" t="s">
+        <v>707</v>
+      </c>
+      <c r="B126" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C126" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D126" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="E126" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F126" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G126" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="H126" s="7" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A127" s="5" t="s">
         <v>530</v>
-      </c>
-      <c r="B126" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C126" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D126" s="5" t="s">
-        <v>531</v>
-      </c>
-      <c r="E126" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F126" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G126" s="6" t="s">
-        <v>594</v>
-      </c>
-      <c r="H126" s="7" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A127" s="5" t="s">
-        <v>618</v>
       </c>
       <c r="B127" s="6" t="s">
         <v>4</v>
@@ -5970,7 +5974,7 @@
         <v>87</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>269</v>
+        <v>531</v>
       </c>
       <c r="E127" s="6" t="s">
         <v>5</v>
@@ -5979,15 +5983,15 @@
         <v>5</v>
       </c>
       <c r="G127" s="6" t="s">
-        <v>583</v>
+        <v>594</v>
       </c>
       <c r="H127" s="7" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" s="5" t="s">
-        <v>357</v>
+        <v>618</v>
       </c>
       <c r="B128" s="6" t="s">
         <v>4</v>
@@ -6005,15 +6009,15 @@
         <v>5</v>
       </c>
       <c r="G128" s="6" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="H128" s="7" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A129" s="5" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="B129" s="6" t="s">
         <v>4</v>
@@ -6022,7 +6026,7 @@
         <v>87</v>
       </c>
       <c r="D129" s="5" t="s">
-        <v>88</v>
+        <v>269</v>
       </c>
       <c r="E129" s="6" t="s">
         <v>5</v>
@@ -6031,15 +6035,15 @@
         <v>5</v>
       </c>
       <c r="G129" s="6" t="s">
-        <v>89</v>
+        <v>584</v>
       </c>
       <c r="H129" s="7" t="s">
-        <v>86</v>
+        <v>271</v>
       </c>
     </row>
     <row r="130" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A130" s="5" t="s">
-        <v>377</v>
+        <v>362</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>4</v>
@@ -6057,15 +6061,15 @@
         <v>5</v>
       </c>
       <c r="G130" s="6" t="s">
-        <v>409</v>
+        <v>89</v>
       </c>
       <c r="H130" s="7" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A131" s="5" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="B131" s="6" t="s">
         <v>4</v>
@@ -6080,18 +6084,18 @@
         <v>5</v>
       </c>
       <c r="F131" s="6" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G131" s="6" t="s">
-        <v>591</v>
+        <v>409</v>
       </c>
       <c r="H131" s="7" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A132" s="5" t="s">
-        <v>533</v>
+        <v>383</v>
       </c>
       <c r="B132" s="6" t="s">
         <v>4</v>
@@ -6100,57 +6104,59 @@
         <v>87</v>
       </c>
       <c r="D132" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E132" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F132" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G132" s="6" t="s">
+        <v>591</v>
+      </c>
+      <c r="H132" s="7" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A133" s="5" t="s">
+        <v>533</v>
+      </c>
+      <c r="B133" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C133" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D133" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="E132" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F132" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G132" s="6" t="s">
+      <c r="E133" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F133" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G133" s="6" t="s">
         <v>595</v>
       </c>
-      <c r="H132" s="7" t="s">
+      <c r="H133" s="7" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A133" s="5" t="s">
+    <row r="134" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A134" s="5" t="s">
         <v>447</v>
       </c>
-      <c r="B133" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C133" s="5" t="s">
+      <c r="B134" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C134" s="5" t="s">
         <v>396</v>
       </c>
-      <c r="D133" s="5" t="s">
+      <c r="D134" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="E133" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F133" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G133" s="6"/>
-      <c r="H133" s="7" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A134" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="B134" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C134" s="5" t="s">
-        <v>404</v>
-      </c>
-      <c r="D134" s="5" t="s">
-        <v>428</v>
       </c>
       <c r="E134" s="6" t="s">
         <v>12</v>
@@ -6160,15 +6166,15 @@
       </c>
       <c r="G134" s="6"/>
       <c r="H134" s="7" t="s">
-        <v>482</v>
+        <v>397</v>
       </c>
     </row>
     <row r="135" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A135" s="5" t="s">
-        <v>430</v>
+        <v>149</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="C135" s="5" t="s">
         <v>404</v>
@@ -6184,21 +6190,21 @@
       </c>
       <c r="G135" s="6"/>
       <c r="H135" s="7" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="136" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A136" s="5" t="s">
-        <v>448</v>
+        <v>430</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="C136" s="5" t="s">
         <v>404</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>405</v>
+        <v>428</v>
       </c>
       <c r="E136" s="6" t="s">
         <v>12</v>
@@ -6208,38 +6214,36 @@
       </c>
       <c r="G136" s="6"/>
       <c r="H136" s="7" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A137" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="B137" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C137" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="D137" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="E137" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F137" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G137" s="6"/>
+      <c r="H137" s="7" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="137" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A137" s="5" t="s">
+    <row r="138" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A138" s="5" t="s">
         <v>439</v>
-      </c>
-      <c r="B137" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C137" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="D137" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E137" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F137" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G137" s="6" t="s">
-        <v>673</v>
-      </c>
-      <c r="H137" s="7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A138" s="5" t="s">
-        <v>674</v>
       </c>
       <c r="B138" s="6" t="s">
         <v>4</v>
@@ -6248,7 +6252,7 @@
         <v>211</v>
       </c>
       <c r="D138" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E138" s="6" t="s">
         <v>5</v>
@@ -6257,15 +6261,15 @@
         <v>5</v>
       </c>
       <c r="G138" s="6" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="H138" s="7" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A139" s="5" t="s">
-        <v>295</v>
+        <v>674</v>
       </c>
       <c r="B139" s="6" t="s">
         <v>4</v>
@@ -6283,74 +6287,74 @@
         <v>5</v>
       </c>
       <c r="G139" s="6" t="s">
-        <v>695</v>
+        <v>675</v>
       </c>
       <c r="H139" s="7" t="s">
-        <v>294</v>
+        <v>219</v>
       </c>
     </row>
     <row r="140" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A140" s="5" t="s">
-        <v>596</v>
+        <v>295</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="C140" s="5" t="s">
         <v>211</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>399</v>
+        <v>220</v>
       </c>
       <c r="E140" s="6" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F140" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G140" s="6"/>
+      <c r="G140" s="6" t="s">
+        <v>694</v>
+      </c>
       <c r="H140" s="7" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A141" s="5" t="s">
-        <v>438</v>
+        <v>596</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="C141" s="5" t="s">
         <v>211</v>
       </c>
       <c r="D141" s="5" t="s">
-        <v>216</v>
+        <v>399</v>
       </c>
       <c r="E141" s="6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F141" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G141" s="6" t="s">
-        <v>672</v>
-      </c>
+      <c r="G141" s="6"/>
       <c r="H141" s="7" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A142" s="5" t="s">
-        <v>625</v>
+        <v>438</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="C142" s="5" t="s">
         <v>211</v>
       </c>
       <c r="D142" s="5" t="s">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="E142" s="6" t="s">
         <v>5</v>
@@ -6359,24 +6363,24 @@
         <v>5</v>
       </c>
       <c r="G142" s="6" t="s">
-        <v>626</v>
+        <v>672</v>
       </c>
       <c r="H142" s="7" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A143" s="5" t="s">
-        <v>299</v>
+        <v>625</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="C143" s="5" t="s">
         <v>211</v>
       </c>
       <c r="D143" s="5" t="s">
-        <v>300</v>
+        <v>187</v>
       </c>
       <c r="E143" s="6" t="s">
         <v>5</v>
@@ -6385,15 +6389,15 @@
         <v>5</v>
       </c>
       <c r="G143" s="6" t="s">
-        <v>442</v>
+        <v>626</v>
       </c>
       <c r="H143" s="7" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A144" s="5" t="s">
-        <v>436</v>
+        <v>299</v>
       </c>
       <c r="B144" s="6" t="s">
         <v>4</v>
@@ -6402,7 +6406,7 @@
         <v>211</v>
       </c>
       <c r="D144" s="5" t="s">
-        <v>212</v>
+        <v>300</v>
       </c>
       <c r="E144" s="6" t="s">
         <v>5</v>
@@ -6411,15 +6415,15 @@
         <v>5</v>
       </c>
       <c r="G144" s="6" t="s">
-        <v>670</v>
+        <v>442</v>
       </c>
       <c r="H144" s="7" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A145" s="5" t="s">
-        <v>302</v>
+        <v>436</v>
       </c>
       <c r="B145" s="6" t="s">
         <v>4</v>
@@ -6437,15 +6441,15 @@
         <v>5</v>
       </c>
       <c r="G145" s="6" t="s">
-        <v>443</v>
+        <v>670</v>
       </c>
       <c r="H145" s="7" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A146" s="5" t="s">
-        <v>437</v>
+        <v>302</v>
       </c>
       <c r="B146" s="6" t="s">
         <v>4</v>
@@ -6454,7 +6458,7 @@
         <v>211</v>
       </c>
       <c r="D146" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E146" s="6" t="s">
         <v>5</v>
@@ -6463,15 +6467,15 @@
         <v>5</v>
       </c>
       <c r="G146" s="6" t="s">
-        <v>671</v>
+        <v>443</v>
       </c>
       <c r="H146" s="7" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A147" s="5" t="s">
-        <v>297</v>
+        <v>437</v>
       </c>
       <c r="B147" s="6" t="s">
         <v>4</v>
@@ -6489,39 +6493,41 @@
         <v>5</v>
       </c>
       <c r="G147" s="6" t="s">
+        <v>671</v>
+      </c>
+      <c r="H147" s="7" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A148" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="B148" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C148" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D148" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="E148" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F148" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G148" s="6" t="s">
         <v>441</v>
       </c>
-      <c r="H147" s="7" t="s">
+      <c r="H148" s="7" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="148" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A148" s="5" t="s">
+    <row r="149" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A149" s="5" t="s">
         <v>337</v>
-      </c>
-      <c r="B148" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C148" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D148" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E148" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F148" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G148" s="6"/>
-      <c r="H148" s="7" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="149" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A149" s="5" t="s">
-        <v>746</v>
       </c>
       <c r="B149" s="6" t="s">
         <v>4</v>
@@ -6530,24 +6536,22 @@
         <v>10</v>
       </c>
       <c r="D149" s="5" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="E149" s="6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F149" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G149" s="6" t="s">
-        <v>640</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="G149" s="6"/>
       <c r="H149" s="7" t="s">
-        <v>40</v>
+        <v>336</v>
       </c>
     </row>
     <row r="150" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A150" s="5" t="s">
-        <v>657</v>
+        <v>744</v>
       </c>
       <c r="B150" s="6" t="s">
         <v>4</v>
@@ -6565,15 +6569,15 @@
         <v>5</v>
       </c>
       <c r="G150" s="6" t="s">
-        <v>658</v>
+        <v>640</v>
       </c>
       <c r="H150" s="7" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="151" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A151" s="5" t="s">
-        <v>289</v>
+        <v>657</v>
       </c>
       <c r="B151" s="6" t="s">
         <v>4</v>
@@ -6582,7 +6586,7 @@
         <v>10</v>
       </c>
       <c r="D151" s="5" t="s">
-        <v>290</v>
+        <v>41</v>
       </c>
       <c r="E151" s="6" t="s">
         <v>5</v>
@@ -6591,15 +6595,15 @@
         <v>5</v>
       </c>
       <c r="G151" s="6" t="s">
-        <v>693</v>
+        <v>658</v>
       </c>
       <c r="H151" s="7" t="s">
-        <v>288</v>
+        <v>195</v>
       </c>
     </row>
     <row r="152" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A152" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B152" s="6" t="s">
         <v>4</v>
@@ -6608,7 +6612,7 @@
         <v>10</v>
       </c>
       <c r="D152" s="5" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E152" s="6" t="s">
         <v>5</v>
@@ -6617,15 +6621,15 @@
         <v>5</v>
       </c>
       <c r="G152" s="6" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="H152" s="7" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A153" s="5" t="s">
-        <v>351</v>
+        <v>292</v>
       </c>
       <c r="B153" s="6" t="s">
         <v>4</v>
@@ -6634,7 +6638,7 @@
         <v>10</v>
       </c>
       <c r="D153" s="5" t="s">
-        <v>434</v>
+        <v>293</v>
       </c>
       <c r="E153" s="6" t="s">
         <v>5</v>
@@ -6643,15 +6647,15 @@
         <v>5</v>
       </c>
       <c r="G153" s="6" t="s">
-        <v>382</v>
+        <v>693</v>
       </c>
       <c r="H153" s="7" t="s">
-        <v>191</v>
+        <v>291</v>
       </c>
     </row>
     <row r="154" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A154" s="5" t="s">
-        <v>747</v>
+        <v>351</v>
       </c>
       <c r="B154" s="6" t="s">
         <v>4</v>
@@ -6660,7 +6664,7 @@
         <v>10</v>
       </c>
       <c r="D154" s="5" t="s">
-        <v>95</v>
+        <v>434</v>
       </c>
       <c r="E154" s="6" t="s">
         <v>5</v>
@@ -6669,15 +6673,15 @@
         <v>5</v>
       </c>
       <c r="G154" s="6" t="s">
-        <v>641</v>
+        <v>382</v>
       </c>
       <c r="H154" s="7" t="s">
-        <v>94</v>
+        <v>191</v>
       </c>
     </row>
     <row r="155" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A155" s="5" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="B155" s="6" t="s">
         <v>4</v>
@@ -6695,15 +6699,15 @@
         <v>5</v>
       </c>
       <c r="G155" s="6" t="s">
-        <v>713</v>
+        <v>641</v>
       </c>
       <c r="H155" s="7" t="s">
-        <v>481</v>
+        <v>94</v>
       </c>
     </row>
     <row r="156" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A156" s="5" t="s">
-        <v>552</v>
+        <v>742</v>
       </c>
       <c r="B156" s="6" t="s">
         <v>4</v>
@@ -6715,80 +6719,80 @@
         <v>95</v>
       </c>
       <c r="E156" s="6" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F156" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G156" s="6"/>
+      <c r="G156" s="6" t="s">
+        <v>712</v>
+      </c>
       <c r="H156" s="7" t="s">
-        <v>551</v>
+        <v>481</v>
       </c>
     </row>
     <row r="157" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A157" s="5" t="s">
-        <v>350</v>
+        <v>552</v>
       </c>
       <c r="B157" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>186</v>
+        <v>10</v>
       </c>
       <c r="D157" s="5" t="s">
-        <v>187</v>
+        <v>95</v>
       </c>
       <c r="E157" s="6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F157" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G157" s="6" t="s">
-        <v>653</v>
-      </c>
+      <c r="G157" s="6"/>
       <c r="H157" s="7" t="s">
-        <v>185</v>
+        <v>551</v>
       </c>
     </row>
     <row r="158" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A158" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="B158" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C158" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D158" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E158" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F158" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G158" s="6" t="s">
+        <v>653</v>
+      </c>
+      <c r="H158" s="7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A159" s="5" t="s">
         <v>355</v>
-      </c>
-      <c r="B158" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C158" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="D158" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="E158" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F158" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G158" s="6" t="s">
-        <v>654</v>
-      </c>
-      <c r="H158" s="7" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="159" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A159" s="5" t="s">
-        <v>522</v>
       </c>
       <c r="B159" s="6" t="s">
         <v>99</v>
       </c>
       <c r="C159" s="5" t="s">
-        <v>101</v>
+        <v>260</v>
       </c>
       <c r="D159" s="5" t="s">
-        <v>93</v>
+        <v>261</v>
       </c>
       <c r="E159" s="6" t="s">
         <v>5</v>
@@ -6797,18 +6801,18 @@
         <v>5</v>
       </c>
       <c r="G159" s="6" t="s">
-        <v>622</v>
+        <v>654</v>
       </c>
       <c r="H159" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A160" s="5" t="s">
-        <v>727</v>
+        <v>522</v>
       </c>
       <c r="B160" s="6" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="C160" s="5" t="s">
         <v>101</v>
@@ -6823,94 +6827,96 @@
         <v>5</v>
       </c>
       <c r="G160" s="6" t="s">
-        <v>728</v>
+        <v>622</v>
       </c>
       <c r="H160" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A161" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="B161" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C161" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D161" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E161" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F161" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G161" s="6" t="s">
+        <v>727</v>
+      </c>
+      <c r="H161" s="7" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="161" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A161" s="5" t="s">
+    <row r="162" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A162" s="5" t="s">
         <v>363</v>
       </c>
-      <c r="B161" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C161" s="5" t="s">
+      <c r="B162" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C162" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="D161" s="5" t="s">
+      <c r="D162" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="E161" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F161" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G161" s="6" t="s">
+      <c r="E162" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F162" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G162" s="6" t="s">
         <v>364</v>
       </c>
-      <c r="H161" s="7" t="s">
+      <c r="H162" s="7" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="162" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A162" s="5" t="s">
+    <row r="163" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A163" s="5" t="s">
         <v>359</v>
       </c>
-      <c r="B162" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C162" s="5" t="s">
+      <c r="B163" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C163" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D162" s="5" t="s">
+      <c r="D163" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="E162" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F162" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G162" s="6" t="s">
+      <c r="E163" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F163" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G163" s="6" t="s">
         <v>360</v>
       </c>
-      <c r="H162" s="7" t="s">
+      <c r="H163" s="7" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="163" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A163" s="5" t="s">
+    <row r="164" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A164" s="5" t="s">
         <v>592</v>
       </c>
-      <c r="B163" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C163" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D163" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="E163" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F163" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G163" s="6"/>
-      <c r="H163" s="7" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="164" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A164" s="5" t="s">
-        <v>457</v>
-      </c>
       <c r="B164" s="6" t="s">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="C164" s="5" t="s">
         <v>22</v>
@@ -6926,38 +6932,36 @@
       </c>
       <c r="G164" s="6"/>
       <c r="H164" s="7" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
     </row>
     <row r="165" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A165" s="5" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="B165" s="6" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="C165" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D165" s="5" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="E165" s="6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F165" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G165" s="6" t="s">
-        <v>709</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G165" s="6"/>
       <c r="H165" s="7" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="166" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A166" s="5" t="s">
-        <v>745</v>
+        <v>452</v>
       </c>
       <c r="B166" s="6" t="s">
         <v>4</v>
@@ -6966,7 +6970,7 @@
         <v>22</v>
       </c>
       <c r="D166" s="5" t="s">
-        <v>23</v>
+        <v>453</v>
       </c>
       <c r="E166" s="6" t="s">
         <v>5</v>
@@ -6975,18 +6979,18 @@
         <v>12</v>
       </c>
       <c r="G166" s="6" t="s">
-        <v>24</v>
+        <v>708</v>
       </c>
       <c r="H166" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="167" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A167" s="5" t="s">
-        <v>710</v>
+        <v>743</v>
       </c>
       <c r="B167" s="6" t="s">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="C167" s="5" t="s">
         <v>22</v>
@@ -7001,65 +7005,65 @@
         <v>12</v>
       </c>
       <c r="G167" s="6" t="s">
-        <v>711</v>
+        <v>24</v>
       </c>
       <c r="H167" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A168" s="5" t="s">
+        <v>709</v>
+      </c>
+      <c r="B168" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C168" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D168" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E168" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F168" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G168" s="6" t="s">
+        <v>710</v>
+      </c>
+      <c r="H168" s="7" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A168" s="5" t="s">
+    <row r="169" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A169" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="B168" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C168" s="5" t="s">
+      <c r="B169" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C169" s="5" t="s">
         <v>455</v>
       </c>
-      <c r="D168" s="5" t="s">
+      <c r="D169" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E168" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F168" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G168" s="6"/>
-      <c r="H168" s="7" t="s">
+      <c r="E169" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F169" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G169" s="6"/>
+      <c r="H169" s="7" t="s">
         <v>454</v>
-      </c>
-    </row>
-    <row r="169" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A169" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="B169" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C169" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="D169" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="E169" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F169" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G169" s="6" t="s">
-        <v>445</v>
-      </c>
-      <c r="H169" s="7" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="170" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A170" s="5" t="s">
-        <v>686</v>
+        <v>308</v>
       </c>
       <c r="B170" s="6" t="s">
         <v>4</v>
@@ -7068,24 +7072,24 @@
         <v>197</v>
       </c>
       <c r="D170" s="5" t="s">
-        <v>278</v>
+        <v>306</v>
       </c>
       <c r="E170" s="6" t="s">
         <v>5</v>
       </c>
       <c r="F170" s="6" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G170" s="6" t="s">
-        <v>687</v>
+        <v>445</v>
       </c>
       <c r="H170" s="7" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="171" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A171" s="5" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="B171" s="6" t="s">
         <v>4</v>
@@ -7097,19 +7101,21 @@
         <v>278</v>
       </c>
       <c r="E171" s="6" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F171" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G171" s="6"/>
+        <v>12</v>
+      </c>
+      <c r="G171" s="6" t="s">
+        <v>686</v>
+      </c>
       <c r="H171" s="7" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="172" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A172" s="5" t="s">
-        <v>659</v>
+        <v>752</v>
       </c>
       <c r="B172" s="6" t="s">
         <v>4</v>
@@ -7118,24 +7124,22 @@
         <v>197</v>
       </c>
       <c r="D172" s="5" t="s">
-        <v>198</v>
+        <v>278</v>
       </c>
       <c r="E172" s="6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F172" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G172" s="6" t="s">
-        <v>660</v>
-      </c>
+      <c r="G172" s="6"/>
       <c r="H172" s="7" t="s">
-        <v>196</v>
+        <v>706</v>
       </c>
     </row>
     <row r="173" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A173" s="5" t="s">
-        <v>684</v>
+        <v>659</v>
       </c>
       <c r="B173" s="6" t="s">
         <v>4</v>
@@ -7144,53 +7148,53 @@
         <v>197</v>
       </c>
       <c r="D173" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="E173" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F173" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G173" s="6" t="s">
+        <v>660</v>
+      </c>
+      <c r="H173" s="7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A174" s="5" t="s">
+        <v>684</v>
+      </c>
+      <c r="B174" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C174" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D174" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E173" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F173" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G173" s="6" t="s">
+      <c r="E174" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F174" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G174" s="6" t="s">
         <v>685</v>
       </c>
-      <c r="H173" s="7" t="s">
+      <c r="H174" s="7" t="s">
         <v>276</v>
-      </c>
-    </row>
-    <row r="174" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A174" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="B174" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C174" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="D174" s="5" t="s">
-        <v>428</v>
-      </c>
-      <c r="E174" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F174" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G174" s="6" t="s">
-        <v>635</v>
-      </c>
-      <c r="H174" s="7" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="175" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A175" s="5" t="s">
-        <v>430</v>
+        <v>149</v>
       </c>
       <c r="B175" s="6" t="s">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="C175" s="5" t="s">
         <v>208</v>
@@ -7205,65 +7209,67 @@
         <v>12</v>
       </c>
       <c r="G175" s="6" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="H175" s="7" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="176" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A176" s="5" t="s">
-        <v>668</v>
+        <v>430</v>
       </c>
       <c r="B176" s="6" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="C176" s="5" t="s">
         <v>208</v>
       </c>
       <c r="D176" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="E176" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F176" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G176" s="6" t="s">
+        <v>638</v>
+      </c>
+      <c r="H176" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A177" s="5" t="s">
+        <v>668</v>
+      </c>
+      <c r="B177" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C177" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="D177" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E176" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F176" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G176" s="6" t="s">
+      <c r="E177" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F177" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G177" s="6" t="s">
         <v>669</v>
       </c>
-      <c r="H176" s="7" t="s">
+      <c r="H177" s="7" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="177" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A177" s="5" t="s">
+    <row r="178" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A178" s="5" t="s">
         <v>554</v>
-      </c>
-      <c r="B177" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C177" s="5" t="s">
-        <v>555</v>
-      </c>
-      <c r="D177" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E177" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F177" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G177" s="6"/>
-      <c r="H177" s="7" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A178" s="5" t="s">
-        <v>608</v>
       </c>
       <c r="B178" s="6" t="s">
         <v>4</v>
@@ -7282,12 +7288,12 @@
       </c>
       <c r="G178" s="6"/>
       <c r="H178" s="7" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="179" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A179" s="5" t="s">
-        <v>557</v>
+        <v>608</v>
       </c>
       <c r="B179" s="6" t="s">
         <v>4</v>
@@ -7296,7 +7302,7 @@
         <v>555</v>
       </c>
       <c r="D179" s="5" t="s">
-        <v>558</v>
+        <v>60</v>
       </c>
       <c r="E179" s="6" t="s">
         <v>12</v>
@@ -7306,12 +7312,12 @@
       </c>
       <c r="G179" s="6"/>
       <c r="H179" s="7" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.35">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A180" s="5" t="s">
-        <v>603</v>
+        <v>557</v>
       </c>
       <c r="B180" s="6" t="s">
         <v>4</v>
@@ -7320,7 +7326,7 @@
         <v>555</v>
       </c>
       <c r="D180" s="5" t="s">
-        <v>251</v>
+        <v>558</v>
       </c>
       <c r="E180" s="6" t="s">
         <v>12</v>
@@ -7330,21 +7336,21 @@
       </c>
       <c r="G180" s="6"/>
       <c r="H180" s="7" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="181" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A181" s="5" t="s">
-        <v>560</v>
+        <v>603</v>
       </c>
       <c r="B181" s="6" t="s">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="C181" s="5" t="s">
         <v>555</v>
       </c>
       <c r="D181" s="5" t="s">
-        <v>561</v>
+        <v>251</v>
       </c>
       <c r="E181" s="6" t="s">
         <v>12</v>
@@ -7354,12 +7360,12 @@
       </c>
       <c r="G181" s="6"/>
       <c r="H181" s="7" t="s">
-        <v>559</v>
+        <v>602</v>
       </c>
     </row>
     <row r="182" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A182" s="5" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="B182" s="6" t="s">
         <v>99</v>
@@ -7378,12 +7384,12 @@
       </c>
       <c r="G182" s="6"/>
       <c r="H182" s="7" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="183" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A183" s="5" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B183" s="6" t="s">
         <v>99</v>
@@ -7402,21 +7408,21 @@
       </c>
       <c r="G183" s="6"/>
       <c r="H183" s="7" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.35">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A184" s="5" t="s">
-        <v>605</v>
+        <v>565</v>
       </c>
       <c r="B184" s="6" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="C184" s="5" t="s">
         <v>555</v>
       </c>
       <c r="D184" s="5" t="s">
-        <v>606</v>
+        <v>561</v>
       </c>
       <c r="E184" s="6" t="s">
         <v>12</v>
@@ -7426,47 +7432,45 @@
       </c>
       <c r="G184" s="6"/>
       <c r="H184" s="7" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A185" s="5" t="s">
+        <v>605</v>
+      </c>
+      <c r="B185" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C185" s="5" t="s">
+        <v>555</v>
+      </c>
+      <c r="D185" s="5" t="s">
+        <v>606</v>
+      </c>
+      <c r="E185" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F185" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G185" s="6"/>
+      <c r="H185" s="7" t="s">
         <v>604</v>
-      </c>
-    </row>
-    <row r="185" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A185" s="5" t="s">
-        <v>493</v>
-      </c>
-      <c r="B185" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C185" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="D185" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E185" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F185" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G185" s="6" t="s">
-        <v>718</v>
-      </c>
-      <c r="H185" s="7" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="186" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A186" s="5" t="s">
-        <v>517</v>
+        <v>493</v>
       </c>
       <c r="B186" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C186" s="5" t="s">
-        <v>26</v>
+        <v>165</v>
       </c>
       <c r="D186" s="5" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="E186" s="6" t="s">
         <v>5</v>
@@ -7475,15 +7479,15 @@
         <v>5</v>
       </c>
       <c r="G186" s="6" t="s">
-        <v>28</v>
+        <v>717</v>
       </c>
       <c r="H186" s="7" t="s">
-        <v>25</v>
+        <v>492</v>
       </c>
     </row>
     <row r="187" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A187" s="5" t="s">
-        <v>325</v>
+        <v>517</v>
       </c>
       <c r="B187" s="6" t="s">
         <v>4</v>
@@ -7492,22 +7496,24 @@
         <v>26</v>
       </c>
       <c r="D187" s="5" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="E187" s="6" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F187" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G187" s="6"/>
+      <c r="G187" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="H187" s="7" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="188" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A188" s="5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B188" s="6" t="s">
         <v>4</v>
@@ -7526,12 +7532,12 @@
       </c>
       <c r="G188" s="6"/>
       <c r="H188" s="7" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="189" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A189" s="5" t="s">
-        <v>152</v>
+        <v>327</v>
       </c>
       <c r="B189" s="6" t="s">
         <v>4</v>
@@ -7540,27 +7546,25 @@
         <v>26</v>
       </c>
       <c r="D189" s="5" t="s">
-        <v>428</v>
+        <v>11</v>
       </c>
       <c r="E189" s="6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F189" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G189" s="6" t="s">
-        <v>636</v>
-      </c>
+      <c r="G189" s="6"/>
       <c r="H189" s="7" t="s">
-        <v>151</v>
+        <v>326</v>
       </c>
     </row>
     <row r="190" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A190" s="5" t="s">
-        <v>429</v>
+        <v>152</v>
       </c>
       <c r="B190" s="6" t="s">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="C190" s="5" t="s">
         <v>26</v>
@@ -7575,39 +7579,41 @@
         <v>5</v>
       </c>
       <c r="G190" s="6" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="H190" s="7" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="191" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A191" s="5" t="s">
-        <v>398</v>
+        <v>429</v>
       </c>
       <c r="B191" s="6" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="C191" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D191" s="5" t="s">
-        <v>399</v>
+        <v>428</v>
       </c>
       <c r="E191" s="6" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F191" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G191" s="6"/>
+      <c r="G191" s="6" t="s">
+        <v>637</v>
+      </c>
       <c r="H191" s="7" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="192" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A192" s="5" t="s">
-        <v>614</v>
+        <v>398</v>
       </c>
       <c r="B192" s="6" t="s">
         <v>4</v>
@@ -7616,24 +7622,22 @@
         <v>26</v>
       </c>
       <c r="D192" s="5" t="s">
-        <v>55</v>
+        <v>399</v>
       </c>
       <c r="E192" s="6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F192" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G192" s="6" t="s">
-        <v>56</v>
-      </c>
+      <c r="G192" s="6"/>
       <c r="H192" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="193" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A193" s="5" t="s">
-        <v>666</v>
+        <v>614</v>
       </c>
       <c r="B193" s="6" t="s">
         <v>4</v>
@@ -7642,7 +7646,7 @@
         <v>26</v>
       </c>
       <c r="D193" s="5" t="s">
-        <v>206</v>
+        <v>55</v>
       </c>
       <c r="E193" s="6" t="s">
         <v>5</v>
@@ -7651,15 +7655,15 @@
         <v>5</v>
       </c>
       <c r="G193" s="6" t="s">
-        <v>667</v>
+        <v>56</v>
       </c>
       <c r="H193" s="7" t="s">
-        <v>205</v>
+        <v>54</v>
       </c>
     </row>
     <row r="194" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A194" s="5" t="s">
-        <v>643</v>
+        <v>666</v>
       </c>
       <c r="B194" s="6" t="s">
         <v>4</v>
@@ -7668,7 +7672,7 @@
         <v>26</v>
       </c>
       <c r="D194" s="5" t="s">
-        <v>431</v>
+        <v>206</v>
       </c>
       <c r="E194" s="6" t="s">
         <v>5</v>
@@ -7677,15 +7681,15 @@
         <v>5</v>
       </c>
       <c r="G194" s="6" t="s">
-        <v>644</v>
+        <v>667</v>
       </c>
       <c r="H194" s="7" t="s">
-        <v>164</v>
+        <v>205</v>
       </c>
     </row>
     <row r="195" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A195" s="5" t="s">
-        <v>435</v>
+        <v>643</v>
       </c>
       <c r="B195" s="6" t="s">
         <v>4</v>
@@ -7703,48 +7707,50 @@
         <v>5</v>
       </c>
       <c r="G195" s="6" t="s">
-        <v>665</v>
+        <v>644</v>
       </c>
       <c r="H195" s="7" t="s">
-        <v>204</v>
+        <v>164</v>
       </c>
     </row>
     <row r="196" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A196" s="5" t="s">
-        <v>580</v>
+        <v>435</v>
       </c>
       <c r="B196" s="6" t="s">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="C196" s="5" t="s">
-        <v>581</v>
+        <v>26</v>
       </c>
       <c r="D196" s="5" t="s">
-        <v>399</v>
+        <v>431</v>
       </c>
       <c r="E196" s="6" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F196" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G196" s="6"/>
+      <c r="G196" s="6" t="s">
+        <v>665</v>
+      </c>
       <c r="H196" s="7" t="s">
-        <v>579</v>
+        <v>204</v>
       </c>
     </row>
     <row r="197" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A197" s="5" t="s">
-        <v>573</v>
+        <v>580</v>
       </c>
       <c r="B197" s="6" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="C197" s="5" t="s">
-        <v>425</v>
+        <v>581</v>
       </c>
       <c r="D197" s="5" t="s">
-        <v>60</v>
+        <v>399</v>
       </c>
       <c r="E197" s="6" t="s">
         <v>12</v>
@@ -7754,12 +7760,12 @@
       </c>
       <c r="G197" s="6"/>
       <c r="H197" s="7" t="s">
-        <v>572</v>
+        <v>579</v>
       </c>
     </row>
     <row r="198" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A198" s="5" t="s">
-        <v>613</v>
+        <v>573</v>
       </c>
       <c r="B198" s="6" t="s">
         <v>4</v>
@@ -7768,74 +7774,72 @@
         <v>425</v>
       </c>
       <c r="D198" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E198" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F198" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G198" s="6"/>
+      <c r="H198" s="7" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A199" s="5" t="s">
+        <v>613</v>
+      </c>
+      <c r="B199" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C199" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="D199" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="E198" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F198" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G198" s="6" t="s">
+      <c r="E199" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F199" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G199" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="H198" s="7" t="s">
+      <c r="H199" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A199" s="5" t="s">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A200" s="5" t="s">
         <v>506</v>
       </c>
-      <c r="B199" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C199" s="5" t="s">
+      <c r="B200" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C200" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="D199" s="5" t="s">
+      <c r="D200" s="5" t="s">
         <v>508</v>
       </c>
-      <c r="E199" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F199" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G199" s="6"/>
-      <c r="H199" s="7" t="s">
+      <c r="E200" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F200" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G200" s="6"/>
+      <c r="H200" s="7" t="s">
         <v>505</v>
-      </c>
-    </row>
-    <row r="200" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A200" s="5" t="s">
-        <v>692</v>
-      </c>
-      <c r="B200" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C200" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D200" s="5" t="s">
-        <v>587</v>
-      </c>
-      <c r="E200" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F200" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G200" s="6" t="s">
-        <v>570</v>
-      </c>
-      <c r="H200" s="7" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="201" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A201" s="5" t="s">
-        <v>424</v>
+        <v>691</v>
       </c>
       <c r="B201" s="6" t="s">
         <v>4</v>
@@ -7844,7 +7848,7 @@
         <v>8</v>
       </c>
       <c r="D201" s="5" t="s">
-        <v>9</v>
+        <v>587</v>
       </c>
       <c r="E201" s="6" t="s">
         <v>5</v>
@@ -7853,15 +7857,15 @@
         <v>5</v>
       </c>
       <c r="G201" s="6" t="s">
-        <v>407</v>
+        <v>570</v>
       </c>
       <c r="H201" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="202" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A202" s="5" t="s">
-        <v>615</v>
+        <v>424</v>
       </c>
       <c r="B202" s="6" t="s">
         <v>4</v>
@@ -7870,7 +7874,7 @@
         <v>8</v>
       </c>
       <c r="D202" s="5" t="s">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="E202" s="6" t="s">
         <v>5</v>
@@ -7879,15 +7883,15 @@
         <v>5</v>
       </c>
       <c r="G202" s="6" t="s">
-        <v>63</v>
+        <v>407</v>
       </c>
       <c r="H202" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="203" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A203" s="5" t="s">
-        <v>177</v>
+        <v>615</v>
       </c>
       <c r="B203" s="6" t="s">
         <v>4</v>
@@ -7905,15 +7909,15 @@
         <v>5</v>
       </c>
       <c r="G203" s="6" t="s">
-        <v>648</v>
+        <v>63</v>
       </c>
       <c r="H203" s="7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="204" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A204" s="5" t="s">
-        <v>519</v>
+        <v>177</v>
       </c>
       <c r="B204" s="6" t="s">
         <v>4</v>
@@ -7922,7 +7926,7 @@
         <v>8</v>
       </c>
       <c r="D204" s="5" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E204" s="6" t="s">
         <v>5</v>
@@ -7931,15 +7935,15 @@
         <v>5</v>
       </c>
       <c r="G204" s="6" t="s">
-        <v>73</v>
+        <v>648</v>
       </c>
       <c r="H204" s="7" t="s">
-        <v>71</v>
+        <v>176</v>
       </c>
     </row>
     <row r="205" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A205" s="5" t="s">
-        <v>585</v>
+        <v>519</v>
       </c>
       <c r="B205" s="6" t="s">
         <v>4</v>
@@ -7957,15 +7961,15 @@
         <v>5</v>
       </c>
       <c r="G205" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H205" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="206" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A206" s="5" t="s">
-        <v>69</v>
+        <v>585</v>
       </c>
       <c r="B206" s="6" t="s">
         <v>4</v>
@@ -7974,7 +7978,7 @@
         <v>8</v>
       </c>
       <c r="D206" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E206" s="6" t="s">
         <v>5</v>
@@ -7983,15 +7987,15 @@
         <v>5</v>
       </c>
       <c r="G206" s="6" t="s">
-        <v>569</v>
+        <v>75</v>
       </c>
       <c r="H206" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="207" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A207" s="5" t="s">
-        <v>175</v>
+        <v>69</v>
       </c>
       <c r="B207" s="6" t="s">
         <v>4</v>
@@ -8009,15 +8013,15 @@
         <v>5</v>
       </c>
       <c r="G207" s="6" t="s">
-        <v>432</v>
+        <v>569</v>
       </c>
       <c r="H207" s="7" t="s">
-        <v>174</v>
+        <v>68</v>
       </c>
     </row>
     <row r="208" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A208" s="5" t="s">
-        <v>548</v>
+        <v>175</v>
       </c>
       <c r="B208" s="6" t="s">
         <v>4</v>
@@ -8026,7 +8030,7 @@
         <v>8</v>
       </c>
       <c r="D208" s="5" t="s">
-        <v>173</v>
+        <v>70</v>
       </c>
       <c r="E208" s="6" t="s">
         <v>5</v>
@@ -8035,15 +8039,15 @@
         <v>5</v>
       </c>
       <c r="G208" s="6" t="s">
-        <v>566</v>
+        <v>432</v>
       </c>
       <c r="H208" s="7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="209" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A209" s="5" t="s">
-        <v>30</v>
+        <v>548</v>
       </c>
       <c r="B209" s="6" t="s">
         <v>4</v>
@@ -8052,7 +8056,7 @@
         <v>8</v>
       </c>
       <c r="D209" s="5" t="s">
-        <v>31</v>
+        <v>173</v>
       </c>
       <c r="E209" s="6" t="s">
         <v>5</v>
@@ -8061,15 +8065,15 @@
         <v>5</v>
       </c>
       <c r="G209" s="6" t="s">
-        <v>32</v>
+        <v>566</v>
       </c>
       <c r="H209" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="210" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A210" s="5" t="s">
-        <v>547</v>
+        <v>30</v>
       </c>
       <c r="B210" s="6" t="s">
         <v>4</v>
@@ -8087,15 +8091,15 @@
         <v>5</v>
       </c>
       <c r="G210" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H210" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="211" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A211" s="5" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B211" s="6" t="s">
         <v>4</v>
@@ -8104,7 +8108,7 @@
         <v>8</v>
       </c>
       <c r="D211" s="5" t="s">
-        <v>235</v>
+        <v>31</v>
       </c>
       <c r="E211" s="6" t="s">
         <v>5</v>
@@ -8113,15 +8117,15 @@
         <v>5</v>
       </c>
       <c r="G211" s="6" t="s">
-        <v>567</v>
+        <v>34</v>
       </c>
       <c r="H211" s="7" t="s">
-        <v>234</v>
+        <v>33</v>
       </c>
     </row>
     <row r="212" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A212" s="5" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B212" s="6" t="s">
         <v>4</v>
@@ -8130,27 +8134,53 @@
         <v>8</v>
       </c>
       <c r="D212" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="E212" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F212" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G212" s="6" t="s">
+        <v>567</v>
+      </c>
+      <c r="H212" s="7" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A213" s="5" t="s">
+        <v>550</v>
+      </c>
+      <c r="B213" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C213" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D213" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="E212" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F212" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G212" s="6" t="s">
+      <c r="E213" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F213" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G213" s="6" t="s">
         <v>568</v>
       </c>
-      <c r="H212" s="7" t="s">
+      <c r="H213" s="7" t="s">
         <v>236</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H199" xr:uid="{B9FACE88-1C57-4099-A43D-8DA482706A91}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H212">
-    <sortCondition ref="C8:C212"/>
-    <sortCondition ref="D8:D212"/>
-    <sortCondition ref="H8:H212"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H213">
+    <sortCondition ref="C8:C213"/>
+    <sortCondition ref="D8:D213"/>
+    <sortCondition ref="H8:H213"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added 1 more rule #532
</commit_message>
<xml_diff>
--- a/Deliverables/RULES/USDM_CORE_Rules.xlsx
+++ b/Deliverables/RULES/USDM_CORE_Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stack\CL027\Publish\CORE\3.10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235231A2-FF39-4BA0-AD59-BC173E417838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40994008-9B16-48E0-9DDC-17527580F1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13560" yWindow="-21720" windowWidth="51840" windowHeight="21120" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
+    <workbookView xWindow="-5145" yWindow="-20895" windowWidth="27975" windowHeight="18150" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
   </bookViews>
   <sheets>
     <sheet name="Version 3.0 and 3.10 CORE rules" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1772" uniqueCount="804">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1779" uniqueCount="806">
   <si>
     <t>Textual statement of rule</t>
   </si>
@@ -2451,6 +2451,12 @@
   </si>
   <si>
     <t>includesDNA</t>
+  </si>
+  <si>
+    <t>An observational study (including patient registries) is expected to have a study phase decode value of "NOT APPLICABLE".</t>
+  </si>
+  <si>
+    <t>CHK0276</t>
   </si>
 </sst>
 </file>
@@ -2540,10 +2546,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2863,10 +2865,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FACE88-1C57-4099-A43D-8DA482706A91}">
-  <dimension ref="A1:H232"/>
+  <dimension ref="A1:H233"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5446,18 +5448,18 @@
         <v>787</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
-        <v>795</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>4</v>
+        <v>804</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>783</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>206</v>
+        <v>55</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>12</v>
@@ -5466,12 +5468,12 @@
         <v>5</v>
       </c>
       <c r="H105" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>791</v>
+        <v>795</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>4</v>
@@ -5480,7 +5482,7 @@
         <v>783</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>770</v>
+        <v>206</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>12</v>
@@ -5489,12 +5491,12 @@
         <v>5</v>
       </c>
       <c r="H106" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>785</v>
+        <v>791</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>4</v>
@@ -5503,53 +5505,53 @@
         <v>783</v>
       </c>
       <c r="D107" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H107" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A108" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="D108" s="1" t="s">
         <v>786</v>
       </c>
-      <c r="E107" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F107" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H107" t="s">
+      <c r="E108" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H108" t="s">
         <v>784</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A108" s="1" t="s">
+    <row r="109" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A109" s="1" t="s">
         <v>590</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="B109" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>759</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="E108" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F108" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H108" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A109" s="1" t="s">
-        <v>797</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>759</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>55</v>
+        <v>396</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>12</v>
@@ -5558,12 +5560,12 @@
         <v>5</v>
       </c>
       <c r="H109" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>4</v>
@@ -5572,39 +5574,39 @@
         <v>759</v>
       </c>
       <c r="D110" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H110" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A111" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="D111" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="E110" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F110" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H110" t="s">
+      <c r="E111" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H111" t="s">
         <v>798</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A111" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>595</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E111" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F111" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H111" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="58" x14ac:dyDescent="0.35">
@@ -5615,53 +5617,50 @@
         <v>4</v>
       </c>
       <c r="C112" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H112" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A113" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C113" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="D112" s="1" t="s">
+      <c r="D113" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="E112" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F112" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G112" s="2" t="s">
+      <c r="E113" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G113" s="2" t="s">
         <v>704</v>
       </c>
-      <c r="H112" t="s">
+      <c r="H113" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A113" s="1" t="s">
+    <row r="114" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A114" s="1" t="s">
         <v>740</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="E113" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F113" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G113" s="2" t="s">
-        <v>671</v>
-      </c>
-      <c r="H113" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" ht="116" x14ac:dyDescent="0.35">
-      <c r="A114" s="1" t="s">
-        <v>741</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>4</v>
@@ -5679,44 +5678,44 @@
         <v>5</v>
       </c>
       <c r="G114" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="H114" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="116" x14ac:dyDescent="0.35">
+      <c r="A115" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G115" s="2" t="s">
         <v>692</v>
       </c>
-      <c r="H114" t="s">
+      <c r="H115" t="s">
         <v>329</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A115" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E115" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F115" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G115" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="H115" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="116" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>139</v>
@@ -5731,41 +5730,44 @@
         <v>5</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>638</v>
+        <v>407</v>
       </c>
       <c r="H116" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
-        <v>749</v>
+        <v>343</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>99</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>746</v>
+        <v>139</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F117" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G117" s="2" t="s">
+        <v>638</v>
+      </c>
       <c r="H117" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>746</v>
@@ -5780,38 +5782,35 @@
         <v>5</v>
       </c>
       <c r="H118" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A119" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H119" t="s">
         <v>750</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A119" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="E119" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F119" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G119" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="H119" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="120" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
-        <v>378</v>
+        <v>351</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>99</v>
@@ -5820,24 +5819,27 @@
         <v>192</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
+      </c>
+      <c r="G120" s="2" t="s">
+        <v>372</v>
       </c>
       <c r="H120" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
     </row>
     <row r="121" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
-        <v>752</v>
+        <v>378</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>192</v>
@@ -5846,105 +5848,102 @@
         <v>263</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G121" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H121" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A122" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G122" s="2" t="s">
         <v>587</v>
       </c>
-      <c r="H121" t="s">
+      <c r="H122" t="s">
         <v>456</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A122" s="1" t="s">
-        <v>742</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E122" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F122" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G122" s="2" t="s">
-        <v>709</v>
-      </c>
-      <c r="H122" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="123" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G123" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="H123" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A124" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="B123" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C123" s="1" t="s">
+      <c r="B124" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C124" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="D123" s="1" t="s">
+      <c r="D124" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E123" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F123" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H123" t="s">
+      <c r="E124" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H124" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A124" s="1" t="s">
+    <row r="125" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A125" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="B124" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E124" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F124" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G124" s="2" t="s">
-        <v>643</v>
-      </c>
-      <c r="H124" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A125" s="1" t="s">
-        <v>162</v>
-      </c>
       <c r="B125" s="2" t="s">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>163</v>
+        <v>181</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>5</v>
@@ -5953,15 +5952,15 @@
         <v>5</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>635</v>
+        <v>643</v>
       </c>
       <c r="H125" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
     </row>
     <row r="126" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
-        <v>672</v>
+        <v>162</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>99</v>
@@ -5979,24 +5978,24 @@
         <v>5</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>673</v>
+        <v>635</v>
       </c>
       <c r="H126" t="s">
-        <v>266</v>
+        <v>161</v>
       </c>
     </row>
     <row r="127" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
-        <v>168</v>
+        <v>672</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>5</v>
@@ -6005,15 +6004,15 @@
         <v>5</v>
       </c>
       <c r="G127" s="2" t="s">
-        <v>366</v>
+        <v>673</v>
       </c>
       <c r="H127" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
-        <v>346</v>
+        <v>168</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>4</v>
@@ -6031,15 +6030,15 @@
         <v>5</v>
       </c>
       <c r="G128" s="2" t="s">
-        <v>644</v>
+        <v>366</v>
       </c>
       <c r="H128" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
-        <v>77</v>
+        <v>346</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>4</v>
@@ -6048,7 +6047,7 @@
         <v>46</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>78</v>
+        <v>169</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>5</v>
@@ -6057,15 +6056,15 @@
         <v>5</v>
       </c>
       <c r="G129" s="2" t="s">
-        <v>79</v>
+        <v>644</v>
       </c>
       <c r="H129" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
-        <v>353</v>
+        <v>77</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>4</v>
@@ -6083,15 +6082,15 @@
         <v>5</v>
       </c>
       <c r="G130" s="2" t="s">
-        <v>639</v>
+        <v>79</v>
       </c>
       <c r="H130" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
-        <v>45</v>
+        <v>353</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>4</v>
@@ -6100,7 +6099,7 @@
         <v>46</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>5</v>
@@ -6109,41 +6108,41 @@
         <v>5</v>
       </c>
       <c r="G131" s="2" t="s">
-        <v>48</v>
+        <v>639</v>
       </c>
       <c r="H131" t="s">
-        <v>44</v>
+        <v>267</v>
       </c>
     </row>
     <row r="132" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E132" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F132" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G132" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H132" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A133" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="B132" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D132" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="E132" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F132" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G132" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="H132" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A133" s="1" t="s">
-        <v>344</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>4</v>
@@ -6152,50 +6151,53 @@
         <v>179</v>
       </c>
       <c r="D133" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F133" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G133" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="H133" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A134" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D134" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E133" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F133" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G133" s="2" t="s">
+      <c r="E134" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F134" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G134" s="2" t="s">
         <v>642</v>
       </c>
-      <c r="H133" t="s">
+      <c r="H134" t="s">
         <v>178</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A134" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="D134" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="E134" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F134" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H134" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="135" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>313</v>
@@ -6204,21 +6206,18 @@
         <v>233</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G135" s="2" t="s">
-        <v>584</v>
+        <v>5</v>
       </c>
       <c r="H135" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
     </row>
     <row r="136" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>99</v>
@@ -6227,7 +6226,7 @@
         <v>313</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>169</v>
+        <v>233</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>5</v>
@@ -6236,15 +6235,15 @@
         <v>12</v>
       </c>
       <c r="G136" s="2" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="H136" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
     </row>
     <row r="137" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>99</v>
@@ -6253,50 +6252,50 @@
         <v>313</v>
       </c>
       <c r="D137" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F137" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G137" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="H137" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A138" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D138" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E137" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F137" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G137" s="2" t="s">
+      <c r="E138" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F138" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G138" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="H137" t="s">
+      <c r="H138" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A138" s="1" t="s">
+    <row r="139" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A139" s="1" t="s">
         <v>738</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E138" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F138" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G138" s="2" t="s">
-        <v>645</v>
-      </c>
-      <c r="H138" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A139" s="1" t="s">
-        <v>514</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>4</v>
@@ -6305,7 +6304,7 @@
         <v>65</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>66</v>
+        <v>184</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>5</v>
@@ -6314,87 +6313,87 @@
         <v>5</v>
       </c>
       <c r="G139" s="2" t="s">
-        <v>67</v>
+        <v>645</v>
       </c>
       <c r="H139" t="s">
-        <v>64</v>
+        <v>183</v>
       </c>
     </row>
     <row r="140" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F140" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G140" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H140" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A141" s="1" t="s">
         <v>512</v>
       </c>
-      <c r="B140" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C140" s="1" t="s">
+      <c r="B141" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C141" s="1" t="s">
         <v>508</v>
       </c>
-      <c r="D140" s="1" t="s">
+      <c r="D141" s="1" t="s">
         <v>509</v>
       </c>
-      <c r="E140" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F140" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H140" t="s">
+      <c r="E141" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F141" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H141" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="141" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A141" s="1" t="s">
+    <row r="142" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A142" s="1" t="s">
         <v>592</v>
       </c>
-      <c r="B141" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C141" s="1" t="s">
+      <c r="B142" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C142" s="1" t="s">
         <v>593</v>
       </c>
-      <c r="D141" s="1" t="s">
+      <c r="D142" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E141" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F141" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H141" t="s">
+      <c r="E142" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H142" t="s">
         <v>591</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A142" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C142" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="D142" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="E142" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F142" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G142" s="2" t="s">
-        <v>707</v>
-      </c>
-      <c r="H142" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="143" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
-        <v>336</v>
+        <v>483</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>4</v>
@@ -6403,50 +6402,50 @@
         <v>337</v>
       </c>
       <c r="D143" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F143" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G143" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="H143" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A144" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D144" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="E143" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F143" s="2" t="s">
+      <c r="E144" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F144" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G143" s="2" t="s">
+      <c r="G144" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="H143" t="s">
+      <c r="H144" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="144" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A144" s="1" t="s">
+    <row r="145" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A145" s="1" t="s">
         <v>743</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C144" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D144" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="E144" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F144" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G144" s="2" t="s">
-        <v>713</v>
-      </c>
-      <c r="H144" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A145" s="1" t="s">
-        <v>408</v>
       </c>
       <c r="B145" s="2" t="s">
         <v>4</v>
@@ -6455,7 +6454,7 @@
         <v>157</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>158</v>
+        <v>498</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>5</v>
@@ -6464,15 +6463,15 @@
         <v>5</v>
       </c>
       <c r="G145" s="2" t="s">
-        <v>409</v>
+        <v>713</v>
       </c>
       <c r="H145" t="s">
-        <v>156</v>
+        <v>497</v>
       </c>
     </row>
     <row r="146" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
-        <v>700</v>
+        <v>408</v>
       </c>
       <c r="B146" s="2" t="s">
         <v>4</v>
@@ -6490,41 +6489,41 @@
         <v>5</v>
       </c>
       <c r="G146" s="2" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="H146" t="s">
-        <v>412</v>
+        <v>156</v>
       </c>
     </row>
     <row r="147" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E147" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F147" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G147" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="H147" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A148" s="1" t="s">
         <v>526</v>
-      </c>
-      <c r="B147" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C147" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D147" s="1" t="s">
-        <v>527</v>
-      </c>
-      <c r="E147" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F147" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G147" s="2" t="s">
-        <v>588</v>
-      </c>
-      <c r="H147" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A148" s="1" t="s">
-        <v>611</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>4</v>
@@ -6533,7 +6532,7 @@
         <v>87</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>269</v>
+        <v>527</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>5</v>
@@ -6542,15 +6541,15 @@
         <v>5</v>
       </c>
       <c r="G148" s="2" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="H148" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="149" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
-        <v>354</v>
+        <v>611</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>4</v>
@@ -6568,15 +6567,15 @@
         <v>5</v>
       </c>
       <c r="G149" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="H149" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="150" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>4</v>
@@ -6585,7 +6584,7 @@
         <v>87</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>88</v>
+        <v>269</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>5</v>
@@ -6594,15 +6593,15 @@
         <v>5</v>
       </c>
       <c r="G150" s="2" t="s">
-        <v>89</v>
+        <v>578</v>
       </c>
       <c r="H150" t="s">
-        <v>86</v>
+        <v>271</v>
       </c>
     </row>
     <row r="151" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
-        <v>374</v>
+        <v>359</v>
       </c>
       <c r="B151" s="2" t="s">
         <v>4</v>
@@ -6620,15 +6619,15 @@
         <v>5</v>
       </c>
       <c r="G151" s="2" t="s">
-        <v>406</v>
+        <v>89</v>
       </c>
       <c r="H151" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="B152" s="2" t="s">
         <v>4</v>
@@ -6643,18 +6642,18 @@
         <v>5</v>
       </c>
       <c r="F152" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G152" s="2" t="s">
-        <v>585</v>
+        <v>406</v>
       </c>
       <c r="H152" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
-        <v>529</v>
+        <v>380</v>
       </c>
       <c r="B153" s="2" t="s">
         <v>4</v>
@@ -6663,73 +6662,76 @@
         <v>87</v>
       </c>
       <c r="D153" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E153" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F153" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G153" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="H153" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A154" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D154" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E153" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F153" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G153" s="2" t="s">
+      <c r="E154" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F154" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G154" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="H153" t="s">
+      <c r="H154" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="154" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A154" s="1" t="s">
+    <row r="155" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A155" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="B154" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C154" s="1" t="s">
+      <c r="B155" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C155" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="D154" s="1" t="s">
+      <c r="D155" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E154" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F154" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H154" t="s">
+      <c r="E155" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F155" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H155" t="s">
         <v>394</v>
-      </c>
-    </row>
-    <row r="155" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A155" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B155" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C155" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="E155" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F155" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H155" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="156" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
-        <v>427</v>
+        <v>149</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>401</v>
@@ -6744,61 +6746,58 @@
         <v>5</v>
       </c>
       <c r="H156" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="157" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
-        <v>445</v>
+        <v>427</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>401</v>
       </c>
       <c r="D157" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="E157" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F157" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H157" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A158" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D158" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="E157" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F157" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H157" t="s">
+      <c r="E158" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F158" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H158" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="158" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A158" s="1" t="s">
+    <row r="159" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A159" s="1" t="s">
         <v>436</v>
-      </c>
-      <c r="B158" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D158" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E158" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F158" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G158" s="2" t="s">
-        <v>666</v>
-      </c>
-      <c r="H158" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="159" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A159" s="1" t="s">
-        <v>667</v>
       </c>
       <c r="B159" s="2" t="s">
         <v>4</v>
@@ -6807,7 +6806,7 @@
         <v>211</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E159" s="2" t="s">
         <v>5</v>
@@ -6816,15 +6815,15 @@
         <v>12</v>
       </c>
       <c r="G159" s="2" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="H159" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
-        <v>295</v>
+        <v>667</v>
       </c>
       <c r="B160" s="2" t="s">
         <v>4</v>
@@ -6842,15 +6841,15 @@
         <v>12</v>
       </c>
       <c r="G160" s="2" t="s">
-        <v>687</v>
+        <v>668</v>
       </c>
       <c r="H160" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="161" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
-        <v>435</v>
+        <v>295</v>
       </c>
       <c r="B161" s="2" t="s">
         <v>4</v>
@@ -6859,7 +6858,7 @@
         <v>211</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="E161" s="2" t="s">
         <v>5</v>
@@ -6868,24 +6867,24 @@
         <v>12</v>
       </c>
       <c r="G161" s="2" t="s">
-        <v>665</v>
+        <v>687</v>
       </c>
       <c r="H161" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
-        <v>618</v>
+        <v>435</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>211</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="E162" s="2" t="s">
         <v>5</v>
@@ -6894,24 +6893,24 @@
         <v>12</v>
       </c>
       <c r="G162" s="2" t="s">
-        <v>619</v>
+        <v>665</v>
       </c>
       <c r="H162" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="163" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
-        <v>299</v>
+        <v>618</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>211</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>300</v>
+        <v>187</v>
       </c>
       <c r="E163" s="2" t="s">
         <v>5</v>
@@ -6920,15 +6919,15 @@
         <v>12</v>
       </c>
       <c r="G163" s="2" t="s">
-        <v>439</v>
+        <v>619</v>
       </c>
       <c r="H163" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="164" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
-        <v>433</v>
+        <v>299</v>
       </c>
       <c r="B164" s="2" t="s">
         <v>4</v>
@@ -6937,7 +6936,7 @@
         <v>211</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>212</v>
+        <v>300</v>
       </c>
       <c r="E164" s="2" t="s">
         <v>5</v>
@@ -6946,15 +6945,15 @@
         <v>12</v>
       </c>
       <c r="G164" s="2" t="s">
-        <v>663</v>
+        <v>439</v>
       </c>
       <c r="H164" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
-        <v>302</v>
+        <v>433</v>
       </c>
       <c r="B165" s="2" t="s">
         <v>4</v>
@@ -6972,15 +6971,15 @@
         <v>12</v>
       </c>
       <c r="G165" s="2" t="s">
-        <v>440</v>
+        <v>663</v>
       </c>
       <c r="H165" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="166" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
-        <v>434</v>
+        <v>302</v>
       </c>
       <c r="B166" s="2" t="s">
         <v>4</v>
@@ -6989,7 +6988,7 @@
         <v>211</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E166" s="2" t="s">
         <v>5</v>
@@ -6998,15 +6997,15 @@
         <v>12</v>
       </c>
       <c r="G166" s="2" t="s">
-        <v>664</v>
+        <v>440</v>
       </c>
       <c r="H166" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="167" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
-        <v>297</v>
+        <v>434</v>
       </c>
       <c r="B167" s="2" t="s">
         <v>4</v>
@@ -7024,38 +7023,41 @@
         <v>12</v>
       </c>
       <c r="G167" s="2" t="s">
+        <v>664</v>
+      </c>
+      <c r="H167" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A168" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E168" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F168" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G168" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="H167" t="s">
+      <c r="H168" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A168" s="1" t="s">
+    <row r="169" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A169" s="1" t="s">
         <v>334</v>
-      </c>
-      <c r="B168" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C168" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D168" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E168" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F168" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H168" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="169" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A169" s="1" t="s">
-        <v>736</v>
       </c>
       <c r="B169" s="2" t="s">
         <v>4</v>
@@ -7064,24 +7066,21 @@
         <v>10</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="E169" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F169" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G169" s="2" t="s">
-        <v>633</v>
+        <v>13</v>
       </c>
       <c r="H169" t="s">
-        <v>40</v>
+        <v>333</v>
       </c>
     </row>
     <row r="170" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
-        <v>650</v>
+        <v>736</v>
       </c>
       <c r="B170" s="2" t="s">
         <v>4</v>
@@ -7099,15 +7098,15 @@
         <v>5</v>
       </c>
       <c r="G170" s="2" t="s">
-        <v>651</v>
+        <v>633</v>
       </c>
       <c r="H170" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="171" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
-        <v>289</v>
+        <v>650</v>
       </c>
       <c r="B171" s="2" t="s">
         <v>4</v>
@@ -7116,7 +7115,7 @@
         <v>10</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>290</v>
+        <v>41</v>
       </c>
       <c r="E171" s="2" t="s">
         <v>5</v>
@@ -7125,15 +7124,15 @@
         <v>5</v>
       </c>
       <c r="G171" s="2" t="s">
-        <v>685</v>
+        <v>651</v>
       </c>
       <c r="H171" t="s">
-        <v>288</v>
+        <v>195</v>
       </c>
     </row>
     <row r="172" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A172" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B172" s="2" t="s">
         <v>4</v>
@@ -7142,7 +7141,7 @@
         <v>10</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E172" s="2" t="s">
         <v>5</v>
@@ -7151,15 +7150,15 @@
         <v>5</v>
       </c>
       <c r="G172" s="2" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="H172" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="173" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="s">
-        <v>348</v>
+        <v>292</v>
       </c>
       <c r="B173" s="2" t="s">
         <v>4</v>
@@ -7168,7 +7167,7 @@
         <v>10</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>431</v>
+        <v>293</v>
       </c>
       <c r="E173" s="2" t="s">
         <v>5</v>
@@ -7177,15 +7176,15 @@
         <v>5</v>
       </c>
       <c r="G173" s="2" t="s">
-        <v>379</v>
+        <v>686</v>
       </c>
       <c r="H173" t="s">
-        <v>191</v>
+        <v>291</v>
       </c>
     </row>
     <row r="174" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
-        <v>737</v>
+        <v>348</v>
       </c>
       <c r="B174" s="2" t="s">
         <v>4</v>
@@ -7194,7 +7193,7 @@
         <v>10</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>95</v>
+        <v>431</v>
       </c>
       <c r="E174" s="2" t="s">
         <v>5</v>
@@ -7203,15 +7202,15 @@
         <v>5</v>
       </c>
       <c r="G174" s="2" t="s">
-        <v>634</v>
+        <v>379</v>
       </c>
       <c r="H174" t="s">
-        <v>94</v>
+        <v>191</v>
       </c>
     </row>
     <row r="175" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A175" s="1" t="s">
-        <v>754</v>
+        <v>737</v>
       </c>
       <c r="B175" s="2" t="s">
         <v>4</v>
@@ -7229,15 +7228,15 @@
         <v>5</v>
       </c>
       <c r="G175" s="2" t="s">
-        <v>705</v>
+        <v>634</v>
       </c>
       <c r="H175" t="s">
-        <v>477</v>
+        <v>94</v>
       </c>
     </row>
     <row r="176" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A176" s="1" t="s">
-        <v>548</v>
+        <v>754</v>
       </c>
       <c r="B176" s="2" t="s">
         <v>4</v>
@@ -7249,79 +7248,79 @@
         <v>95</v>
       </c>
       <c r="E176" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F176" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G176" s="2" t="s">
+        <v>705</v>
+      </c>
       <c r="H176" t="s">
-        <v>547</v>
+        <v>477</v>
       </c>
     </row>
     <row r="177" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A177" s="1" t="s">
-        <v>347</v>
+        <v>548</v>
       </c>
       <c r="B177" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>186</v>
+        <v>10</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>187</v>
+        <v>95</v>
       </c>
       <c r="E177" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F177" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G177" s="2" t="s">
-        <v>646</v>
-      </c>
       <c r="H177" t="s">
-        <v>185</v>
+        <v>547</v>
       </c>
     </row>
     <row r="178" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A178" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E178" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F178" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G178" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="H178" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A179" s="1" t="s">
         <v>352</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C178" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="D178" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="E178" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F178" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G178" s="2" t="s">
-        <v>647</v>
-      </c>
-      <c r="H178" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="179" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A179" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="B179" s="2" t="s">
         <v>99</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>101</v>
+        <v>260</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>93</v>
+        <v>261</v>
       </c>
       <c r="E179" s="2" t="s">
         <v>5</v>
@@ -7330,18 +7329,18 @@
         <v>5</v>
       </c>
       <c r="G179" s="2" t="s">
-        <v>615</v>
+        <v>647</v>
       </c>
       <c r="H179" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="180" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A180" s="1" t="s">
-        <v>719</v>
+        <v>518</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>101</v>
@@ -7356,93 +7355,96 @@
         <v>5</v>
       </c>
       <c r="G180" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="H180" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A181" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E181" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F181" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G181" s="2" t="s">
         <v>720</v>
       </c>
-      <c r="H180" t="s">
+      <c r="H181" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="181" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A181" s="1" t="s">
+    <row r="182" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A182" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="B181" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C181" s="1" t="s">
+      <c r="B182" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C182" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D181" s="1" t="s">
+      <c r="D182" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="E181" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F181" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G181" s="2" t="s">
+      <c r="E182" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F182" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G182" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="H181" t="s">
+      <c r="H182" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="182" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A182" s="1" t="s">
+    <row r="183" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A183" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="B182" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C182" s="1" t="s">
+      <c r="B183" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C183" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D182" s="1" t="s">
+      <c r="D183" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E182" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F182" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G182" s="2" t="s">
+      <c r="E183" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F183" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G183" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="H182" t="s">
+      <c r="H183" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="183" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A183" s="1" t="s">
+    <row r="184" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A184" s="1" t="s">
         <v>586</v>
       </c>
-      <c r="B183" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C183" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D183" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="E183" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F183" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H183" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="184" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A184" s="1" t="s">
-        <v>454</v>
-      </c>
       <c r="B184" s="2" t="s">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>22</v>
@@ -7457,38 +7459,35 @@
         <v>5</v>
       </c>
       <c r="H184" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
     </row>
     <row r="185" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A185" s="1" t="s">
-        <v>449</v>
+        <v>454</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="E185" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F185" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G185" s="2" t="s">
-        <v>701</v>
+        <v>5</v>
       </c>
       <c r="H185" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="186" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A186" s="1" t="s">
-        <v>735</v>
+        <v>449</v>
       </c>
       <c r="B186" s="2" t="s">
         <v>4</v>
@@ -7497,7 +7496,7 @@
         <v>22</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>23</v>
+        <v>450</v>
       </c>
       <c r="E186" s="2" t="s">
         <v>5</v>
@@ -7506,18 +7505,18 @@
         <v>12</v>
       </c>
       <c r="G186" s="2" t="s">
-        <v>24</v>
+        <v>701</v>
       </c>
       <c r="H186" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="187" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A187" s="1" t="s">
-        <v>702</v>
+        <v>735</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="C187" s="1" t="s">
         <v>22</v>
@@ -7532,64 +7531,64 @@
         <v>12</v>
       </c>
       <c r="G187" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H187" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A188" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E188" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F188" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G188" s="2" t="s">
         <v>703</v>
       </c>
-      <c r="H187" t="s">
+      <c r="H188" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="188" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A188" s="1" t="s">
+    <row r="189" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A189" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="B188" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C188" s="1" t="s">
+      <c r="B189" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C189" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="D188" s="1" t="s">
+      <c r="D189" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E188" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F188" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H188" t="s">
+      <c r="E189" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F189" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H189" t="s">
         <v>451</v>
-      </c>
-    </row>
-    <row r="189" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A189" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="B189" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C189" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D189" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E189" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F189" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G189" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="H189" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="190" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A190" s="1" t="s">
-        <v>747</v>
+        <v>308</v>
       </c>
       <c r="B190" s="2" t="s">
         <v>4</v>
@@ -7598,24 +7597,24 @@
         <v>197</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>278</v>
+        <v>306</v>
       </c>
       <c r="E190" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F190" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G190" s="2" t="s">
-        <v>679</v>
+        <v>442</v>
       </c>
       <c r="H190" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="191" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A191" s="1" t="s">
-        <v>744</v>
+        <v>747</v>
       </c>
       <c r="B191" s="2" t="s">
         <v>4</v>
@@ -7627,18 +7626,21 @@
         <v>278</v>
       </c>
       <c r="E191" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F191" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="G191" s="2" t="s">
+        <v>679</v>
       </c>
       <c r="H191" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="192" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A192" s="1" t="s">
-        <v>652</v>
+        <v>744</v>
       </c>
       <c r="B192" s="2" t="s">
         <v>4</v>
@@ -7647,24 +7649,21 @@
         <v>197</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>198</v>
+        <v>278</v>
       </c>
       <c r="E192" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F192" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G192" s="2" t="s">
-        <v>653</v>
-      </c>
       <c r="H192" t="s">
-        <v>196</v>
+        <v>699</v>
       </c>
     </row>
     <row r="193" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A193" s="1" t="s">
-        <v>677</v>
+        <v>652</v>
       </c>
       <c r="B193" s="2" t="s">
         <v>4</v>
@@ -7673,53 +7672,53 @@
         <v>197</v>
       </c>
       <c r="D193" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E193" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F193" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G193" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="H193" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A194" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D194" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E193" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F193" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G193" s="2" t="s">
+      <c r="E194" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F194" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G194" s="2" t="s">
         <v>678</v>
       </c>
-      <c r="H193" t="s">
+      <c r="H194" t="s">
         <v>276</v>
-      </c>
-    </row>
-    <row r="194" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A194" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B194" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C194" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="D194" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="E194" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F194" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G194" s="2" t="s">
-        <v>628</v>
-      </c>
-      <c r="H194" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="195" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A195" s="1" t="s">
-        <v>427</v>
+        <v>149</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>208</v>
@@ -7734,64 +7733,67 @@
         <v>12</v>
       </c>
       <c r="G195" s="2" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="H195" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="196" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A196" s="1" t="s">
-        <v>661</v>
+        <v>427</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>208</v>
       </c>
       <c r="D196" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="E196" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F196" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G196" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="H196" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A197" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D197" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E196" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F196" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G196" s="2" t="s">
+      <c r="E197" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F197" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G197" s="2" t="s">
         <v>662</v>
       </c>
-      <c r="H196" t="s">
+      <c r="H197" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="197" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A197" s="1" t="s">
+    <row r="198" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A198" s="1" t="s">
         <v>550</v>
-      </c>
-      <c r="B197" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C197" s="1" t="s">
-        <v>551</v>
-      </c>
-      <c r="D197" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E197" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F197" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H197" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A198" s="1" t="s">
-        <v>602</v>
       </c>
       <c r="B198" s="2" t="s">
         <v>4</v>
@@ -7809,12 +7811,12 @@
         <v>5</v>
       </c>
       <c r="H198" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="199" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A199" s="1" t="s">
-        <v>553</v>
+        <v>602</v>
       </c>
       <c r="B199" s="2" t="s">
         <v>4</v>
@@ -7823,7 +7825,7 @@
         <v>551</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>554</v>
+        <v>60</v>
       </c>
       <c r="E199" s="2" t="s">
         <v>12</v>
@@ -7832,12 +7834,12 @@
         <v>5</v>
       </c>
       <c r="H199" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.35">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A200" s="1" t="s">
-        <v>597</v>
+        <v>553</v>
       </c>
       <c r="B200" s="2" t="s">
         <v>4</v>
@@ -7846,7 +7848,7 @@
         <v>551</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>251</v>
+        <v>554</v>
       </c>
       <c r="E200" s="2" t="s">
         <v>12</v>
@@ -7855,21 +7857,21 @@
         <v>5</v>
       </c>
       <c r="H200" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="201" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A201" s="1" t="s">
-        <v>556</v>
+        <v>597</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>551</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>557</v>
+        <v>251</v>
       </c>
       <c r="E201" s="2" t="s">
         <v>12</v>
@@ -7878,12 +7880,12 @@
         <v>5</v>
       </c>
       <c r="H201" t="s">
-        <v>555</v>
+        <v>596</v>
       </c>
     </row>
     <row r="202" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A202" s="1" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B202" s="2" t="s">
         <v>99</v>
@@ -7901,12 +7903,12 @@
         <v>5</v>
       </c>
       <c r="H202" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="203" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A203" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B203" s="2" t="s">
         <v>99</v>
@@ -7924,70 +7926,67 @@
         <v>5</v>
       </c>
       <c r="H203" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.35">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A204" s="1" t="s">
-        <v>599</v>
+        <v>561</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>551</v>
       </c>
       <c r="D204" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="E204" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F204" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H204" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A205" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="D205" s="1" t="s">
         <v>600</v>
       </c>
-      <c r="E204" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F204" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H204" t="s">
+      <c r="E205" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F205" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H205" t="s">
         <v>598</v>
-      </c>
-    </row>
-    <row r="205" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A205" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="B205" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C205" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D205" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E205" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F205" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G205" s="2" t="s">
-        <v>710</v>
-      </c>
-      <c r="H205" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="206" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A206" s="1" t="s">
-        <v>513</v>
+        <v>489</v>
       </c>
       <c r="B206" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>26</v>
+        <v>165</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="E206" s="2" t="s">
         <v>5</v>
@@ -7996,15 +7995,15 @@
         <v>5</v>
       </c>
       <c r="G206" s="2" t="s">
-        <v>28</v>
+        <v>710</v>
       </c>
       <c r="H206" t="s">
-        <v>25</v>
+        <v>488</v>
       </c>
     </row>
     <row r="207" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A207" s="1" t="s">
-        <v>325</v>
+        <v>513</v>
       </c>
       <c r="B207" s="2" t="s">
         <v>4</v>
@@ -8013,21 +8012,24 @@
         <v>26</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="E207" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F207" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G207" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="H207" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="208" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A208" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B208" s="2" t="s">
         <v>4</v>
@@ -8045,12 +8047,12 @@
         <v>5</v>
       </c>
       <c r="H208" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="209" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A209" s="1" t="s">
-        <v>152</v>
+        <v>327</v>
       </c>
       <c r="B209" s="2" t="s">
         <v>4</v>
@@ -8059,27 +8061,24 @@
         <v>26</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>425</v>
+        <v>11</v>
       </c>
       <c r="E209" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F209" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G209" s="2" t="s">
-        <v>629</v>
-      </c>
       <c r="H209" t="s">
-        <v>151</v>
+        <v>326</v>
       </c>
     </row>
     <row r="210" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A210" s="1" t="s">
-        <v>426</v>
+        <v>152</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>26</v>
@@ -8094,38 +8093,41 @@
         <v>5</v>
       </c>
       <c r="G210" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="H210" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="211" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A211" s="1" t="s">
-        <v>395</v>
+        <v>426</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>396</v>
+        <v>425</v>
       </c>
       <c r="E211" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F211" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G211" s="2" t="s">
+        <v>630</v>
+      </c>
       <c r="H211" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="212" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A212" s="1" t="s">
-        <v>607</v>
+        <v>395</v>
       </c>
       <c r="B212" s="2" t="s">
         <v>4</v>
@@ -8134,24 +8136,21 @@
         <v>26</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>55</v>
+        <v>396</v>
       </c>
       <c r="E212" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F212" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G212" s="2" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="H212" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="213" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A213" s="1" t="s">
-        <v>659</v>
+        <v>607</v>
       </c>
       <c r="B213" s="2" t="s">
         <v>4</v>
@@ -8160,7 +8159,7 @@
         <v>26</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>206</v>
+        <v>55</v>
       </c>
       <c r="E213" s="2" t="s">
         <v>5</v>
@@ -8169,15 +8168,15 @@
         <v>12</v>
       </c>
       <c r="G213" s="2" t="s">
-        <v>660</v>
+        <v>56</v>
       </c>
       <c r="H213" t="s">
-        <v>205</v>
+        <v>54</v>
       </c>
     </row>
     <row r="214" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A214" s="1" t="s">
-        <v>636</v>
+        <v>659</v>
       </c>
       <c r="B214" s="2" t="s">
         <v>4</v>
@@ -8186,24 +8185,24 @@
         <v>26</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>428</v>
+        <v>206</v>
       </c>
       <c r="E214" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F214" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G214" s="2" t="s">
-        <v>637</v>
+        <v>660</v>
       </c>
       <c r="H214" t="s">
-        <v>164</v>
+        <v>205</v>
       </c>
     </row>
     <row r="215" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A215" s="1" t="s">
-        <v>432</v>
+        <v>636</v>
       </c>
       <c r="B215" s="2" t="s">
         <v>4</v>
@@ -8221,61 +8220,64 @@
         <v>5</v>
       </c>
       <c r="G215" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="H215" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A216" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="E216" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F216" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G216" s="2" t="s">
         <v>658</v>
       </c>
-      <c r="H215" t="s">
+      <c r="H216" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="216" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A216" s="1" t="s">
+    <row r="217" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A217" s="1" t="s">
         <v>576</v>
       </c>
-      <c r="B216" s="2" t="s">
+      <c r="B217" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C216" s="1" t="s">
+      <c r="C217" s="1" t="s">
         <v>761</v>
       </c>
-      <c r="D216" s="1" t="s">
+      <c r="D217" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="E216" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F216" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H216" t="s">
+      <c r="E217" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F217" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H217" t="s">
         <v>575</v>
-      </c>
-    </row>
-    <row r="217" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A217" s="1" t="s">
-        <v>569</v>
-      </c>
-      <c r="B217" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C217" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="D217" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E217" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F217" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H217" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="218" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A218" s="1" t="s">
-        <v>606</v>
+        <v>569</v>
       </c>
       <c r="B218" s="2" t="s">
         <v>4</v>
@@ -8284,73 +8286,70 @@
         <v>422</v>
       </c>
       <c r="D218" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E218" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F218" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H218" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A219" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="B219" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D219" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="E218" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F218" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G218" s="2" t="s">
+      <c r="E219" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F219" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G219" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="H218" t="s">
+      <c r="H219" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A219" s="1" t="s">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A220" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="B219" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C219" s="1" t="s">
+      <c r="B220" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C220" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="D219" s="1" t="s">
+      <c r="D220" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="E219" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F219" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H219" t="s">
+      <c r="E220" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F220" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H220" t="s">
         <v>501</v>
-      </c>
-    </row>
-    <row r="220" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A220" s="1" t="s">
-        <v>684</v>
-      </c>
-      <c r="B220" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C220" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D220" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="E220" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F220" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G220" s="2" t="s">
-        <v>566</v>
-      </c>
-      <c r="H220" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="221" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A221" s="1" t="s">
-        <v>421</v>
+        <v>684</v>
       </c>
       <c r="B221" s="2" t="s">
         <v>4</v>
@@ -8359,7 +8358,7 @@
         <v>8</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>9</v>
+        <v>581</v>
       </c>
       <c r="E221" s="2" t="s">
         <v>5</v>
@@ -8368,15 +8367,15 @@
         <v>5</v>
       </c>
       <c r="G221" s="2" t="s">
-        <v>404</v>
+        <v>566</v>
       </c>
       <c r="H221" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="222" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A222" s="1" t="s">
-        <v>608</v>
+        <v>421</v>
       </c>
       <c r="B222" s="2" t="s">
         <v>4</v>
@@ -8385,7 +8384,7 @@
         <v>8</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="E222" s="2" t="s">
         <v>5</v>
@@ -8394,15 +8393,15 @@
         <v>5</v>
       </c>
       <c r="G222" s="2" t="s">
-        <v>63</v>
+        <v>404</v>
       </c>
       <c r="H222" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="223" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A223" s="1" t="s">
-        <v>177</v>
+        <v>608</v>
       </c>
       <c r="B223" s="2" t="s">
         <v>4</v>
@@ -8420,15 +8419,15 @@
         <v>5</v>
       </c>
       <c r="G223" s="2" t="s">
-        <v>641</v>
+        <v>63</v>
       </c>
       <c r="H223" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="224" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A224" s="1" t="s">
-        <v>515</v>
+        <v>177</v>
       </c>
       <c r="B224" s="2" t="s">
         <v>4</v>
@@ -8437,7 +8436,7 @@
         <v>8</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E224" s="2" t="s">
         <v>5</v>
@@ -8446,15 +8445,15 @@
         <v>5</v>
       </c>
       <c r="G224" s="2" t="s">
-        <v>73</v>
+        <v>641</v>
       </c>
       <c r="H224" t="s">
-        <v>71</v>
+        <v>176</v>
       </c>
     </row>
     <row r="225" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A225" s="1" t="s">
-        <v>579</v>
+        <v>515</v>
       </c>
       <c r="B225" s="2" t="s">
         <v>4</v>
@@ -8472,15 +8471,15 @@
         <v>5</v>
       </c>
       <c r="G225" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H225" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="226" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A226" s="1" t="s">
-        <v>69</v>
+        <v>579</v>
       </c>
       <c r="B226" s="2" t="s">
         <v>4</v>
@@ -8489,7 +8488,7 @@
         <v>8</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E226" s="2" t="s">
         <v>5</v>
@@ -8498,15 +8497,15 @@
         <v>5</v>
       </c>
       <c r="G226" s="2" t="s">
-        <v>565</v>
+        <v>75</v>
       </c>
       <c r="H226" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="227" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A227" s="1" t="s">
-        <v>175</v>
+        <v>69</v>
       </c>
       <c r="B227" s="2" t="s">
         <v>4</v>
@@ -8524,15 +8523,15 @@
         <v>5</v>
       </c>
       <c r="G227" s="2" t="s">
-        <v>429</v>
+        <v>565</v>
       </c>
       <c r="H227" t="s">
-        <v>174</v>
+        <v>68</v>
       </c>
     </row>
     <row r="228" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A228" s="1" t="s">
-        <v>544</v>
+        <v>175</v>
       </c>
       <c r="B228" s="2" t="s">
         <v>4</v>
@@ -8541,7 +8540,7 @@
         <v>8</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>173</v>
+        <v>70</v>
       </c>
       <c r="E228" s="2" t="s">
         <v>5</v>
@@ -8550,15 +8549,15 @@
         <v>5</v>
       </c>
       <c r="G228" s="2" t="s">
-        <v>562</v>
+        <v>429</v>
       </c>
       <c r="H228" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="229" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A229" s="1" t="s">
-        <v>30</v>
+        <v>544</v>
       </c>
       <c r="B229" s="2" t="s">
         <v>4</v>
@@ -8567,7 +8566,7 @@
         <v>8</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>31</v>
+        <v>173</v>
       </c>
       <c r="E229" s="2" t="s">
         <v>5</v>
@@ -8576,15 +8575,15 @@
         <v>5</v>
       </c>
       <c r="G229" s="2" t="s">
-        <v>32</v>
+        <v>562</v>
       </c>
       <c r="H229" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="230" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A230" s="1" t="s">
-        <v>543</v>
+        <v>30</v>
       </c>
       <c r="B230" s="2" t="s">
         <v>4</v>
@@ -8602,15 +8601,15 @@
         <v>5</v>
       </c>
       <c r="G230" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H230" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="231" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A231" s="1" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B231" s="2" t="s">
         <v>4</v>
@@ -8619,7 +8618,7 @@
         <v>8</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>235</v>
+        <v>31</v>
       </c>
       <c r="E231" s="2" t="s">
         <v>5</v>
@@ -8628,15 +8627,15 @@
         <v>5</v>
       </c>
       <c r="G231" s="2" t="s">
-        <v>563</v>
+        <v>34</v>
       </c>
       <c r="H231" t="s">
-        <v>234</v>
+        <v>33</v>
       </c>
     </row>
     <row r="232" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A232" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B232" s="2" t="s">
         <v>4</v>
@@ -8645,27 +8644,53 @@
         <v>8</v>
       </c>
       <c r="D232" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E232" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F232" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G232" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="H232" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A233" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C233" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D233" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="E232" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F232" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G232" s="2" t="s">
+      <c r="E233" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F233" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G233" s="2" t="s">
         <v>564</v>
       </c>
-      <c r="H232" t="s">
+      <c r="H233" t="s">
         <v>236</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H1" xr:uid="{B9FACE88-1C57-4099-A43D-8DA482706A91}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H232">
-    <sortCondition ref="C8:C232"/>
-    <sortCondition ref="D8:D232"/>
-    <sortCondition ref="H8:H232"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H233">
+    <sortCondition ref="C8:C233"/>
+    <sortCondition ref="D8:D233"/>
+    <sortCondition ref="H8:H233"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Last changes see ticket #682
</commit_message>
<xml_diff>
--- a/Deliverables/RULES/USDM_CORE_Rules.xlsx
+++ b/Deliverables/RULES/USDM_CORE_Rules.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stack\CL027\Publish\CORE\3.13\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stack\CL027\Publish\CORE\4.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08AA5203-7700-4960-ADF0-97893E942B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8526A368-FF39-418E-B7E6-D26FC6AD0693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
+    <workbookView xWindow="38040" yWindow="-10920" windowWidth="29040" windowHeight="15720" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
   </bookViews>
   <sheets>
     <sheet name="Version 3.0 and 4.0 CORE rules" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Version 3.0 and 4.0 CORE rules'!$A$1:$H$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Version 3.0 and 4.0 CORE rules'!$A$1:$H$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4294961657" uniqueCount="971">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2080" uniqueCount="975">
   <si>
     <t>Textual statement of rule</t>
   </si>
@@ -1688,9 +1688,6 @@
     <t>CHK0195</t>
   </si>
   <si>
-    <t>StudyIdentifier, ReferenceIdentifier, AdministrableProductIdentifier</t>
-  </si>
-  <si>
     <t>CHK0196</t>
   </si>
   <si>
@@ -2858,9 +2855,6 @@
     <t>Version 4.0</t>
   </si>
   <si>
-    <t>If the reason for a study amendment is 'Other' then this must be specified (attribute reasonOther must be completed).</t>
-  </si>
-  <si>
     <t>relativeFromScheduleInstance, relativeToScheduledInstance</t>
   </si>
   <si>
@@ -2900,9 +2894,6 @@
     <t>A reference identifier type must be specified according to the extensible reference identifier type (C215478) DDF codelist  (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
   </si>
   <si>
-    <t>A referenced substance must not have any references to itself.</t>
-  </si>
-  <si>
     <t>An study impact type must be specified according to the extensible study amendment impact type (C215481) DDF codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
   </si>
   <si>
@@ -2952,6 +2943,27 @@
   </si>
   <si>
     <t>DDF00260</t>
+  </si>
+  <si>
+    <t>If the reason for a study amendment is 'Other' then this must be specified (attribute reasonOther must be completed), and vice versa.</t>
+  </si>
+  <si>
+    <t>StudyIdentifier, ReferenceIdentifier, AdministrableProductIdentifier, MedicalDeviceIdentifier</t>
+  </si>
+  <si>
+    <t>A substance must not references itself as a reference substance.</t>
+  </si>
+  <si>
+    <t>A reference substance must not have a reference substance.</t>
+  </si>
+  <si>
+    <t>CHK0316</t>
+  </si>
+  <si>
+    <t>If a geographic scope type is global then no code is expected to specify the specific area within scope while if it is not global then a code is expected to specify the specific area within scope.</t>
+  </si>
+  <si>
+    <t>DDF00261</t>
   </si>
 </sst>
 </file>
@@ -2983,7 +2995,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2993,12 +3005,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3069,7 +3075,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3090,7 +3096,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3435,7 +3440,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FACE88-1C57-4099-A43D-8DA482706A91}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H291"/>
+  <dimension ref="A1:H261"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
@@ -3469,7 +3474,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>6</v>
@@ -3531,7 +3536,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>410</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -3610,7 +3615,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>58</v>
@@ -3628,10 +3633,10 @@
         <v>11</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>968</v>
+        <v>965</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -3671,16 +3676,16 @@
         <v>539</v>
       </c>
       <c r="D9" s="6" t="s">
+        <v>810</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>811</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>812</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>537</v>
@@ -3688,7 +3693,7 @@
     </row>
     <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>58</v>
@@ -3697,23 +3702,23 @@
         <v>539</v>
       </c>
       <c r="D10" s="6" t="s">
+        <v>813</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>814</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>815</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>540</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="8" t="s">
         <v>182</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -3758,7 +3763,7 @@
         <v>11</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>506</v>
@@ -3766,7 +3771,7 @@
     </row>
     <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>10</v>
@@ -3784,10 +3789,10 @@
         <v>11</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -3818,7 +3823,7 @@
     </row>
     <row r="15" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>10</v>
@@ -3836,7 +3841,7 @@
         <v>11</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>508</v>
@@ -3844,7 +3849,7 @@
     </row>
     <row r="16" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>10</v>
@@ -3862,15 +3867,15 @@
         <v>11</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>10</v>
@@ -3888,10 +3893,10 @@
         <v>11</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -4018,25 +4023,25 @@
         <v>11</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C23" s="6" t="s">
+        <v>567</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>568</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>569</v>
-      </c>
       <c r="E23" s="7" t="s">
         <v>23</v>
       </c>
@@ -4044,24 +4049,24 @@
         <v>11</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>23</v>
@@ -4070,24 +4075,24 @@
         <v>11</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
-        <v>958</v>
+        <v>955</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>23</v>
@@ -4096,21 +4101,21 @@
         <v>11</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>99</v>
@@ -4122,25 +4127,25 @@
         <v>11</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
+        <v>698</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>558</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>699</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>559</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>700</v>
-      </c>
       <c r="E27" s="7" t="s">
         <v>23</v>
       </c>
@@ -4148,25 +4153,25 @@
         <v>11</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>558</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>565</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>559</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>566</v>
-      </c>
       <c r="E28" s="7" t="s">
         <v>23</v>
       </c>
@@ -4174,25 +4179,25 @@
         <v>11</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
+        <v>618</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>558</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>619</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>559</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>620</v>
-      </c>
       <c r="E29" s="7" t="s">
         <v>23</v>
       </c>
@@ -4200,24 +4205,24 @@
         <v>11</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="6" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>58</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>23</v>
@@ -4226,21 +4231,21 @@
         <v>11</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>340</v>
@@ -4252,21 +4257,21 @@
         <v>11</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>431</v>
@@ -4278,10 +4283,10 @@
         <v>11</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -4468,7 +4473,7 @@
     </row>
     <row r="40" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="6" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>58</v>
@@ -4486,10 +4491,10 @@
         <v>11</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -4526,7 +4531,7 @@
         <v>10</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>170</v>
@@ -4572,17 +4577,17 @@
     </row>
     <row r="44" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44" s="6" t="s">
+        <v>751</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" s="6" t="s">
         <v>752</v>
       </c>
-      <c r="B44" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C44" s="6" t="s">
+      <c r="D44" s="6" t="s">
         <v>753</v>
       </c>
-      <c r="D44" s="6" t="s">
-        <v>754</v>
-      </c>
       <c r="E44" s="7" t="s">
         <v>23</v>
       </c>
@@ -4590,10 +4595,10 @@
         <v>11</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -4701,7 +4706,7 @@
       </c>
     </row>
     <row r="49" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="9" t="s">
         <v>215</v>
       </c>
       <c r="B49" s="7" t="s">
@@ -4780,17 +4785,17 @@
     </row>
     <row r="52" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="6" t="s">
+        <v>675</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52" s="6" t="s">
         <v>676</v>
       </c>
-      <c r="B52" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C52" s="6" t="s">
+      <c r="D52" s="6" t="s">
         <v>677</v>
       </c>
-      <c r="D52" s="6" t="s">
-        <v>678</v>
-      </c>
       <c r="E52" s="7" t="s">
         <v>23</v>
       </c>
@@ -4798,10 +4803,10 @@
         <v>11</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -4812,7 +4817,7 @@
         <v>10</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>52</v>
@@ -4824,21 +4829,21 @@
         <v>11</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>922</v>
-      </c>
-      <c r="H53" s="10" t="s">
         <v>921</v>
       </c>
+      <c r="H53" s="5" t="s">
+        <v>920</v>
+      </c>
     </row>
     <row r="54" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A54" s="9" t="s">
-        <v>924</v>
+      <c r="A54" s="6" t="s">
+        <v>923</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>58</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>63</v>
@@ -4850,36 +4855,36 @@
         <v>11</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="6" t="s">
+        <v>916</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55" s="6" t="s">
         <v>917</v>
       </c>
-      <c r="B55" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C55" s="6" t="s">
+      <c r="D55" s="6" t="s">
         <v>918</v>
       </c>
-      <c r="D55" s="6" t="s">
+      <c r="E55" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G55" s="7" t="s">
         <v>919</v>
       </c>
-      <c r="E55" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G55" s="7" t="s">
-        <v>920</v>
-      </c>
-      <c r="H55" s="10" t="s">
-        <v>916</v>
+      <c r="H55" s="5" t="s">
+        <v>915</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -4910,7 +4915,7 @@
     </row>
     <row r="57" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="6" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>10</v>
@@ -4919,7 +4924,7 @@
         <v>135</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
       <c r="E57" s="7" t="s">
         <v>23</v>
@@ -4928,15 +4933,15 @@
         <v>11</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A58" s="9" t="s">
-        <v>777</v>
+      <c r="A58" s="6" t="s">
+        <v>776</v>
       </c>
       <c r="B58" s="7" t="s">
         <v>58</v>
@@ -4945,7 +4950,7 @@
         <v>135</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
       <c r="E58" s="7" t="s">
         <v>23</v>
@@ -4954,10 +4959,10 @@
         <v>11</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -4988,7 +4993,7 @@
     </row>
     <row r="60" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A60" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B60" s="7" t="s">
         <v>58</v>
@@ -5006,10 +5011,10 @@
         <v>23</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="58" x14ac:dyDescent="0.35">
@@ -5020,7 +5025,7 @@
         <v>10</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>157</v>
@@ -5032,21 +5037,21 @@
         <v>11</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A62" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>58</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>157</v>
@@ -5058,10 +5063,10 @@
         <v>11</v>
       </c>
       <c r="G62" s="7" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.35">
@@ -5188,7 +5193,7 @@
         <v>11</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="H67" s="5" t="s">
         <v>491</v>
@@ -5196,7 +5201,7 @@
     </row>
     <row r="68" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A68" s="6" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="B68" s="7" t="s">
         <v>10</v>
@@ -5214,7 +5219,7 @@
         <v>11</v>
       </c>
       <c r="G68" s="7" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="H68" s="5" t="s">
         <v>494</v>
@@ -5248,7 +5253,7 @@
     </row>
     <row r="70" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A70" s="6" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>10</v>
@@ -5266,10 +5271,10 @@
         <v>11</v>
       </c>
       <c r="G70" s="7" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -5300,7 +5305,7 @@
     </row>
     <row r="72" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A72" s="6" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B72" s="7" t="s">
         <v>10</v>
@@ -5318,10 +5323,10 @@
         <v>11</v>
       </c>
       <c r="G72" s="7" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -5377,8 +5382,8 @@
       </c>
     </row>
     <row r="75" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A75" s="6" t="s">
-        <v>606</v>
+      <c r="A75" s="9" t="s">
+        <v>605</v>
       </c>
       <c r="B75" s="7" t="s">
         <v>10</v>
@@ -5396,10 +5401,10 @@
         <v>11</v>
       </c>
       <c r="G75" s="7" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -5419,7 +5424,7 @@
         <v>11</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="G76" s="7" t="s">
         <v>222</v>
@@ -5428,253 +5433,253 @@
         <v>218</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A77" s="6" t="s">
-        <v>589</v>
+        <v>973</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>220</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>99</v>
+        <v>221</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="F77" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G77" s="7" t="s">
-        <v>590</v>
+        <v>974</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>588</v>
+        <v>972</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A78" s="6" t="s">
+        <v>588</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E78" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G78" s="7" t="s">
+        <v>589</v>
+      </c>
+      <c r="H78" s="5" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A79" s="6" t="s">
+        <v>625</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>582</v>
+      </c>
+      <c r="D79" s="6" t="s">
         <v>626</v>
       </c>
-      <c r="B78" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C78" s="6" t="s">
+      <c r="E79" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G79" s="7" t="s">
+        <v>627</v>
+      </c>
+      <c r="H79" s="5" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A80" s="6" t="s">
+        <v>581</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>582</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E80" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F80" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G80" s="7" t="s">
         <v>583</v>
       </c>
-      <c r="D78" s="6" t="s">
-        <v>627</v>
-      </c>
-      <c r="E78" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F78" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G78" s="7" t="s">
-        <v>628</v>
-      </c>
-      <c r="H78" s="5" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A79" s="6" t="s">
-        <v>582</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>583</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E79" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F79" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G79" s="7" t="s">
-        <v>584</v>
-      </c>
-      <c r="H79" s="5" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A80" s="6" t="s">
+      <c r="H80" s="5" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A81" s="6" t="s">
         <v>469</v>
       </c>
-      <c r="B80" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C80" s="6" t="s">
+      <c r="B81" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C81" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="D80" s="6" t="s">
+      <c r="D81" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="E80" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F80" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G80" s="7" t="s">
+      <c r="E81" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G81" s="7" t="s">
         <v>472</v>
       </c>
-      <c r="H80" s="5" t="s">
+      <c r="H81" s="5" t="s">
         <v>468</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A81" s="6" t="s">
-        <v>373</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>716</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>374</v>
-      </c>
-      <c r="E81" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F81" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G81" s="7" t="s">
-        <v>861</v>
-      </c>
-      <c r="H81" s="5" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A82" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>715</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="E82" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G82" s="7" t="s">
+        <v>860</v>
+      </c>
+      <c r="H82" s="5" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A83" s="6" t="s">
+        <v>718</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>715</v>
+      </c>
+      <c r="D83" s="6" t="s">
         <v>719</v>
       </c>
-      <c r="B82" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C82" s="6" t="s">
+      <c r="E83" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F83" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G83" s="7" t="s">
+        <v>857</v>
+      </c>
+      <c r="H83" s="5" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A84" s="6" t="s">
+        <v>732</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>715</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>719</v>
+      </c>
+      <c r="E84" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G84" s="7" t="s">
+        <v>865</v>
+      </c>
+      <c r="H84" s="5" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A85" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>715</v>
+      </c>
+      <c r="D85" s="6" t="s">
         <v>716</v>
       </c>
-      <c r="D82" s="6" t="s">
-        <v>720</v>
-      </c>
-      <c r="E82" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F82" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G82" s="7" t="s">
-        <v>858</v>
-      </c>
-      <c r="H82" s="5" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A83" s="6" t="s">
-        <v>733</v>
-      </c>
-      <c r="B83" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C83" s="6" t="s">
+      <c r="E85" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F85" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G85" s="7" t="s">
+        <v>856</v>
+      </c>
+      <c r="H85" s="5" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A86" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>715</v>
+      </c>
+      <c r="D86" s="6" t="s">
         <v>716</v>
       </c>
-      <c r="D83" s="6" t="s">
-        <v>720</v>
-      </c>
-      <c r="E83" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F83" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G83" s="7" t="s">
-        <v>866</v>
-      </c>
-      <c r="H83" s="5" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A84" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="B84" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>716</v>
-      </c>
-      <c r="D84" s="6" t="s">
-        <v>717</v>
-      </c>
-      <c r="E84" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F84" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G84" s="7" t="s">
-        <v>857</v>
-      </c>
-      <c r="H84" s="5" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A85" s="6" t="s">
-        <v>369</v>
-      </c>
-      <c r="B85" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>716</v>
-      </c>
-      <c r="D85" s="6" t="s">
-        <v>717</v>
-      </c>
-      <c r="E85" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F85" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G85" s="7" t="s">
-        <v>860</v>
-      </c>
-      <c r="H85" s="5" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A86" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C86" s="6" t="s">
-        <v>716</v>
-      </c>
-      <c r="D86" s="6" t="s">
-        <v>155</v>
-      </c>
       <c r="E86" s="7" t="s">
         <v>23</v>
       </c>
@@ -5682,21 +5687,21 @@
         <v>11</v>
       </c>
       <c r="G86" s="7" t="s">
-        <v>893</v>
+        <v>859</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>786</v>
+        <v>723</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A87" s="6" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
       <c r="B87" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D87" s="6" t="s">
         <v>354</v>
@@ -5708,25 +5713,25 @@
         <v>11</v>
       </c>
       <c r="G87" s="7" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A88" s="6" t="s">
+        <v>721</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>715</v>
+      </c>
+      <c r="D88" s="6" t="s">
         <v>722</v>
       </c>
-      <c r="B88" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C88" s="6" t="s">
-        <v>716</v>
-      </c>
-      <c r="D88" s="6" t="s">
-        <v>723</v>
-      </c>
       <c r="E88" s="7" t="s">
         <v>23</v>
       </c>
@@ -5734,21 +5739,21 @@
         <v>11</v>
       </c>
       <c r="G88" s="7" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="H88" s="5" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A89" s="6" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
       <c r="B89" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D89" s="6" t="s">
         <v>378</v>
@@ -5760,10 +5765,10 @@
         <v>11</v>
       </c>
       <c r="G89" s="7" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="H89" s="5" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -5774,7 +5779,7 @@
         <v>10</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D90" s="6" t="s">
         <v>378</v>
@@ -5786,21 +5791,21 @@
         <v>11</v>
       </c>
       <c r="G90" s="7" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="H90" s="5" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A91" s="6" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
       <c r="B91" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D91" s="6" t="s">
         <v>378</v>
@@ -5812,21 +5817,21 @@
         <v>11</v>
       </c>
       <c r="G91" s="7" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="H91" s="5" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A92" s="6" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="B92" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D92" s="6" t="s">
         <v>378</v>
@@ -5838,21 +5843,21 @@
         <v>11</v>
       </c>
       <c r="G92" s="7" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="H92" s="5" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A93" s="6" t="s">
-        <v>966</v>
+      <c r="A93" s="9" t="s">
+        <v>963</v>
       </c>
       <c r="B93" s="7" t="s">
         <v>58</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D93" s="6" t="s">
         <v>378</v>
@@ -5864,24 +5869,24 @@
         <v>11</v>
       </c>
       <c r="G93" s="7" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="H93" s="5" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A94" s="6" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B94" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E94" s="7" t="s">
         <v>23</v>
@@ -5890,10 +5895,10 @@
         <v>11</v>
       </c>
       <c r="G94" s="7" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="H94" s="5" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -5904,7 +5909,7 @@
         <v>10</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D95" s="6" t="s">
         <v>463</v>
@@ -5916,10 +5921,10 @@
         <v>11</v>
       </c>
       <c r="G95" s="7" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="H95" s="5" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -5950,16 +5955,16 @@
     </row>
     <row r="97" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A97" s="6" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
       <c r="B97" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="E97" s="7" t="s">
         <v>23</v>
@@ -5968,21 +5973,21 @@
         <v>11</v>
       </c>
       <c r="G97" s="7" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="H97" s="5" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A98" s="6" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
       <c r="B98" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D98" s="6" t="s">
         <v>99</v>
@@ -5994,10 +5999,10 @@
         <v>11</v>
       </c>
       <c r="G98" s="7" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="H98" s="5" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -6020,7 +6025,7 @@
         <v>11</v>
       </c>
       <c r="G99" s="7" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="H99" s="5" t="s">
         <v>514</v>
@@ -6046,7 +6051,7 @@
         <v>11</v>
       </c>
       <c r="G100" s="7" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="H100" s="5" t="s">
         <v>528</v>
@@ -6054,7 +6059,7 @@
     </row>
     <row r="101" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A101" s="6" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B101" s="7" t="s">
         <v>10</v>
@@ -6063,7 +6068,7 @@
         <v>162</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="E101" s="7" t="s">
         <v>23</v>
@@ -6072,10 +6077,10 @@
         <v>11</v>
       </c>
       <c r="G101" s="7" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="H101" s="5" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -6124,10 +6129,10 @@
         <v>11</v>
       </c>
       <c r="G103" s="7" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="H103" s="5" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -6150,7 +6155,7 @@
         <v>11</v>
       </c>
       <c r="G104" s="7" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="H104" s="5" t="s">
         <v>517</v>
@@ -6176,7 +6181,7 @@
         <v>11</v>
       </c>
       <c r="G105" s="7" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="H105" s="5" t="s">
         <v>520</v>
@@ -6210,7 +6215,7 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" s="6" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B107" s="7" t="s">
         <v>58</v>
@@ -6228,15 +6233,15 @@
         <v>23</v>
       </c>
       <c r="G107" s="7" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="H107" s="5" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A108" s="6" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="B108" s="7" t="s">
         <v>10</v>
@@ -6254,7 +6259,7 @@
         <v>11</v>
       </c>
       <c r="G108" s="7" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="H108" s="5" t="s">
         <v>512</v>
@@ -6262,7 +6267,7 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" s="6" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B109" s="7" t="s">
         <v>58</v>
@@ -6280,15 +6285,15 @@
         <v>11</v>
       </c>
       <c r="G109" s="7" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="H109" s="5" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A110" s="9" t="s">
-        <v>903</v>
+      <c r="A110" s="6" t="s">
+        <v>902</v>
       </c>
       <c r="B110" s="7" t="s">
         <v>10</v>
@@ -6306,10 +6311,10 @@
         <v>11</v>
       </c>
       <c r="G110" s="7" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="H110" s="5" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -6340,7 +6345,7 @@
     </row>
     <row r="112" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A112" s="6" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B112" s="7" t="s">
         <v>10</v>
@@ -6358,24 +6363,24 @@
         <v>11</v>
       </c>
       <c r="G112" s="7" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="H112" s="5" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="113" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A113" s="6" t="s">
+        <v>734</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C113" s="6" t="s">
         <v>735</v>
       </c>
-      <c r="B113" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C113" s="6" t="s">
-        <v>736</v>
-      </c>
       <c r="D113" s="6" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="E113" s="7" t="s">
         <v>23</v>
@@ -6384,25 +6389,25 @@
         <v>11</v>
       </c>
       <c r="G113" s="7" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="H113" s="5" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="114" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A114" s="6" t="s">
+        <v>740</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C114" s="6" t="s">
+        <v>735</v>
+      </c>
+      <c r="D114" s="6" t="s">
         <v>741</v>
       </c>
-      <c r="B114" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C114" s="6" t="s">
-        <v>736</v>
-      </c>
-      <c r="D114" s="6" t="s">
-        <v>742</v>
-      </c>
       <c r="E114" s="7" t="s">
         <v>23</v>
       </c>
@@ -6410,21 +6415,21 @@
         <v>11</v>
       </c>
       <c r="G114" s="7" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="H114" s="5" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="115" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A115" s="6" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B115" s="7" t="s">
         <v>58</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D115" s="6" t="s">
         <v>77</v>
@@ -6436,21 +6441,21 @@
         <v>11</v>
       </c>
       <c r="G115" s="7" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="H115" s="5" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="116" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A116" s="6" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B116" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D116" s="6" t="s">
         <v>354</v>
@@ -6462,24 +6467,24 @@
         <v>11</v>
       </c>
       <c r="G116" s="7" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="H116" s="5" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="117" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A117" s="6" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
       <c r="B117" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D117" s="6" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E117" s="7" t="s">
         <v>23</v>
@@ -6488,47 +6493,47 @@
         <v>11</v>
       </c>
       <c r="G117" s="7" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="H117" s="5" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A118" s="6" t="s">
+        <v>737</v>
+      </c>
+      <c r="B118" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>735</v>
+      </c>
+      <c r="D118" s="6" t="s">
         <v>738</v>
       </c>
-      <c r="B118" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C118" s="6" t="s">
+      <c r="E118" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F118" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G118" s="7" t="s">
+        <v>867</v>
+      </c>
+      <c r="H118" s="5" t="s">
         <v>736</v>
-      </c>
-      <c r="D118" s="6" t="s">
-        <v>739</v>
-      </c>
-      <c r="E118" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F118" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G118" s="7" t="s">
-        <v>868</v>
-      </c>
-      <c r="H118" s="5" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="119" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A119" s="6" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="B119" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="D119" s="6" t="s">
         <v>22</v>
@@ -6540,7 +6545,7 @@
         <v>11</v>
       </c>
       <c r="G119" s="7" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="H119" s="5" t="s">
         <v>498</v>
@@ -6548,13 +6553,13 @@
     </row>
     <row r="120" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A120" s="6" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="B120" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="D120" s="6" t="s">
         <v>22</v>
@@ -6566,7 +6571,7 @@
         <v>11</v>
       </c>
       <c r="G120" s="7" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="H120" s="5" t="s">
         <v>499</v>
@@ -6574,13 +6579,13 @@
     </row>
     <row r="121" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A121" s="6" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B121" s="7" t="s">
         <v>58</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="D121" s="6" t="s">
         <v>527</v>
@@ -6592,21 +6597,21 @@
         <v>11</v>
       </c>
       <c r="G121" s="7" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="H121" s="5" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A122" s="6" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B122" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="D122" s="6" t="s">
         <v>77</v>
@@ -6618,21 +6623,21 @@
         <v>11</v>
       </c>
       <c r="G122" s="7" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="H122" s="5" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="123" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A123" s="6" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B123" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="D123" s="6" t="s">
         <v>354</v>
@@ -6644,21 +6649,21 @@
         <v>11</v>
       </c>
       <c r="G123" s="7" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="H123" s="5" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A124" s="6" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B124" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>99</v>
@@ -6670,36 +6675,36 @@
         <v>11</v>
       </c>
       <c r="G124" s="7" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="H124" s="5" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A125" s="6" t="s">
+        <v>572</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C125" s="6" t="s">
         <v>573</v>
       </c>
-      <c r="B125" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C125" s="6" t="s">
+      <c r="D125" s="6" t="s">
         <v>574</v>
       </c>
-      <c r="D125" s="6" t="s">
+      <c r="E125" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F125" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G125" s="7" t="s">
         <v>575</v>
       </c>
-      <c r="E125" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F125" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G125" s="7" t="s">
-        <v>576</v>
-      </c>
       <c r="H125" s="5" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="126" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -6756,28 +6761,28 @@
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" s="6" t="s">
+        <v>911</v>
+      </c>
+      <c r="B128" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C128" s="6" t="s">
         <v>912</v>
       </c>
-      <c r="B128" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C128" s="6" t="s">
+      <c r="D128" s="6" t="s">
         <v>913</v>
       </c>
-      <c r="D128" s="6" t="s">
+      <c r="E128" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F128" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G128" s="7" t="s">
         <v>914</v>
       </c>
-      <c r="E128" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F128" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G128" s="7" t="s">
-        <v>915</v>
-      </c>
       <c r="H128" s="5" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -6834,7 +6839,7 @@
     </row>
     <row r="131" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A131" s="6" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="B131" s="7" t="s">
         <v>10</v>
@@ -6852,21 +6857,21 @@
         <v>11</v>
       </c>
       <c r="G131" s="7" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="H131" s="5" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="132" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A132" s="6" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B132" s="7" t="s">
         <v>58</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D132" s="6" t="s">
         <v>82</v>
@@ -6878,21 +6883,21 @@
         <v>11</v>
       </c>
       <c r="G132" s="7" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="H132" s="5" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="133" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A133" s="6" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B133" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D133" s="6" t="s">
         <v>82</v>
@@ -6904,24 +6909,24 @@
         <v>11</v>
       </c>
       <c r="G133" s="7" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="H133" s="5" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="134" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A134" s="6" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B134" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="D134" s="6" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E134" s="7" t="s">
         <v>23</v>
@@ -6930,10 +6935,10 @@
         <v>11</v>
       </c>
       <c r="G134" s="7" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="H134" s="5" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.35">
@@ -6964,7 +6969,7 @@
     </row>
     <row r="136" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A136" s="6" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B136" s="7" t="s">
         <v>10</v>
@@ -6982,15 +6987,15 @@
         <v>23</v>
       </c>
       <c r="G136" s="7" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H136" s="5" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="137" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A137" s="9" t="s">
-        <v>767</v>
+      <c r="A137" s="6" t="s">
+        <v>766</v>
       </c>
       <c r="B137" s="7" t="s">
         <v>10</v>
@@ -7008,15 +7013,15 @@
         <v>11</v>
       </c>
       <c r="G137" s="7" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="H137" s="5" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="138" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A138" s="6" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="B138" s="7" t="s">
         <v>10</v>
@@ -7034,47 +7039,47 @@
         <v>11</v>
       </c>
       <c r="G138" s="7" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="H138" s="5" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="139" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A139" s="6" t="s">
+        <v>591</v>
+      </c>
+      <c r="B139" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C139" s="6" t="s">
         <v>592</v>
       </c>
-      <c r="B139" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C139" s="6" t="s">
+      <c r="D139" s="6" t="s">
         <v>593</v>
       </c>
-      <c r="D139" s="6" t="s">
+      <c r="E139" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F139" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G139" s="7" t="s">
         <v>594</v>
       </c>
-      <c r="E139" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F139" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G139" s="7" t="s">
-        <v>595</v>
-      </c>
       <c r="H139" s="5" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="140" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A140" s="6" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="B140" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D140" s="6" t="s">
         <v>99</v>
@@ -7086,10 +7091,10 @@
         <v>11</v>
       </c>
       <c r="G140" s="7" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="H140" s="5" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="141" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -7372,7 +7377,7 @@
         <v>11</v>
       </c>
       <c r="G151" s="7" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="H151" s="5" t="s">
         <v>486</v>
@@ -7510,7 +7515,7 @@
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A157" s="6" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B157" s="7" t="s">
         <v>58</v>
@@ -7519,34 +7524,34 @@
         <v>94</v>
       </c>
       <c r="D157" s="6" t="s">
+        <v>927</v>
+      </c>
+      <c r="E157" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F157" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G157" s="7" t="s">
         <v>928</v>
       </c>
-      <c r="E157" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F157" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G157" s="7" t="s">
-        <v>929</v>
-      </c>
       <c r="H157" s="5" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A158" s="6" t="s">
+        <v>621</v>
+      </c>
+      <c r="B158" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C158" s="6" t="s">
         <v>622</v>
       </c>
-      <c r="B158" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C158" s="6" t="s">
+      <c r="D158" s="6" t="s">
         <v>623</v>
       </c>
-      <c r="D158" s="6" t="s">
-        <v>624</v>
-      </c>
       <c r="E158" s="7" t="s">
         <v>23</v>
       </c>
@@ -7554,50 +7559,50 @@
         <v>11</v>
       </c>
       <c r="G158" s="7" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="H158" s="5" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A159" s="6" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B159" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C159" s="6" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D159" s="6" t="s">
+        <v>879</v>
+      </c>
+      <c r="E159" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F159" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G159" s="7" t="s">
         <v>880</v>
       </c>
-      <c r="E159" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F159" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G159" s="7" t="s">
-        <v>881</v>
-      </c>
       <c r="H159" s="5" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="160" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A160" s="6" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B160" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C160" s="6" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D160" s="6" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="E160" s="7" t="s">
         <v>23</v>
@@ -7606,21 +7611,21 @@
         <v>11</v>
       </c>
       <c r="G160" s="7" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="H160" s="5" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="161" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A161" s="6" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
       <c r="B161" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C161" s="6" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="D161" s="6" t="s">
         <v>99</v>
@@ -7632,15 +7637,15 @@
         <v>11</v>
       </c>
       <c r="G161" s="7" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="H161" s="5" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="162" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A162" s="6" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B162" s="7" t="s">
         <v>10</v>
@@ -7658,15 +7663,15 @@
         <v>11</v>
       </c>
       <c r="G162" s="7" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="H162" s="5" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A163" s="9" t="s">
-        <v>790</v>
+      <c r="A163" s="6" t="s">
+        <v>789</v>
       </c>
       <c r="B163" s="7" t="s">
         <v>58</v>
@@ -7684,15 +7689,15 @@
         <v>11</v>
       </c>
       <c r="G163" s="7" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="H163" s="5" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="164" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A164" s="6" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B164" s="7" t="s">
         <v>58</v>
@@ -7710,15 +7715,15 @@
         <v>11</v>
       </c>
       <c r="G164" s="7" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="H164" s="5" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="165" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A165" s="6" t="s">
-        <v>939</v>
+        <v>968</v>
       </c>
       <c r="B165" s="7" t="s">
         <v>10</v>
@@ -7744,7 +7749,7 @@
     </row>
     <row r="166" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A166" s="6" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B166" s="7" t="s">
         <v>10</v>
@@ -7753,23 +7758,23 @@
         <v>202</v>
       </c>
       <c r="D166" s="6" t="s">
+        <v>609</v>
+      </c>
+      <c r="E166" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F166" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G166" s="7" t="s">
         <v>610</v>
       </c>
-      <c r="E166" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F166" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G166" s="7" t="s">
-        <v>611</v>
-      </c>
       <c r="H166" s="5" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="167" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A167" s="6" t="s">
+      <c r="A167" s="9" t="s">
         <v>201</v>
       </c>
       <c r="B167" s="7" t="s">
@@ -7785,7 +7790,7 @@
         <v>11</v>
       </c>
       <c r="F167" s="7" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="G167" s="7" t="s">
         <v>204</v>
@@ -7822,7 +7827,7 @@
     </row>
     <row r="169" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A169" s="6" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B169" s="7" t="s">
         <v>10</v>
@@ -7831,19 +7836,19 @@
         <v>123</v>
       </c>
       <c r="D169" s="6" t="s">
+        <v>630</v>
+      </c>
+      <c r="E169" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F169" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G169" s="7" t="s">
         <v>631</v>
       </c>
-      <c r="E169" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F169" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G169" s="7" t="s">
-        <v>632</v>
-      </c>
       <c r="H169" s="5" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.35">
@@ -7900,7 +7905,7 @@
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A172" s="6" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="B172" s="7" t="s">
         <v>58</v>
@@ -7918,10 +7923,10 @@
         <v>11</v>
       </c>
       <c r="G172" s="7" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="H172" s="5" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.35">
@@ -8004,7 +8009,7 @@
     </row>
     <row r="176" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A176" s="6" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B176" s="7" t="s">
         <v>10</v>
@@ -8022,25 +8027,25 @@
         <v>11</v>
       </c>
       <c r="G176" s="7" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="H176" s="5" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="177" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A177" s="6" t="s">
+        <v>780</v>
+      </c>
+      <c r="B177" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C177" s="6" t="s">
         <v>781</v>
       </c>
-      <c r="B177" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C177" s="6" t="s">
+      <c r="D177" s="6" t="s">
         <v>782</v>
       </c>
-      <c r="D177" s="6" t="s">
-        <v>783</v>
-      </c>
       <c r="E177" s="7" t="s">
         <v>23</v>
       </c>
@@ -8048,15 +8053,15 @@
         <v>11</v>
       </c>
       <c r="G177" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="H177" s="5" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="178" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A178" s="6" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="B178" s="7" t="s">
         <v>10</v>
@@ -8074,7 +8079,7 @@
         <v>11</v>
       </c>
       <c r="G178" s="7" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="H178" s="5" t="s">
         <v>523</v>
@@ -8100,10 +8105,10 @@
         <v>11</v>
       </c>
       <c r="G179" s="7" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="H179" s="5" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="180" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -8126,15 +8131,15 @@
         <v>11</v>
       </c>
       <c r="G180" s="7" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="H180" s="5" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="181" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A181" s="6" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="B181" s="7" t="s">
         <v>10</v>
@@ -8152,7 +8157,7 @@
         <v>11</v>
       </c>
       <c r="G181" s="7" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="H181" s="5" t="s">
         <v>531</v>
@@ -8341,7 +8346,7 @@
       </c>
     </row>
     <row r="189" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A189" s="6" t="s">
+      <c r="A189" s="9" t="s">
         <v>466</v>
       </c>
       <c r="B189" s="7" t="s">
@@ -8367,7 +8372,7 @@
       </c>
     </row>
     <row r="190" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A190" s="6" t="s">
+      <c r="A190" s="9" t="s">
         <v>365</v>
       </c>
       <c r="B190" s="7" t="s">
@@ -8419,8 +8424,8 @@
       </c>
     </row>
     <row r="192" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A192" s="9" t="s">
-        <v>779</v>
+      <c r="A192" s="6" t="s">
+        <v>778</v>
       </c>
       <c r="B192" s="7" t="s">
         <v>10</v>
@@ -8438,10 +8443,10 @@
         <v>11</v>
       </c>
       <c r="G192" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="H192" s="5" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="193" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -8516,10 +8521,10 @@
         <v>11</v>
       </c>
       <c r="G195" s="7" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="H195" s="5" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="196" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -8550,7 +8555,7 @@
     </row>
     <row r="197" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A197" s="6" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="B197" s="7" t="s">
         <v>10</v>
@@ -8568,10 +8573,10 @@
         <v>11</v>
       </c>
       <c r="G197" s="7" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="H197" s="5" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="198" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -8602,7 +8607,7 @@
     </row>
     <row r="199" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A199" s="6" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B199" s="7" t="s">
         <v>10</v>
@@ -8620,10 +8625,10 @@
         <v>11</v>
       </c>
       <c r="G199" s="7" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H199" s="5" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="200" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -8680,7 +8685,7 @@
     </row>
     <row r="202" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A202" s="6" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="B202" s="7" t="s">
         <v>10</v>
@@ -8698,15 +8703,15 @@
         <v>11</v>
       </c>
       <c r="G202" s="7" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="H202" s="5" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="203" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A203" s="6" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B203" s="7" t="s">
         <v>10</v>
@@ -8724,10 +8729,10 @@
         <v>11</v>
       </c>
       <c r="G203" s="7" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="H203" s="5" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="204" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -8758,7 +8763,7 @@
     </row>
     <row r="205" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A205" s="6" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="B205" s="7" t="s">
         <v>10</v>
@@ -8776,10 +8781,10 @@
         <v>11</v>
       </c>
       <c r="G205" s="7" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="H205" s="5" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="206" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -8836,7 +8841,7 @@
     </row>
     <row r="208" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A208" s="6" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B208" s="7" t="s">
         <v>10</v>
@@ -8854,10 +8859,10 @@
         <v>11</v>
       </c>
       <c r="G208" s="7" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="H208" s="5" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="209" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -8932,7 +8937,7 @@
         <v>11</v>
       </c>
       <c r="G211" s="7" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="H211" s="5" t="s">
         <v>541</v>
@@ -8940,7 +8945,7 @@
     </row>
     <row r="212" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A212" s="6" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B212" s="7" t="s">
         <v>58</v>
@@ -8958,10 +8963,10 @@
         <v>11</v>
       </c>
       <c r="G212" s="7" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H212" s="5" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="213" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -9018,7 +9023,7 @@
     </row>
     <row r="215" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A215" s="6" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B215" s="7" t="s">
         <v>58</v>
@@ -9036,13 +9041,13 @@
         <v>23</v>
       </c>
       <c r="G215" s="7" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="H215" s="5" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="216" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A216" s="6" t="s">
         <v>545</v>
       </c>
@@ -9050,7 +9055,7 @@
         <v>10</v>
       </c>
       <c r="C216" s="6" t="s">
-        <v>549</v>
+        <v>969</v>
       </c>
       <c r="D216" s="6" t="s">
         <v>157</v>
@@ -9062,7 +9067,7 @@
         <v>11</v>
       </c>
       <c r="G216" s="7" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H216" s="5" t="s">
         <v>548</v>
@@ -9122,7 +9127,7 @@
     </row>
     <row r="219" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A219" s="6" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B219" s="7" t="s">
         <v>10</v>
@@ -9140,10 +9145,10 @@
         <v>11</v>
       </c>
       <c r="G219" s="7" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="H219" s="5" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="220" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -9278,13 +9283,13 @@
     </row>
     <row r="225" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A225" s="6" t="s">
+        <v>658</v>
+      </c>
+      <c r="B225" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C225" s="6" t="s">
         <v>659</v>
-      </c>
-      <c r="B225" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C225" s="6" t="s">
-        <v>660</v>
       </c>
       <c r="D225" s="6" t="s">
         <v>82</v>
@@ -9296,21 +9301,21 @@
         <v>11</v>
       </c>
       <c r="G225" s="7" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="H225" s="5" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A226" s="6" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B226" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C226" s="6" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D226" s="6" t="s">
         <v>82</v>
@@ -9322,47 +9327,47 @@
         <v>11</v>
       </c>
       <c r="G226" s="7" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="H226" s="5" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A227" s="6" t="s">
+        <v>661</v>
+      </c>
+      <c r="B227" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C227" s="6" t="s">
+        <v>659</v>
+      </c>
+      <c r="D227" s="6" t="s">
         <v>662</v>
       </c>
-      <c r="B227" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C227" s="6" t="s">
+      <c r="E227" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F227" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G227" s="7" t="s">
+        <v>833</v>
+      </c>
+      <c r="H227" s="5" t="s">
         <v>660</v>
-      </c>
-      <c r="D227" s="6" t="s">
-        <v>663</v>
-      </c>
-      <c r="E227" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F227" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G227" s="7" t="s">
-        <v>834</v>
-      </c>
-      <c r="H227" s="5" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A228" s="6" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
       <c r="B228" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C228" s="6" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D228" s="6" t="s">
         <v>221</v>
@@ -9374,21 +9379,21 @@
         <v>11</v>
       </c>
       <c r="G228" s="7" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="H228" s="5" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="229" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A229" s="6" t="s">
-        <v>967</v>
+      <c r="A229" s="9" t="s">
+        <v>964</v>
       </c>
       <c r="B229" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C229" s="6" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D229" s="6" t="s">
         <v>221</v>
@@ -9400,24 +9405,24 @@
         <v>11</v>
       </c>
       <c r="G229" s="7" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="H229" s="5" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="230" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A230" s="6" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B230" s="7" t="s">
         <v>58</v>
       </c>
       <c r="C230" s="6" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D230" s="6" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="E230" s="7" t="s">
         <v>23</v>
@@ -9426,50 +9431,50 @@
         <v>11</v>
       </c>
       <c r="G230" s="7" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="H230" s="5" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="231" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A231" s="6" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B231" s="7" t="s">
         <v>58</v>
       </c>
       <c r="C231" s="6" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D231" s="6" t="s">
+        <v>665</v>
+      </c>
+      <c r="E231" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F231" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G231" s="7" t="s">
+        <v>835</v>
+      </c>
+      <c r="H231" s="5" t="s">
         <v>666</v>
-      </c>
-      <c r="E231" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F231" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G231" s="7" t="s">
-        <v>836</v>
-      </c>
-      <c r="H231" s="5" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="232" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A232" s="6" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B232" s="7" t="s">
         <v>58</v>
       </c>
       <c r="C232" s="6" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D232" s="6" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="E232" s="7" t="s">
         <v>23</v>
@@ -9478,25 +9483,25 @@
         <v>11</v>
       </c>
       <c r="G232" s="7" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="H232" s="5" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A233" s="6" t="s">
+        <v>690</v>
+      </c>
+      <c r="B233" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C233" s="6" t="s">
+        <v>659</v>
+      </c>
+      <c r="D233" s="6" t="s">
         <v>691</v>
       </c>
-      <c r="B233" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C233" s="6" t="s">
-        <v>660</v>
-      </c>
-      <c r="D233" s="6" t="s">
-        <v>692</v>
-      </c>
       <c r="E233" s="7" t="s">
         <v>23</v>
       </c>
@@ -9504,21 +9509,21 @@
         <v>11</v>
       </c>
       <c r="G233" s="7" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="H233" s="5" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="234" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A234" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="B234" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C234" s="6" t="s">
         <v>597</v>
-      </c>
-      <c r="B234" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C234" s="6" t="s">
-        <v>598</v>
       </c>
       <c r="D234" s="6" t="s">
         <v>99</v>
@@ -9530,10 +9535,10 @@
         <v>11</v>
       </c>
       <c r="G234" s="7" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="H234" s="5" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="235" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -9615,7 +9620,7 @@
       </c>
     </row>
     <row r="238" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A238" s="6" t="s">
+      <c r="A238" s="9" t="s">
         <v>526</v>
       </c>
       <c r="B238" s="7" t="s">
@@ -9634,7 +9639,7 @@
         <v>11</v>
       </c>
       <c r="G238" s="7" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="H238" s="5" t="s">
         <v>525</v>
@@ -9746,13 +9751,13 @@
     </row>
     <row r="243" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A243" s="6" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B243" s="7" t="s">
         <v>58</v>
       </c>
       <c r="C243" s="6" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D243" s="6" t="s">
         <v>527</v>
@@ -9764,15 +9769,15 @@
         <v>11</v>
       </c>
       <c r="G243" s="7" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="H243" s="5" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="244" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A244" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B244" s="7" t="s">
         <v>10</v>
@@ -9781,7 +9786,7 @@
         <v>62</v>
       </c>
       <c r="D244" s="6" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="E244" s="7" t="s">
         <v>23</v>
@@ -9790,10 +9795,10 @@
         <v>11</v>
       </c>
       <c r="G244" s="7" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="H244" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="245" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -9824,17 +9829,17 @@
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A246" s="6" t="s">
-        <v>953</v>
+        <v>970</v>
       </c>
       <c r="B246" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C246" s="6" t="s">
+        <v>615</v>
+      </c>
+      <c r="D246" s="6" t="s">
         <v>616</v>
       </c>
-      <c r="D246" s="6" t="s">
-        <v>617</v>
-      </c>
       <c r="E246" s="7" t="s">
         <v>23</v>
       </c>
@@ -9842,41 +9847,41 @@
         <v>11</v>
       </c>
       <c r="G246" s="7" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="H246" s="5" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A247" s="6" t="s">
+        <v>971</v>
+      </c>
+      <c r="B247" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C247" s="6" t="s">
         <v>615</v>
       </c>
-    </row>
-    <row r="247" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A247" s="6" t="s">
-        <v>444</v>
-      </c>
-      <c r="B247" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C247" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="D247" s="6" t="s">
-        <v>445</v>
+        <v>616</v>
       </c>
       <c r="E247" s="7" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="F247" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G247" s="7" t="s">
-        <v>446</v>
+        <v>892</v>
       </c>
       <c r="H247" s="5" t="s">
-        <v>443</v>
+        <v>785</v>
       </c>
     </row>
     <row r="248" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A248" s="6" t="s">
-        <v>17</v>
+        <v>444</v>
       </c>
       <c r="B248" s="7" t="s">
         <v>10</v>
@@ -9885,7 +9890,7 @@
         <v>18</v>
       </c>
       <c r="D248" s="6" t="s">
-        <v>19</v>
+        <v>445</v>
       </c>
       <c r="E248" s="7" t="s">
         <v>11</v>
@@ -9894,15 +9899,15 @@
         <v>11</v>
       </c>
       <c r="G248" s="7" t="s">
-        <v>20</v>
+        <v>446</v>
       </c>
       <c r="H248" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="249" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A249" s="6" t="s">
-        <v>106</v>
+        <v>17</v>
       </c>
       <c r="B249" s="7" t="s">
         <v>10</v>
@@ -9911,7 +9916,7 @@
         <v>18</v>
       </c>
       <c r="D249" s="6" t="s">
-        <v>940</v>
+        <v>19</v>
       </c>
       <c r="E249" s="7" t="s">
         <v>11</v>
@@ -9920,15 +9925,15 @@
         <v>11</v>
       </c>
       <c r="G249" s="7" t="s">
-        <v>107</v>
+        <v>20</v>
       </c>
       <c r="H249" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="250" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A250" s="6" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="B250" s="7" t="s">
         <v>10</v>
@@ -9937,7 +9942,7 @@
         <v>18</v>
       </c>
       <c r="D250" s="6" t="s">
-        <v>90</v>
+        <v>938</v>
       </c>
       <c r="E250" s="7" t="s">
         <v>11</v>
@@ -9946,15 +9951,15 @@
         <v>11</v>
       </c>
       <c r="G250" s="7" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="H250" s="5" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
     </row>
     <row r="251" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A251" s="6" t="s">
-        <v>285</v>
+        <v>89</v>
       </c>
       <c r="B251" s="7" t="s">
         <v>10</v>
@@ -9972,15 +9977,15 @@
         <v>11</v>
       </c>
       <c r="G251" s="7" t="s">
-        <v>286</v>
+        <v>91</v>
       </c>
       <c r="H251" s="5" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="252" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A252" s="6" t="s">
-        <v>102</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A252" s="9" t="s">
+        <v>285</v>
       </c>
       <c r="B252" s="7" t="s">
         <v>10</v>
@@ -9989,7 +9994,7 @@
         <v>18</v>
       </c>
       <c r="D252" s="6" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="E252" s="7" t="s">
         <v>11</v>
@@ -9998,15 +10003,15 @@
         <v>11</v>
       </c>
       <c r="G252" s="7" t="s">
-        <v>104</v>
+        <v>286</v>
       </c>
       <c r="H252" s="5" t="s">
-        <v>101</v>
+        <v>284</v>
       </c>
     </row>
     <row r="253" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A253" s="6" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B253" s="7" t="s">
         <v>10</v>
@@ -10015,7 +10020,7 @@
         <v>18</v>
       </c>
       <c r="D253" s="6" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E253" s="7" t="s">
         <v>11</v>
@@ -10024,15 +10029,15 @@
         <v>11</v>
       </c>
       <c r="G253" s="7" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="H253" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="254" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A254" s="6" t="s">
-        <v>282</v>
+        <v>98</v>
       </c>
       <c r="B254" s="7" t="s">
         <v>10</v>
@@ -10050,15 +10055,15 @@
         <v>11</v>
       </c>
       <c r="G254" s="7" t="s">
-        <v>283</v>
+        <v>100</v>
       </c>
       <c r="H254" s="5" t="s">
-        <v>281</v>
+        <v>97</v>
       </c>
     </row>
     <row r="255" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A255" s="6" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="B255" s="7" t="s">
         <v>10</v>
@@ -10067,7 +10072,7 @@
         <v>18</v>
       </c>
       <c r="D255" s="6" t="s">
-        <v>279</v>
+        <v>99</v>
       </c>
       <c r="E255" s="7" t="s">
         <v>11</v>
@@ -10076,15 +10081,15 @@
         <v>11</v>
       </c>
       <c r="G255" s="7" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="H255" s="5" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="256" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A256" s="6" t="s">
-        <v>43</v>
+        <v>278</v>
       </c>
       <c r="B256" s="7" t="s">
         <v>10</v>
@@ -10093,7 +10098,7 @@
         <v>18</v>
       </c>
       <c r="D256" s="6" t="s">
-        <v>44</v>
+        <v>279</v>
       </c>
       <c r="E256" s="7" t="s">
         <v>11</v>
@@ -10102,15 +10107,15 @@
         <v>11</v>
       </c>
       <c r="G256" s="7" t="s">
-        <v>45</v>
+        <v>280</v>
       </c>
       <c r="H256" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="257" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A257" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B257" s="7" t="s">
         <v>10</v>
@@ -10128,15 +10133,15 @@
         <v>11</v>
       </c>
       <c r="G257" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H257" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="258" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A258" s="6" t="s">
-        <v>402</v>
+        <v>47</v>
       </c>
       <c r="B258" s="7" t="s">
         <v>10</v>
@@ -10145,7 +10150,7 @@
         <v>18</v>
       </c>
       <c r="D258" s="6" t="s">
-        <v>403</v>
+        <v>44</v>
       </c>
       <c r="E258" s="7" t="s">
         <v>11</v>
@@ -10154,15 +10159,15 @@
         <v>11</v>
       </c>
       <c r="G258" s="7" t="s">
-        <v>404</v>
+        <v>48</v>
       </c>
       <c r="H258" s="5" t="s">
-        <v>401</v>
+        <v>46</v>
       </c>
     </row>
     <row r="259" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A259" s="6" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="B259" s="7" t="s">
         <v>10</v>
@@ -10171,347 +10176,63 @@
         <v>18</v>
       </c>
       <c r="D259" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="E259" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F259" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G259" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="H259" s="5" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="260" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A260" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="B260" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C260" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D260" s="6" t="s">
         <v>407</v>
       </c>
-      <c r="E259" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F259" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G259" s="7" t="s">
+      <c r="E260" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F260" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G260" s="7" t="s">
         <v>408</v>
       </c>
-      <c r="H259" s="5" t="s">
+      <c r="H260" s="5" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A260" s="6"/>
-      <c r="B260" s="7"/>
-      <c r="C260" s="6"/>
-      <c r="D260" s="6"/>
-      <c r="E260" s="7"/>
-      <c r="F260" s="7"/>
-      <c r="G260" s="7"/>
-      <c r="H260" s="5"/>
-    </row>
     <row r="261" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A261" s="6"/>
-      <c r="B261" s="7"/>
-      <c r="C261" s="6"/>
-      <c r="D261" s="6"/>
-      <c r="E261" s="7"/>
-      <c r="F261" s="7"/>
-      <c r="G261" s="7"/>
-      <c r="H261" s="5"/>
-    </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A262" s="6"/>
-      <c r="B262" s="7"/>
-      <c r="C262" s="6"/>
-      <c r="D262" s="6"/>
-      <c r="E262" s="7"/>
-      <c r="F262" s="7"/>
-      <c r="G262" s="7"/>
-      <c r="H262" s="5"/>
-    </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A263" s="6"/>
-      <c r="B263" s="7"/>
-      <c r="C263" s="6"/>
-      <c r="D263" s="6"/>
-      <c r="E263" s="7"/>
-      <c r="F263" s="7"/>
-      <c r="G263" s="7"/>
-      <c r="H263" s="5"/>
-    </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A264" s="6"/>
-      <c r="B264" s="7"/>
-      <c r="C264" s="6"/>
-      <c r="D264" s="6"/>
-      <c r="E264" s="7"/>
-      <c r="F264" s="7"/>
-      <c r="G264" s="7"/>
-      <c r="H264" s="5"/>
-    </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A265" s="6"/>
-      <c r="B265" s="7"/>
-      <c r="C265" s="6"/>
-      <c r="D265" s="6"/>
-      <c r="E265" s="7"/>
-      <c r="F265" s="7"/>
-      <c r="G265" s="7"/>
-      <c r="H265" s="5"/>
-    </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A266" s="6"/>
-      <c r="B266" s="7"/>
-      <c r="C266" s="6"/>
-      <c r="D266" s="6"/>
-      <c r="E266" s="7"/>
-      <c r="F266" s="7"/>
-      <c r="G266" s="7"/>
-      <c r="H266" s="5"/>
-    </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A267" s="6"/>
-      <c r="B267" s="7"/>
-      <c r="C267" s="6"/>
-      <c r="D267" s="6"/>
-      <c r="E267" s="7"/>
-      <c r="F267" s="7"/>
-      <c r="G267" s="7"/>
-      <c r="H267" s="5"/>
-    </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A268" s="6"/>
-      <c r="B268" s="7"/>
-      <c r="C268" s="6"/>
-      <c r="D268" s="6"/>
-      <c r="E268" s="7"/>
-      <c r="F268" s="7"/>
-      <c r="G268" s="7"/>
-      <c r="H268" s="5"/>
-    </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A269" s="6"/>
-      <c r="B269" s="7"/>
-      <c r="C269" s="6"/>
-      <c r="D269" s="6"/>
-      <c r="E269" s="7"/>
-      <c r="F269" s="7"/>
-      <c r="G269" s="7"/>
-      <c r="H269" s="5"/>
-    </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A270" s="6"/>
-      <c r="B270" s="7"/>
-      <c r="C270" s="6"/>
-      <c r="D270" s="6"/>
-      <c r="E270" s="7"/>
-      <c r="F270" s="7"/>
-      <c r="G270" s="7"/>
-      <c r="H270" s="5"/>
-    </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A271" s="6"/>
-      <c r="B271" s="7"/>
-      <c r="C271" s="6"/>
-      <c r="D271" s="6"/>
-      <c r="E271" s="7"/>
-      <c r="F271" s="7"/>
-      <c r="G271" s="7"/>
-      <c r="H271" s="5"/>
-    </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A272" s="6"/>
-      <c r="B272" s="7"/>
-      <c r="C272" s="6"/>
-      <c r="D272" s="6"/>
-      <c r="E272" s="7"/>
-      <c r="F272" s="7"/>
-      <c r="G272" s="7"/>
-      <c r="H272" s="5"/>
-    </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A273" s="6"/>
-      <c r="B273" s="7"/>
-      <c r="C273" s="6"/>
-      <c r="D273" s="6"/>
-      <c r="E273" s="7"/>
-      <c r="F273" s="7"/>
-      <c r="G273" s="7"/>
-      <c r="H273" s="5"/>
-    </row>
-    <row r="274" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A274" s="6"/>
-      <c r="B274" s="7"/>
-      <c r="C274" s="6"/>
-      <c r="D274" s="6"/>
-      <c r="E274" s="7"/>
-      <c r="F274" s="7"/>
-      <c r="G274" s="7"/>
-      <c r="H274" s="5"/>
-    </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A275" s="6"/>
-      <c r="B275" s="7"/>
-      <c r="C275" s="6"/>
-      <c r="D275" s="6"/>
-      <c r="E275" s="7"/>
-      <c r="F275" s="7"/>
-      <c r="G275" s="7"/>
-      <c r="H275" s="5"/>
-    </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A276" s="6"/>
-      <c r="B276" s="7"/>
-      <c r="C276" s="6"/>
-      <c r="D276" s="6"/>
-      <c r="E276" s="7"/>
-      <c r="F276" s="7"/>
-      <c r="G276" s="7"/>
-      <c r="H276" s="5"/>
-    </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A277" s="6"/>
-      <c r="B277" s="7"/>
-      <c r="C277" s="6"/>
-      <c r="D277" s="6"/>
-      <c r="E277" s="7"/>
-      <c r="F277" s="7"/>
-      <c r="G277" s="7"/>
-      <c r="H277" s="5"/>
-    </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A278" s="6"/>
-      <c r="B278" s="7"/>
-      <c r="C278" s="6"/>
-      <c r="D278" s="6"/>
-      <c r="E278" s="7"/>
-      <c r="F278" s="7"/>
-      <c r="G278" s="7"/>
-      <c r="H278" s="5"/>
-    </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A279" s="6"/>
-      <c r="B279" s="7"/>
-      <c r="C279" s="6"/>
-      <c r="D279" s="6"/>
-      <c r="E279" s="7"/>
-      <c r="F279" s="7"/>
-      <c r="G279" s="7"/>
-      <c r="H279" s="5"/>
-    </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A280" s="8"/>
-      <c r="B280" s="7"/>
-      <c r="C280" s="6"/>
-      <c r="D280" s="6"/>
-      <c r="E280" s="7"/>
-      <c r="F280" s="7"/>
-      <c r="G280" s="7"/>
-      <c r="H280" s="5"/>
-    </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A281" s="6"/>
-      <c r="B281" s="7"/>
-      <c r="C281" s="6"/>
-      <c r="D281" s="6"/>
-      <c r="E281" s="7"/>
-      <c r="F281" s="7"/>
-      <c r="G281" s="7"/>
-      <c r="H281" s="5"/>
-    </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A282" s="6"/>
-      <c r="B282" s="7"/>
-      <c r="C282" s="6"/>
-      <c r="D282" s="6"/>
-      <c r="E282" s="7"/>
-      <c r="F282" s="7"/>
-      <c r="G282" s="7"/>
-      <c r="H282" s="5"/>
-    </row>
-    <row r="283" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A283" s="6"/>
-      <c r="B283" s="7"/>
-      <c r="C283" s="6"/>
-      <c r="D283" s="6"/>
-      <c r="E283" s="7"/>
-      <c r="F283" s="7"/>
-      <c r="G283" s="7"/>
-      <c r="H283" s="5"/>
-    </row>
-    <row r="284" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A284" s="6"/>
-      <c r="B284" s="7"/>
-      <c r="C284" s="6"/>
-      <c r="D284" s="6"/>
-      <c r="E284" s="7"/>
-      <c r="F284" s="7"/>
-      <c r="G284" s="7"/>
-      <c r="H284" s="5"/>
-    </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A285" s="6"/>
-      <c r="B285" s="7"/>
-      <c r="C285" s="6"/>
-      <c r="D285" s="6"/>
-      <c r="E285" s="7"/>
-      <c r="F285" s="7"/>
-      <c r="G285" s="7"/>
-      <c r="H285" s="5"/>
-    </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A286" s="6"/>
-      <c r="B286" s="7"/>
-      <c r="C286" s="6"/>
-      <c r="D286" s="6"/>
-      <c r="E286" s="7"/>
-      <c r="F286" s="7"/>
-      <c r="G286" s="7"/>
-      <c r="H286" s="5"/>
-    </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A287" s="6"/>
-      <c r="B287" s="7"/>
-      <c r="C287" s="6"/>
-      <c r="D287" s="6"/>
-      <c r="E287" s="7"/>
-      <c r="F287" s="7"/>
-      <c r="G287" s="7"/>
-      <c r="H287" s="5"/>
-    </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A288" s="6"/>
-      <c r="B288" s="7"/>
-      <c r="C288" s="6"/>
-      <c r="D288" s="6"/>
-      <c r="E288" s="7"/>
-      <c r="F288" s="7"/>
-      <c r="G288" s="7"/>
-      <c r="H288" s="5"/>
-    </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A289" s="9"/>
-      <c r="B289" s="7"/>
-      <c r="C289" s="6"/>
-      <c r="D289" s="6"/>
-      <c r="E289" s="7"/>
-      <c r="F289" s="7"/>
-      <c r="G289" s="7"/>
-      <c r="H289" s="5"/>
-    </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A290" s="9"/>
-      <c r="B290" s="7"/>
-      <c r="C290" s="6"/>
-      <c r="D290" s="6"/>
-      <c r="E290" s="7"/>
-      <c r="F290" s="7"/>
-      <c r="G290" s="7"/>
-      <c r="H290" s="5"/>
-    </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A291" s="11"/>
-      <c r="B291" s="12"/>
-      <c r="C291" s="11"/>
-      <c r="D291" s="11"/>
-      <c r="E291" s="12"/>
-      <c r="F291" s="12"/>
-      <c r="G291" s="12"/>
-      <c r="H291" s="13"/>
+      <c r="A261" s="10"/>
+      <c r="B261" s="11"/>
+      <c r="C261" s="10"/>
+      <c r="D261" s="10"/>
+      <c r="E261" s="11"/>
+      <c r="F261" s="11"/>
+      <c r="G261" s="11"/>
+      <c r="H261" s="12"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H11" xr:uid="{B9FACE88-1C57-4099-A43D-8DA482706A91}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H291">
-    <sortCondition ref="C9:C291"/>
-    <sortCondition ref="D9:D291"/>
-    <sortCondition ref="H9:H291"/>
+  <autoFilter ref="A1:H18" xr:uid="{B9FACE88-1C57-4099-A43D-8DA482706A91}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H261">
+    <sortCondition ref="C9:C261"/>
+    <sortCondition ref="D9:D261"/>
+    <sortCondition ref="H9:H261"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated based on last commetn Richard
</commit_message>
<xml_diff>
--- a/Deliverables/RULES/USDM_CORE_Rules.xlsx
+++ b/Deliverables/RULES/USDM_CORE_Rules.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stack\CL027\Publish\CORE\4.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8526A368-FF39-418E-B7E6-D26FC6AD0693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6905ADAD-B16E-4A31-B5DD-217C5593F6BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38040" yWindow="-10920" windowWidth="29040" windowHeight="15720" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
+    <workbookView xWindow="11100" yWindow="-15975" windowWidth="25050" windowHeight="14955" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
   </bookViews>
   <sheets>
     <sheet name="Version 3.0 and 4.0 CORE rules" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Version 3.0 and 4.0 CORE rules'!$A$1:$H$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Version 3.0 and 4.0 CORE rules'!$A$1:$H$260</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -3075,7 +3075,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3096,11 +3096,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3116,10 +3111,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3440,10 +3431,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FACE88-1C57-4099-A43D-8DA482706A91}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H261"/>
+  <dimension ref="A1:H260"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D247" sqref="D247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9858,7 +9849,7 @@
         <v>971</v>
       </c>
       <c r="B247" s="7" t="s">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="C247" s="6" t="s">
         <v>615</v>
@@ -10217,18 +10208,8 @@
         <v>405</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A261" s="10"/>
-      <c r="B261" s="11"/>
-      <c r="C261" s="10"/>
-      <c r="D261" s="10"/>
-      <c r="E261" s="11"/>
-      <c r="F261" s="11"/>
-      <c r="G261" s="11"/>
-      <c r="H261" s="12"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:H18" xr:uid="{B9FACE88-1C57-4099-A43D-8DA482706A91}"/>
+  <autoFilter ref="A1:H260" xr:uid="{B9FACE88-1C57-4099-A43D-8DA482706A91}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H261">
     <sortCondition ref="C9:C261"/>
     <sortCondition ref="D9:D261"/>

</xml_diff>